<commit_message>
CIERRE 29 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
@@ -630,7 +630,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2370" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2382" uniqueCount="888">
   <si>
     <t>MORRALLA EN CAJA DE 11 SUR   2,800.00  +  $ 1,200.00 Total    $  4,000.00</t>
   </si>
@@ -3248,16 +3248,52 @@
     <t>ELIAS /  PEPE</t>
   </si>
   <si>
-    <t># 298065</t>
-  </si>
-  <si>
-    <t># 298066</t>
-  </si>
-  <si>
     <t>POLLO-MAIZ-,MANTECA</t>
   </si>
   <si>
     <t>NOMINA #  36</t>
+  </si>
+  <si>
+    <t>TOCINETA-CHISCHORRA-CECINA-POLLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLLO  </t>
+  </si>
+  <si>
+    <t>DESTAPAR DRENAJE</t>
+  </si>
+  <si>
+    <t>CHORIZO--LONGANIZA--MANTECA--POLLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELIAS  </t>
+  </si>
+  <si>
+    <t>POLLO-CHORIZO-MOLE--TOSTADAS-MAIZ</t>
+  </si>
+  <si>
+    <t>RETAZO-POLLO</t>
+  </si>
+  <si>
+    <t>ELIAS</t>
+  </si>
+  <si>
+    <t>QUESOS--POLLO--TOSTADAS</t>
+  </si>
+  <si>
+    <t>LONGANIZA-POLLO-CHORIZO-MAIZ</t>
+  </si>
+  <si>
+    <t>NOMINA #  37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#  </t>
+  </si>
+  <si>
+    <t>#  300498</t>
+  </si>
+  <si>
+    <t># 300500</t>
   </si>
 </sst>
 </file>
@@ -5144,7 +5180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="663">
+  <cellXfs count="667">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6289,31 +6325,27 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6355,26 +6387,31 @@
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="15" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6389,14 +6426,14 @@
     <xf numFmtId="166" fontId="6" fillId="15" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6415,6 +6452,15 @@
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6494,26 +6540,32 @@
     <xf numFmtId="44" fontId="49" fillId="0" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="8" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6554,32 +6606,53 @@
     <xf numFmtId="44" fontId="16" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="7" fontId="6" fillId="11" borderId="73" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6605,42 +6678,6 @@
     <xf numFmtId="44" fontId="35" fillId="7" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="8" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6648,6 +6685,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6668,22 +6720,16 @@
     <xf numFmtId="7" fontId="35" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="13" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -6693,15 +6739,15 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FF9966FF"/>
+      <color rgb="FF0000FF"/>
       <color rgb="FF66FFFF"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FFFF3300"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF800000"/>
-      <color rgb="FFCC99FF"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FF990033"/>
-      <color rgb="FF9966FF"/>
       <color rgb="FFFF00FF"/>
     </mruColors>
   </colors>
@@ -12877,17 +12923,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -12918,17 +12964,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -12957,14 +13003,14 @@
       <c r="D4" s="23">
         <v>44201</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="558" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="537" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -15606,30 +15652,30 @@
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="530">
+      <c r="P65" s="552">
         <f>P62+Q62</f>
         <v>3321521.28</v>
       </c>
-      <c r="Q65" s="531"/>
+      <c r="Q65" s="553"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="532" t="s">
+      <c r="D66" s="554" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="532"/>
+      <c r="E66" s="554"/>
       <c r="F66" s="95">
         <v>-2276696.6800000002</v>
       </c>
-      <c r="I66" s="533" t="s">
+      <c r="I66" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="534"/>
-      <c r="K66" s="535">
+      <c r="J66" s="556"/>
+      <c r="K66" s="557">
         <f>F68+F69+F70</f>
         <v>344253.98999999964</v>
       </c>
-      <c r="L66" s="536"/>
+      <c r="L66" s="558"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -15663,11 +15709,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="537">
+      <c r="K68" s="559">
         <f>-C4</f>
         <v>-250864.68</v>
       </c>
-      <c r="L68" s="538"/>
+      <c r="L68" s="560"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -15810,11 +15856,11 @@
     <sortCondition ref="J35:J54"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
@@ -15822,11 +15868,11 @@
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="K70:L70"/>
     <mergeCell ref="D65:E65"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.2" right="0.16" top="0.34" bottom="0.32" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -17251,20 +17297,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="600" t="s">
+      <c r="B1" s="574" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -17274,7 +17320,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="601"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -17293,27 +17339,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="583" t="s">
+      <c r="AB2" s="587" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="583"/>
-      <c r="AD2" s="583"/>
-      <c r="AE2" s="583"/>
-      <c r="AF2" s="583"/>
-      <c r="AG2" s="583"/>
+      <c r="AC2" s="587"/>
+      <c r="AD2" s="587"/>
+      <c r="AE2" s="587"/>
+      <c r="AF2" s="587"/>
+      <c r="AG2" s="587"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -17321,7 +17367,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="573" t="s">
+      <c r="P3" s="577" t="s">
         <v>562</v>
       </c>
       <c r="Q3" s="393"/>
@@ -17334,12 +17380,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="583"/>
-      <c r="AC3" s="583"/>
-      <c r="AD3" s="583"/>
-      <c r="AE3" s="583"/>
-      <c r="AF3" s="583"/>
-      <c r="AG3" s="583"/>
+      <c r="AB3" s="587"/>
+      <c r="AC3" s="587"/>
+      <c r="AD3" s="587"/>
+      <c r="AE3" s="587"/>
+      <c r="AF3" s="587"/>
+      <c r="AG3" s="587"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -17352,14 +17398,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="558" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="537" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -17370,7 +17416,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="573"/>
+      <c r="P4" s="577"/>
       <c r="Q4" s="393"/>
       <c r="R4" s="30"/>
       <c r="S4" s="31"/>
@@ -17385,16 +17431,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="584" t="s">
+      <c r="AB4" s="588" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="585"/>
+      <c r="AC4" s="589"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="586" t="s">
+      <c r="AE4" s="590" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="586"/>
-      <c r="AG4" s="586"/>
+      <c r="AF4" s="590"/>
+      <c r="AG4" s="590"/>
     </row>
     <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
@@ -18806,10 +18852,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="591" t="s">
+      <c r="AE23" s="595" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="592"/>
+      <c r="AF23" s="596"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -18953,11 +18999,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="593" t="s">
+      <c r="AE25" s="597" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="594"/>
-      <c r="AG25" s="597">
+      <c r="AF25" s="598"/>
+      <c r="AG25" s="601">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -19028,9 +19074,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="595"/>
-      <c r="AF26" s="596"/>
-      <c r="AG26" s="598"/>
+      <c r="AE26" s="599"/>
+      <c r="AF26" s="600"/>
+      <c r="AG26" s="602"/>
     </row>
     <row r="27" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
@@ -19205,10 +19251,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="587" t="s">
+      <c r="AB29" s="591" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="589">
+      <c r="AC29" s="593">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -19244,11 +19290,11 @@
         <v>0</v>
       </c>
       <c r="O30" s="7"/>
-      <c r="P30" s="574">
+      <c r="P30" s="578">
         <f>SUM(P5:P29)</f>
         <v>-163726</v>
       </c>
-      <c r="Q30" s="574"/>
+      <c r="Q30" s="578"/>
       <c r="R30" s="7">
         <v>0</v>
       </c>
@@ -19262,8 +19308,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="588"/>
-      <c r="AC30" s="590"/>
+      <c r="AB30" s="592"/>
+      <c r="AC30" s="594"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -20664,30 +20710,30 @@
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="R65" s="530">
+      <c r="R65" s="552">
         <f>R62+S62</f>
         <v>3138957.44</v>
       </c>
-      <c r="S65" s="531"/>
+      <c r="S65" s="553"/>
       <c r="U65" s="50"/>
     </row>
     <row r="66" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="532" t="s">
+      <c r="D66" s="554" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="532"/>
+      <c r="E66" s="554"/>
       <c r="F66" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I66" s="533" t="s">
+      <c r="I66" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="534"/>
-      <c r="K66" s="535">
+      <c r="J66" s="556"/>
+      <c r="K66" s="557">
         <f>F68+F69+F70</f>
         <v>381077.48999999953</v>
       </c>
-      <c r="L66" s="536"/>
+      <c r="L66" s="558"/>
       <c r="R66" s="50"/>
       <c r="U66" s="107"/>
     </row>
@@ -20721,11 +20767,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="537">
+      <c r="K68" s="559">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L68" s="538"/>
+      <c r="L68" s="560"/>
       <c r="M68" s="116"/>
       <c r="R68" s="50"/>
       <c r="S68" s="7"/>
@@ -20780,14 +20826,14 @@
       <c r="S71" s="7"/>
     </row>
     <row r="72" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I72" s="575" t="s">
+      <c r="I72" s="579" t="s">
         <v>610</v>
       </c>
-      <c r="J72" s="576"/>
-      <c r="K72" s="579">
+      <c r="J72" s="580"/>
+      <c r="K72" s="583">
         <v>163726</v>
       </c>
-      <c r="L72" s="580"/>
+      <c r="L72" s="584"/>
       <c r="R72" s="7"/>
       <c r="S72" s="7"/>
     </row>
@@ -20796,10 +20842,10 @@
       <c r="C73" s="128"/>
       <c r="D73" s="129"/>
       <c r="E73" s="7"/>
-      <c r="I73" s="577"/>
-      <c r="J73" s="578"/>
-      <c r="K73" s="581"/>
-      <c r="L73" s="582"/>
+      <c r="I73" s="581"/>
+      <c r="J73" s="582"/>
+      <c r="K73" s="585"/>
+      <c r="L73" s="586"/>
       <c r="M73" s="2"/>
       <c r="N73" s="60"/>
       <c r="O73" s="165"/>
@@ -20851,7 +20897,7 @@
       <c r="C76" s="130"/>
       <c r="E76" s="7"/>
       <c r="M76" s="4"/>
-      <c r="AC76" s="599"/>
+      <c r="AC76" s="576"/>
       <c r="AD76" s="342"/>
       <c r="AE76" s="342"/>
       <c r="AF76" s="342"/>
@@ -20864,7 +20910,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="273"/>
       <c r="M77" s="4"/>
-      <c r="AC77" s="599"/>
+      <c r="AC77" s="576"/>
       <c r="AD77" s="342"/>
       <c r="AE77" s="342"/>
       <c r="AF77" s="342"/>
@@ -20958,22 +21004,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AC76:AC77"/>
-    <mergeCell ref="R65:S65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="I72:J73"/>
@@ -20989,6 +21019,22 @@
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AC76:AC77"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.49" right="0.23622047244094491" top="0.47244094488188981" bottom="0.27559055118110237" header="0.70866141732283472" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22326,25 +22372,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="600" t="s">
+      <c r="B1" s="574" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="601"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -22354,27 +22400,27 @@
       <c r="L2" s="12"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="Q2" s="583" t="s">
+      <c r="Q2" s="587" t="s">
         <v>596</v>
       </c>
-      <c r="R2" s="583"/>
-      <c r="S2" s="583"/>
-      <c r="T2" s="583"/>
-      <c r="U2" s="583"/>
-      <c r="V2" s="583"/>
+      <c r="R2" s="587"/>
+      <c r="S2" s="587"/>
+      <c r="T2" s="587"/>
+      <c r="U2" s="587"/>
+      <c r="V2" s="587"/>
     </row>
     <row r="3" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -22382,12 +22428,12 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="Q3" s="583"/>
-      <c r="R3" s="583"/>
-      <c r="S3" s="583"/>
-      <c r="T3" s="583"/>
-      <c r="U3" s="583"/>
-      <c r="V3" s="583"/>
+      <c r="Q3" s="587"/>
+      <c r="R3" s="587"/>
+      <c r="S3" s="587"/>
+      <c r="T3" s="587"/>
+      <c r="U3" s="587"/>
+      <c r="V3" s="587"/>
     </row>
     <row r="4" spans="1:23" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -22400,14 +22446,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="558" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="537" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -22419,16 +22465,16 @@
       </c>
       <c r="O4" s="365"/>
       <c r="P4" s="29"/>
-      <c r="Q4" s="584" t="s">
+      <c r="Q4" s="588" t="s">
         <v>527</v>
       </c>
-      <c r="R4" s="585"/>
+      <c r="R4" s="589"/>
       <c r="S4" s="99"/>
-      <c r="T4" s="586" t="s">
+      <c r="T4" s="590" t="s">
         <v>567</v>
       </c>
-      <c r="U4" s="586"/>
-      <c r="V4" s="586"/>
+      <c r="U4" s="590"/>
+      <c r="V4" s="590"/>
       <c r="W4" s="99"/>
     </row>
     <row r="5" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23427,10 +23473,10 @@
         <v>0</v>
       </c>
       <c r="S23" s="99"/>
-      <c r="T23" s="591" t="s">
+      <c r="T23" s="595" t="s">
         <v>564</v>
       </c>
-      <c r="U23" s="592"/>
+      <c r="U23" s="596"/>
       <c r="V23" s="339">
         <f>SUM(V6:V22)</f>
         <v>2323600</v>
@@ -23534,11 +23580,11 @@
         <v>138607</v>
       </c>
       <c r="S25" s="99"/>
-      <c r="T25" s="593" t="s">
+      <c r="T25" s="597" t="s">
         <v>565</v>
       </c>
-      <c r="U25" s="594"/>
-      <c r="V25" s="597">
+      <c r="U25" s="598"/>
+      <c r="V25" s="601">
         <f>R29-V23</f>
         <v>163726</v>
       </c>
@@ -23587,9 +23633,9 @@
         <v>107480</v>
       </c>
       <c r="S26" s="99"/>
-      <c r="T26" s="595"/>
-      <c r="U26" s="596"/>
-      <c r="V26" s="598"/>
+      <c r="T26" s="599"/>
+      <c r="U26" s="600"/>
+      <c r="V26" s="602"/>
       <c r="W26" s="99"/>
     </row>
     <row r="27" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23712,10 +23758,10 @@
       </c>
       <c r="O29" s="7"/>
       <c r="P29" s="29"/>
-      <c r="Q29" s="587" t="s">
+      <c r="Q29" s="591" t="s">
         <v>562</v>
       </c>
-      <c r="R29" s="589">
+      <c r="R29" s="593">
         <f>SUM(R5:R28)</f>
         <v>2487326</v>
       </c>
@@ -23752,8 +23798,8 @@
       </c>
       <c r="O30" s="7"/>
       <c r="P30" s="373"/>
-      <c r="Q30" s="588"/>
-      <c r="R30" s="590"/>
+      <c r="Q30" s="592"/>
+      <c r="R30" s="594"/>
       <c r="S30" s="99"/>
       <c r="T30" s="99"/>
       <c r="U30" s="99"/>
@@ -24416,22 +24462,22 @@
       <c r="J51" s="105"/>
     </row>
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D52" s="532" t="s">
+      <c r="D52" s="554" t="s">
         <v>502</v>
       </c>
-      <c r="E52" s="532"/>
+      <c r="E52" s="554"/>
       <c r="F52" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I52" s="533" t="s">
+      <c r="I52" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J52" s="534"/>
-      <c r="K52" s="535">
+      <c r="J52" s="556"/>
+      <c r="K52" s="557">
         <f>F54+F55+F56</f>
         <v>381077.72999999952</v>
       </c>
-      <c r="L52" s="536"/>
+      <c r="L52" s="558"/>
     </row>
     <row r="53" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="108"/>
@@ -24460,11 +24506,11 @@
         <v>21</v>
       </c>
       <c r="J54" s="115"/>
-      <c r="K54" s="537">
+      <c r="K54" s="559">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L54" s="538"/>
+      <c r="L54" s="560"/>
       <c r="M54" s="116"/>
     </row>
     <row r="55" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24553,7 +24599,7 @@
       <c r="C62" s="130"/>
       <c r="E62" s="7"/>
       <c r="M62" s="4"/>
-      <c r="R62" s="599"/>
+      <c r="R62" s="576"/>
       <c r="S62" s="379"/>
       <c r="T62" s="379"/>
       <c r="U62" s="379"/>
@@ -24566,7 +24612,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="273"/>
       <c r="M63" s="4"/>
-      <c r="R63" s="599"/>
+      <c r="R63" s="576"/>
       <c r="S63" s="379"/>
       <c r="T63" s="379"/>
       <c r="U63" s="379"/>
@@ -24643,23 +24689,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Q2:V3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T25:U26"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="Q29:Q30"/>
-    <mergeCell ref="R29:R30"/>
     <mergeCell ref="R62:R63"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
@@ -24669,6 +24698,23 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="I56:J56"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T25:U26"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="Q29:Q30"/>
+    <mergeCell ref="R29:R30"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="Q2:V3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24722,20 +24768,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="600" t="s">
+      <c r="B1" s="574" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -24745,7 +24791,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="601"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -24764,27 +24810,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="583" t="s">
+      <c r="AB2" s="587" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="583"/>
-      <c r="AD2" s="583"/>
-      <c r="AE2" s="583"/>
-      <c r="AF2" s="583"/>
-      <c r="AG2" s="583"/>
+      <c r="AC2" s="587"/>
+      <c r="AD2" s="587"/>
+      <c r="AE2" s="587"/>
+      <c r="AF2" s="587"/>
+      <c r="AG2" s="587"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -24792,13 +24838,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="602" t="s">
+      <c r="P3" s="625" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="604" t="s">
+      <c r="Q3" s="627" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="605"/>
+      <c r="S3" s="628"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -24808,12 +24854,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="583"/>
-      <c r="AC3" s="583"/>
-      <c r="AD3" s="583"/>
-      <c r="AE3" s="583"/>
-      <c r="AF3" s="583"/>
-      <c r="AG3" s="583"/>
+      <c r="AB3" s="587"/>
+      <c r="AC3" s="587"/>
+      <c r="AD3" s="587"/>
+      <c r="AE3" s="587"/>
+      <c r="AF3" s="587"/>
+      <c r="AG3" s="587"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -24826,14 +24872,14 @@
       <c r="D4" s="23">
         <v>44377</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="603" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="626" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -24844,10 +24890,10 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="602"/>
-      <c r="Q4" s="604"/>
+      <c r="P4" s="625"/>
+      <c r="Q4" s="627"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="605"/>
+      <c r="S4" s="628"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -24859,16 +24905,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="584" t="s">
+      <c r="AB4" s="588" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="585"/>
+      <c r="AC4" s="589"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="586" t="s">
+      <c r="AE4" s="590" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="586"/>
-      <c r="AG4" s="586"/>
+      <c r="AF4" s="590"/>
+      <c r="AG4" s="590"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -26305,10 +26351,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="591" t="s">
+      <c r="AE23" s="595" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="592"/>
+      <c r="AF23" s="596"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -26440,11 +26486,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="593" t="s">
+      <c r="AE25" s="597" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="594"/>
-      <c r="AG25" s="597">
+      <c r="AF25" s="598"/>
+      <c r="AG25" s="601">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -26513,9 +26559,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="595"/>
-      <c r="AF26" s="596"/>
-      <c r="AG26" s="598"/>
+      <c r="AE26" s="599"/>
+      <c r="AF26" s="600"/>
+      <c r="AG26" s="602"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -26714,10 +26760,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="587" t="s">
+      <c r="AB29" s="591" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="589">
+      <c r="AC29" s="593">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -26780,8 +26826,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="588"/>
-      <c r="AC30" s="590"/>
+      <c r="AB30" s="592"/>
+      <c r="AC30" s="594"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -27274,11 +27320,11 @@
       <c r="J39" s="233"/>
       <c r="K39" s="361"/>
       <c r="L39" s="357"/>
-      <c r="M39" s="614">
+      <c r="M39" s="620">
         <f>SUM(M5:M38)</f>
         <v>3989472.22</v>
       </c>
-      <c r="N39" s="616">
+      <c r="N39" s="622">
         <f>SUM(N5:N38)</f>
         <v>689220.5</v>
       </c>
@@ -27327,8 +27373,8 @@
         <f>1145.91+398.99+423.94+498.99+398.99</f>
         <v>2866.8199999999997</v>
       </c>
-      <c r="M40" s="615"/>
-      <c r="N40" s="617"/>
+      <c r="M40" s="621"/>
+      <c r="N40" s="623"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -27521,10 +27567,10 @@
       <c r="L44" s="358">
         <v>73526</v>
       </c>
-      <c r="M44" s="618" t="s">
+      <c r="M44" s="624" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="618"/>
+      <c r="N44" s="624"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -28112,7 +28158,7 @@
       <c r="L57" s="458">
         <v>7482</v>
       </c>
-      <c r="M57" s="606">
+      <c r="M57" s="612">
         <f>SUM(M45:M56)</f>
         <v>3606750</v>
       </c>
@@ -28152,7 +28198,7 @@
       <c r="L58" s="458">
         <v>986</v>
       </c>
-      <c r="M58" s="607"/>
+      <c r="M58" s="613"/>
       <c r="N58" s="475"/>
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
@@ -28227,10 +28273,10 @@
         <f>1033.33+165.33</f>
         <v>1198.6599999999999</v>
       </c>
-      <c r="M60" s="608" t="s">
+      <c r="M60" s="614" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="609"/>
+      <c r="N60" s="615"/>
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -28303,11 +28349,11 @@
       <c r="L62" s="458">
         <v>22595.71</v>
       </c>
-      <c r="M62" s="610">
+      <c r="M62" s="616">
         <f>M57-M39</f>
         <v>-382722.2200000002</v>
       </c>
-      <c r="N62" s="611"/>
+      <c r="N62" s="617"/>
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -28343,8 +28389,8 @@
       <c r="L63" s="458">
         <v>1064</v>
       </c>
-      <c r="M63" s="612"/>
-      <c r="N63" s="613"/>
+      <c r="M63" s="618"/>
+      <c r="N63" s="619"/>
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -28570,30 +28616,30 @@
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="530">
+      <c r="R70" s="552">
         <f>R67+S67</f>
         <v>10503773.959999999</v>
       </c>
-      <c r="S70" s="531"/>
+      <c r="S70" s="553"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="532" t="s">
+      <c r="D71" s="554" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="532"/>
+      <c r="E71" s="554"/>
       <c r="F71" s="95">
         <v>-3290264.27</v>
       </c>
-      <c r="I71" s="533" t="s">
+      <c r="I71" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="534"/>
-      <c r="K71" s="535">
+      <c r="J71" s="556"/>
+      <c r="K71" s="557">
         <f>F73+F74+F75</f>
         <v>426565.1</v>
       </c>
-      <c r="L71" s="536"/>
+      <c r="L71" s="558"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -28627,11 +28673,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="537">
+      <c r="K73" s="559">
         <f>-C4</f>
         <v>-308642.71999999997</v>
       </c>
-      <c r="L73" s="619"/>
+      <c r="L73" s="603"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -28684,14 +28730,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="620" t="s">
+      <c r="I77" s="604" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="621"/>
-      <c r="K77" s="624">
+      <c r="J77" s="605"/>
+      <c r="K77" s="608">
         <v>-383122.22</v>
       </c>
-      <c r="L77" s="625"/>
+      <c r="L77" s="609"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -28700,10 +28746,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="622"/>
-      <c r="J78" s="623"/>
-      <c r="K78" s="626"/>
-      <c r="L78" s="627"/>
+      <c r="I78" s="606"/>
+      <c r="J78" s="607"/>
+      <c r="K78" s="610"/>
+      <c r="L78" s="611"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="165"/>
@@ -28755,7 +28801,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="599"/>
+      <c r="AC81" s="576"/>
       <c r="AD81" s="440"/>
       <c r="AE81" s="440"/>
       <c r="AF81" s="440"/>
@@ -28768,7 +28814,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="599"/>
+      <c r="AC82" s="576"/>
       <c r="AD82" s="440"/>
       <c r="AE82" s="440"/>
       <c r="AF82" s="440"/>
@@ -28862,13 +28908,21 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="AB2:AG3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="K71:L71"/>
@@ -28884,21 +28938,13 @@
     <mergeCell ref="M39:M40"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="M44:N44"/>
-    <mergeCell ref="AG25:AG26"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="AB2:AG3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.27559055118110237" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30581,20 +30627,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="600" t="s">
+      <c r="B1" s="574" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>721</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -30604,7 +30650,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="601"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -30623,27 +30669,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="583" t="s">
+      <c r="AB2" s="587" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="583"/>
-      <c r="AD2" s="583"/>
-      <c r="AE2" s="583"/>
-      <c r="AF2" s="583"/>
-      <c r="AG2" s="583"/>
+      <c r="AC2" s="587"/>
+      <c r="AD2" s="587"/>
+      <c r="AE2" s="587"/>
+      <c r="AF2" s="587"/>
+      <c r="AG2" s="587"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -30654,13 +30700,13 @@
       <c r="O3" s="366" t="s">
         <v>753</v>
       </c>
-      <c r="P3" s="602" t="s">
+      <c r="P3" s="625" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="604" t="s">
+      <c r="Q3" s="627" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="605"/>
+      <c r="S3" s="628"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -30670,12 +30716,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="583"/>
-      <c r="AC3" s="583"/>
-      <c r="AD3" s="583"/>
-      <c r="AE3" s="583"/>
-      <c r="AF3" s="583"/>
-      <c r="AG3" s="583"/>
+      <c r="AB3" s="587"/>
+      <c r="AC3" s="587"/>
+      <c r="AD3" s="587"/>
+      <c r="AE3" s="587"/>
+      <c r="AF3" s="587"/>
+      <c r="AG3" s="587"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -30688,14 +30734,14 @@
       <c r="D4" s="23">
         <v>44411</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="603" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="626" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -30706,10 +30752,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="602"/>
-      <c r="Q4" s="604"/>
+      <c r="P4" s="625"/>
+      <c r="Q4" s="627"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="605"/>
+      <c r="S4" s="628"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -30721,16 +30767,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="584" t="s">
+      <c r="AB4" s="588" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="585"/>
+      <c r="AC4" s="589"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="586" t="s">
+      <c r="AE4" s="590" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="586"/>
-      <c r="AG4" s="586"/>
+      <c r="AF4" s="590"/>
+      <c r="AG4" s="590"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -32218,10 +32264,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="591" t="s">
+      <c r="AE23" s="595" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="592"/>
+      <c r="AF23" s="596"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -32361,11 +32407,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="593" t="s">
+      <c r="AE25" s="597" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="594"/>
-      <c r="AG25" s="597">
+      <c r="AF25" s="598"/>
+      <c r="AG25" s="601">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -32437,9 +32483,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="595"/>
-      <c r="AF26" s="596"/>
-      <c r="AG26" s="598"/>
+      <c r="AE26" s="599"/>
+      <c r="AF26" s="600"/>
+      <c r="AG26" s="602"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -32649,10 +32695,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="587" t="s">
+      <c r="AB29" s="591" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="589">
+      <c r="AC29" s="593">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -32717,8 +32763,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="588"/>
-      <c r="AC30" s="590"/>
+      <c r="AB30" s="592"/>
+      <c r="AC30" s="594"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -33231,11 +33277,11 @@
       <c r="L39" s="357">
         <v>11500</v>
       </c>
-      <c r="M39" s="614">
+      <c r="M39" s="620">
         <f>SUM(M5:M38)</f>
         <v>2842451</v>
       </c>
-      <c r="N39" s="616">
+      <c r="N39" s="622">
         <f>SUM(N5:N38)</f>
         <v>271503</v>
       </c>
@@ -33286,8 +33332,8 @@
       <c r="L40" s="357">
         <v>20880</v>
       </c>
-      <c r="M40" s="615"/>
-      <c r="N40" s="617"/>
+      <c r="M40" s="621"/>
+      <c r="N40" s="623"/>
       <c r="O40" s="392"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -33481,10 +33527,10 @@
       <c r="L44" s="358">
         <v>986</v>
       </c>
-      <c r="M44" s="618" t="s">
+      <c r="M44" s="624" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="618"/>
+      <c r="N44" s="624"/>
       <c r="O44" s="392"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -34058,7 +34104,7 @@
         <f>968.75+155</f>
         <v>1123.75</v>
       </c>
-      <c r="M58" s="636">
+      <c r="M58" s="637">
         <f ca="1">SUM(M45:M58)</f>
         <v>2805120</v>
       </c>
@@ -34096,7 +34142,7 @@
       <c r="L59" s="458">
         <v>1480.06</v>
       </c>
-      <c r="M59" s="637"/>
+      <c r="M59" s="638"/>
       <c r="N59" s="42"/>
       <c r="O59" s="392"/>
       <c r="P59" s="7"/>
@@ -34131,10 +34177,10 @@
       <c r="L60" s="458">
         <v>2479.5</v>
       </c>
-      <c r="M60" s="608" t="s">
+      <c r="M60" s="614" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="609"/>
+      <c r="N60" s="615"/>
       <c r="O60" s="392"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -34201,11 +34247,11 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="640">
+      <c r="M62" s="633">
         <f ca="1">M58-M39</f>
         <v>-37331</v>
       </c>
-      <c r="N62" s="641"/>
+      <c r="N62" s="634"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -34237,8 +34283,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="642"/>
-      <c r="N63" s="643"/>
+      <c r="M63" s="635"/>
+      <c r="N63" s="636"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -34270,10 +34316,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="628">
+      <c r="M64" s="641">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="629"/>
+      <c r="N64" s="642"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -34304,10 +34350,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="630">
+      <c r="M65" s="643">
         <v>-163726</v>
       </c>
-      <c r="N65" s="631"/>
+      <c r="N65" s="644"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -34338,12 +34384,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="632">
+      <c r="M66" s="645">
         <f ca="1">SUM(M65+M64+M62)</f>
         <v>-583779.22</v>
       </c>
-      <c r="N66" s="633"/>
-      <c r="O66" s="638" t="s">
+      <c r="N66" s="646"/>
+      <c r="O66" s="639" t="s">
         <v>821</v>
       </c>
       <c r="P66" s="7"/>
@@ -34397,9 +34443,9 @@
         <f>SUM(L5:L66)</f>
         <v>482695.31000000006</v>
       </c>
-      <c r="M67" s="634"/>
-      <c r="N67" s="635"/>
-      <c r="O67" s="639"/>
+      <c r="M67" s="647"/>
+      <c r="N67" s="648"/>
+      <c r="O67" s="640"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
@@ -34467,30 +34513,30 @@
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="530">
+      <c r="R70" s="552">
         <f>R67+S67</f>
         <v>7378939.6599999992</v>
       </c>
-      <c r="S70" s="531"/>
+      <c r="S70" s="553"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="532" t="s">
+      <c r="D71" s="554" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="532"/>
+      <c r="E71" s="554"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="533" t="s">
+      <c r="I71" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="534"/>
-      <c r="K71" s="535">
+      <c r="J71" s="556"/>
+      <c r="K71" s="557">
         <f>F73+F74+F75</f>
         <v>536310.85999999964</v>
       </c>
-      <c r="L71" s="536"/>
+      <c r="L71" s="558"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -34524,11 +34570,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="537">
+      <c r="K73" s="559">
         <f>-C4</f>
         <v>-250140.85</v>
       </c>
-      <c r="L73" s="619"/>
+      <c r="L73" s="603"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -34581,14 +34627,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="644" t="s">
+      <c r="I77" s="629" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="645"/>
-      <c r="K77" s="640">
+      <c r="J77" s="630"/>
+      <c r="K77" s="633">
         <v>37331</v>
       </c>
-      <c r="L77" s="641"/>
+      <c r="L77" s="634"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -34597,10 +34643,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="646"/>
-      <c r="J78" s="647"/>
-      <c r="K78" s="642"/>
-      <c r="L78" s="643"/>
+      <c r="I78" s="631"/>
+      <c r="J78" s="632"/>
+      <c r="K78" s="635"/>
+      <c r="L78" s="636"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -34652,7 +34698,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="599"/>
+      <c r="AC81" s="576"/>
       <c r="AD81" s="486"/>
       <c r="AE81" s="486"/>
       <c r="AF81" s="486"/>
@@ -34665,7 +34711,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="599"/>
+      <c r="AC82" s="576"/>
       <c r="AD82" s="486"/>
       <c r="AE82" s="486"/>
       <c r="AF82" s="486"/>
@@ -34762,16 +34808,21 @@
     <sortCondition ref="N45:N55"/>
   </sortState>
   <mergeCells count="41">
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AE25:AF26"/>
+    <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="AB2:AG3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="AC29:AC30"/>
     <mergeCell ref="M39:M40"/>
     <mergeCell ref="N39:N40"/>
@@ -34788,21 +34839,16 @@
     <mergeCell ref="M65:N65"/>
     <mergeCell ref="M66:N67"/>
     <mergeCell ref="M44:N44"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="AB2:AG3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AE25:AF26"/>
-    <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36342,8 +36388,8 @@
   </sheetPr>
   <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36378,20 +36424,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="600" t="s">
+      <c r="B1" s="574" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>836</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -36401,7 +36447,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="601"/>
+      <c r="B2" s="575"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -36420,27 +36466,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="583" t="s">
+      <c r="AB2" s="587" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="583"/>
-      <c r="AD2" s="583"/>
-      <c r="AE2" s="583"/>
-      <c r="AF2" s="583"/>
-      <c r="AG2" s="583"/>
+      <c r="AC2" s="587"/>
+      <c r="AD2" s="587"/>
+      <c r="AE2" s="587"/>
+      <c r="AF2" s="587"/>
+      <c r="AG2" s="587"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -36448,13 +36494,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="602" t="s">
+      <c r="P3" s="625" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="604" t="s">
+      <c r="Q3" s="627" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="605" t="s">
+      <c r="S3" s="628" t="s">
         <v>868</v>
       </c>
       <c r="W3" s="213" t="s">
@@ -36466,12 +36512,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="583"/>
-      <c r="AC3" s="583"/>
-      <c r="AD3" s="583"/>
-      <c r="AE3" s="583"/>
-      <c r="AF3" s="583"/>
-      <c r="AG3" s="583"/>
+      <c r="AB3" s="587"/>
+      <c r="AC3" s="587"/>
+      <c r="AD3" s="587"/>
+      <c r="AE3" s="587"/>
+      <c r="AF3" s="587"/>
+      <c r="AG3" s="587"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -36484,14 +36530,14 @@
       <c r="D4" s="23">
         <v>44439</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="603" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="626" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -36502,10 +36548,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="602"/>
-      <c r="Q4" s="604"/>
+      <c r="P4" s="625"/>
+      <c r="Q4" s="627"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="605"/>
+      <c r="S4" s="628"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -36517,16 +36563,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="584" t="s">
+      <c r="AB4" s="588" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="585"/>
+      <c r="AC4" s="589"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="586" t="s">
+      <c r="AE4" s="590" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="586"/>
-      <c r="AG4" s="586"/>
+      <c r="AF4" s="590"/>
+      <c r="AG4" s="590"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -36634,7 +36680,7 @@
       </c>
       <c r="O6" s="491"/>
       <c r="P6" s="389">
-        <v>0</v>
+        <v>5529</v>
       </c>
       <c r="Q6" s="447">
         <v>0</v>
@@ -36766,7 +36812,7 @@
         <v>4195</v>
       </c>
       <c r="D8" s="141" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E8" s="136">
         <v>44443</v>
@@ -36785,7 +36831,7 @@
         <v>44443</v>
       </c>
       <c r="K8" s="158" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="L8" s="46">
         <f>24584.13+400</f>
@@ -36844,25 +36890,34 @@
       <c r="B9" s="134">
         <v>44444</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="141"/>
+      <c r="C9" s="36">
+        <f>16396+80</f>
+        <v>16476</v>
+      </c>
+      <c r="D9" s="141" t="s">
+        <v>874</v>
+      </c>
       <c r="E9" s="136">
         <v>44444</v>
       </c>
-      <c r="F9" s="37"/>
+      <c r="F9" s="37">
+        <v>151604</v>
+      </c>
       <c r="G9" s="137"/>
       <c r="H9" s="138">
         <v>44444</v>
       </c>
-      <c r="I9" s="38"/>
+      <c r="I9" s="38">
+        <v>700</v>
+      </c>
       <c r="J9" s="52"/>
       <c r="K9" s="159"/>
       <c r="L9" s="46"/>
       <c r="M9" s="444">
-        <v>0</v>
+        <v>124399</v>
       </c>
       <c r="N9" s="334">
-        <v>0</v>
+        <v>10029</v>
       </c>
       <c r="O9" s="491"/>
       <c r="P9" s="389">
@@ -36873,7 +36928,7 @@
       </c>
       <c r="R9" s="7">
         <f>C9+I9+M9+N9+L9</f>
-        <v>0</v>
+        <v>151604</v>
       </c>
       <c r="S9" s="6">
         <f t="shared" si="0"/>
@@ -36911,40 +36966,55 @@
       <c r="B10" s="134">
         <v>44445</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="140"/>
+      <c r="C10" s="36">
+        <v>1428</v>
+      </c>
+      <c r="D10" s="140" t="s">
+        <v>875</v>
+      </c>
       <c r="E10" s="136">
         <v>44445</v>
       </c>
-      <c r="F10" s="37"/>
+      <c r="F10" s="37">
+        <v>114440</v>
+      </c>
       <c r="G10" s="137"/>
       <c r="H10" s="138">
         <v>44445</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="160"/>
-      <c r="L10" s="53"/>
+      <c r="I10" s="38">
+        <v>2640</v>
+      </c>
+      <c r="J10" s="52">
+        <v>44445</v>
+      </c>
+      <c r="K10" s="663" t="s">
+        <v>876</v>
+      </c>
+      <c r="L10" s="53">
+        <v>3850</v>
+      </c>
       <c r="M10" s="444">
-        <v>0</v>
-      </c>
-      <c r="N10" s="334">
-        <v>0</v>
+        <v>104650</v>
+      </c>
+      <c r="N10" s="456">
+        <f>4918+60</f>
+        <v>4978</v>
       </c>
       <c r="O10" s="491"/>
       <c r="P10" s="389">
-        <v>0</v>
+        <v>3106</v>
       </c>
       <c r="Q10" s="447">
         <v>0</v>
       </c>
       <c r="R10" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S10" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>117546</v>
+      </c>
+      <c r="S10" s="201">
+        <f t="shared" si="0"/>
+        <v>3106</v>
       </c>
       <c r="T10" s="54"/>
       <c r="W10" s="213" t="s">
@@ -36978,25 +37048,40 @@
       <c r="B11" s="134">
         <v>44446</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="139"/>
+      <c r="C11" s="36">
+        <v>12110</v>
+      </c>
+      <c r="D11" s="139" t="s">
+        <v>877</v>
+      </c>
       <c r="E11" s="136">
         <v>44446</v>
       </c>
-      <c r="F11" s="37"/>
+      <c r="F11" s="37">
+        <v>82272</v>
+      </c>
       <c r="G11" s="137"/>
       <c r="H11" s="138">
         <v>44446</v>
       </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="292"/>
-      <c r="K11" s="161"/>
-      <c r="L11" s="46"/>
+      <c r="I11" s="38">
+        <v>2188</v>
+      </c>
+      <c r="J11" s="292">
+        <v>44446</v>
+      </c>
+      <c r="K11" s="665" t="s">
+        <v>878</v>
+      </c>
+      <c r="L11" s="46">
+        <v>8000</v>
+      </c>
       <c r="M11" s="444">
-        <v>0</v>
-      </c>
-      <c r="N11" s="334">
-        <v>0</v>
+        <v>50319</v>
+      </c>
+      <c r="N11" s="456">
+        <f>9435+220</f>
+        <v>9655</v>
       </c>
       <c r="O11" s="491"/>
       <c r="P11" s="389">
@@ -37007,7 +37092,7 @@
       </c>
       <c r="R11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>82272</v>
       </c>
       <c r="S11" s="6">
         <f t="shared" si="0"/>
@@ -37045,25 +37130,33 @@
       <c r="B12" s="134">
         <v>44447</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="139"/>
+      <c r="C12" s="36">
+        <v>8170</v>
+      </c>
+      <c r="D12" s="139" t="s">
+        <v>879</v>
+      </c>
       <c r="E12" s="136">
         <v>44447</v>
       </c>
-      <c r="F12" s="37"/>
+      <c r="F12" s="37">
+        <v>142225</v>
+      </c>
       <c r="G12" s="137"/>
       <c r="H12" s="138">
         <v>44447</v>
       </c>
-      <c r="I12" s="38"/>
+      <c r="I12" s="38">
+        <v>4495</v>
+      </c>
       <c r="J12" s="52"/>
-      <c r="K12" s="451"/>
+      <c r="K12" s="664"/>
       <c r="L12" s="46"/>
       <c r="M12" s="444">
-        <v>0</v>
+        <v>124239</v>
       </c>
       <c r="N12" s="334">
-        <v>0</v>
+        <v>5321</v>
       </c>
       <c r="O12" s="491"/>
       <c r="P12" s="389">
@@ -37074,7 +37167,7 @@
       </c>
       <c r="R12" s="7">
         <f>C12+M12+N12+I12</f>
-        <v>0</v>
+        <v>142225</v>
       </c>
       <c r="S12" s="6">
         <f t="shared" si="0"/>
@@ -37112,25 +37205,39 @@
       <c r="B13" s="134">
         <v>44448</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="141"/>
+      <c r="C13" s="36">
+        <v>3518</v>
+      </c>
+      <c r="D13" s="141" t="s">
+        <v>880</v>
+      </c>
       <c r="E13" s="136">
         <v>44448</v>
       </c>
-      <c r="F13" s="37"/>
+      <c r="F13" s="37">
+        <v>98134</v>
+      </c>
       <c r="G13" s="137"/>
       <c r="H13" s="138">
         <v>44448</v>
       </c>
-      <c r="I13" s="38"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="171"/>
-      <c r="L13" s="46"/>
+      <c r="I13" s="38">
+        <v>545</v>
+      </c>
+      <c r="J13" s="52">
+        <v>44448</v>
+      </c>
+      <c r="K13" s="171" t="s">
+        <v>881</v>
+      </c>
+      <c r="L13" s="46">
+        <v>8000</v>
+      </c>
       <c r="M13" s="444">
-        <v>0</v>
+        <v>74741</v>
       </c>
       <c r="N13" s="334">
-        <v>0</v>
+        <v>11330</v>
       </c>
       <c r="O13" s="491"/>
       <c r="P13" s="389">
@@ -37141,7 +37248,7 @@
       </c>
       <c r="R13" s="7">
         <f>C13+I13+M13+N13+L13</f>
-        <v>0</v>
+        <v>98134</v>
       </c>
       <c r="S13" s="6">
         <f t="shared" si="0"/>
@@ -37179,25 +37286,39 @@
       <c r="B14" s="134">
         <v>44449</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="140"/>
+      <c r="C14" s="36">
+        <v>7865</v>
+      </c>
+      <c r="D14" s="140" t="s">
+        <v>882</v>
+      </c>
       <c r="E14" s="136">
         <v>44449</v>
       </c>
-      <c r="F14" s="37"/>
+      <c r="F14" s="37">
+        <v>141083</v>
+      </c>
       <c r="G14" s="137"/>
       <c r="H14" s="138">
         <v>44449</v>
       </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="158"/>
-      <c r="L14" s="46"/>
+      <c r="I14" s="38">
+        <v>999</v>
+      </c>
+      <c r="J14" s="52">
+        <v>44449</v>
+      </c>
+      <c r="K14" s="171" t="s">
+        <v>563</v>
+      </c>
+      <c r="L14" s="46">
+        <v>10000</v>
+      </c>
       <c r="M14" s="444">
-        <v>0</v>
+        <v>110524</v>
       </c>
       <c r="N14" s="334">
-        <v>0</v>
+        <v>11695</v>
       </c>
       <c r="O14" s="491"/>
       <c r="P14" s="389">
@@ -37208,7 +37329,7 @@
       </c>
       <c r="R14" s="7">
         <f>C14+I14+M14+N14+L14</f>
-        <v>0</v>
+        <v>141083</v>
       </c>
       <c r="S14" s="6">
         <f t="shared" si="0"/>
@@ -37246,25 +37367,41 @@
       <c r="B15" s="134">
         <v>44450</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="139"/>
+      <c r="C15" s="36">
+        <v>18579</v>
+      </c>
+      <c r="D15" s="139" t="s">
+        <v>883</v>
+      </c>
       <c r="E15" s="136">
         <v>44450</v>
       </c>
-      <c r="F15" s="37"/>
+      <c r="F15" s="37">
+        <v>162172</v>
+      </c>
       <c r="G15" s="137"/>
       <c r="H15" s="138">
         <v>44450</v>
       </c>
-      <c r="I15" s="38"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="158"/>
-      <c r="L15" s="46"/>
+      <c r="I15" s="38">
+        <v>550</v>
+      </c>
+      <c r="J15" s="52">
+        <v>44450</v>
+      </c>
+      <c r="K15" s="158" t="s">
+        <v>884</v>
+      </c>
+      <c r="L15" s="666">
+        <f>23427+400</f>
+        <v>23827</v>
+      </c>
       <c r="M15" s="444">
-        <v>0</v>
-      </c>
-      <c r="N15" s="334">
-        <v>0</v>
+        <v>109704</v>
+      </c>
+      <c r="N15" s="456">
+        <f>9028+349+135</f>
+        <v>9512</v>
       </c>
       <c r="O15" s="491"/>
       <c r="P15" s="389">
@@ -37275,7 +37412,7 @@
       </c>
       <c r="R15" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>162172</v>
       </c>
       <c r="S15" s="6">
         <f t="shared" si="0"/>
@@ -37822,10 +37959,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="591" t="s">
+      <c r="AE23" s="595" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="592"/>
+      <c r="AF23" s="596"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -37945,11 +38082,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="593" t="s">
+      <c r="AE25" s="597" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="594"/>
-      <c r="AG25" s="597">
+      <c r="AF25" s="598"/>
+      <c r="AG25" s="601">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -38011,9 +38148,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="595"/>
-      <c r="AF26" s="596"/>
-      <c r="AG26" s="598"/>
+      <c r="AE26" s="599"/>
+      <c r="AF26" s="600"/>
+      <c r="AG26" s="602"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -38179,10 +38316,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="587" t="s">
+      <c r="AB29" s="591" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="589">
+      <c r="AC29" s="593">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -38237,8 +38374,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="588"/>
-      <c r="AC30" s="590"/>
+      <c r="AB30" s="592"/>
+      <c r="AC30" s="594"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -38593,8 +38730,12 @@
       <c r="W37" s="213" t="s">
         <v>88</v>
       </c>
-      <c r="X37" s="221"/>
-      <c r="Y37" s="207"/>
+      <c r="X37" s="221">
+        <v>44447</v>
+      </c>
+      <c r="Y37" s="207">
+        <v>2000</v>
+      </c>
       <c r="AC37" s="321" t="s">
         <v>603</v>
       </c>
@@ -38639,8 +38780,12 @@
       <c r="W38" s="213" t="s">
         <v>89</v>
       </c>
-      <c r="X38" s="221"/>
-      <c r="Y38" s="207"/>
+      <c r="X38" s="221">
+        <v>44447</v>
+      </c>
+      <c r="Y38" s="207">
+        <v>2000</v>
+      </c>
       <c r="AC38" s="321" t="s">
         <v>604</v>
       </c>
@@ -38663,20 +38808,20 @@
       <c r="J39" s="299"/>
       <c r="K39" s="246"/>
       <c r="L39" s="46"/>
-      <c r="M39" s="614">
+      <c r="M39" s="620">
         <f>SUM(M5:M38)</f>
-        <v>364023</v>
-      </c>
-      <c r="N39" s="616">
+        <v>1062599</v>
+      </c>
+      <c r="N39" s="622">
         <f>SUM(N5:N38)</f>
-        <v>29927</v>
+        <v>92447</v>
       </c>
       <c r="O39" s="392"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <f>SUM(R5:R38)</f>
-        <v>480161.92000000004</v>
+        <v>1375197.92</v>
       </c>
       <c r="T39" s="48"/>
       <c r="W39" s="213" t="s">
@@ -38706,8 +38851,8 @@
       <c r="J40" s="299"/>
       <c r="K40" s="172"/>
       <c r="L40" s="46"/>
-      <c r="M40" s="615"/>
-      <c r="N40" s="617"/>
+      <c r="M40" s="621"/>
+      <c r="N40" s="623"/>
       <c r="O40" s="392"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -38851,10 +38996,10 @@
       <c r="J44" s="299"/>
       <c r="K44" s="528"/>
       <c r="L44" s="71"/>
-      <c r="M44" s="618" t="s">
+      <c r="M44" s="624" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="618"/>
+      <c r="N44" s="624"/>
       <c r="O44" s="392"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -39320,7 +39465,7 @@
       <c r="J58" s="529"/>
       <c r="K58" s="468"/>
       <c r="L58" s="50"/>
-      <c r="M58" s="636">
+      <c r="M58" s="637">
         <f t="shared" ref="M58" si="2">SUM(M45:M57)</f>
         <v>0</v>
       </c>
@@ -39354,7 +39499,7 @@
       <c r="J59" s="529"/>
       <c r="K59" s="243"/>
       <c r="L59" s="50"/>
-      <c r="M59" s="637"/>
+      <c r="M59" s="638"/>
       <c r="N59" s="42"/>
       <c r="O59" s="392"/>
       <c r="P59" s="7"/>
@@ -39385,10 +39530,10 @@
       <c r="J60" s="529"/>
       <c r="K60" s="468"/>
       <c r="L60" s="50"/>
-      <c r="M60" s="608" t="s">
+      <c r="M60" s="614" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="609"/>
+      <c r="N60" s="615"/>
       <c r="O60" s="392"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -39449,10 +39594,10 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="640">
+      <c r="M62" s="633">
         <v>-37331</v>
       </c>
-      <c r="N62" s="641"/>
+      <c r="N62" s="634"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -39484,8 +39629,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="642"/>
-      <c r="N63" s="643"/>
+      <c r="M63" s="635"/>
+      <c r="N63" s="636"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -39517,10 +39662,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="628">
+      <c r="M64" s="641">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="629"/>
+      <c r="N64" s="642"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -39551,10 +39696,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="630">
+      <c r="M65" s="643">
         <v>-163726</v>
       </c>
-      <c r="N65" s="631"/>
+      <c r="N65" s="644"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -39585,12 +39730,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="632">
+      <c r="M66" s="645">
         <f>SUM(M65+M64+M62)</f>
         <v>-583779.22</v>
       </c>
-      <c r="N66" s="633"/>
-      <c r="O66" s="638"/>
+      <c r="N66" s="646"/>
+      <c r="O66" s="639"/>
       <c r="P66" s="7"/>
       <c r="Q66" s="7"/>
       <c r="R66" s="84">
@@ -39616,7 +39761,7 @@
       </c>
       <c r="C67" s="86">
         <f>SUM(C5:C66)</f>
-        <v>38596.79</v>
+        <v>106742.79000000001</v>
       </c>
       <c r="D67" s="87"/>
       <c r="E67" s="88" t="s">
@@ -39624,7 +39769,7 @@
       </c>
       <c r="F67" s="89">
         <f>SUM(F5:F66)</f>
-        <v>466103</v>
+        <v>1358033</v>
       </c>
       <c r="G67" s="87"/>
       <c r="H67" s="90" t="s">
@@ -39632,7 +39777,7 @@
       </c>
       <c r="I67" s="91">
         <f>SUM(I5:I66)</f>
-        <v>2631</v>
+        <v>14748</v>
       </c>
       <c r="J67" s="92"/>
       <c r="K67" s="93" t="s">
@@ -39640,20 +39785,20 @@
       </c>
       <c r="L67" s="522">
         <f>SUM(L5:L66)</f>
-        <v>44984.130000000005</v>
-      </c>
-      <c r="M67" s="634"/>
-      <c r="N67" s="635"/>
-      <c r="O67" s="639"/>
+        <v>98661.13</v>
+      </c>
+      <c r="M67" s="647"/>
+      <c r="N67" s="648"/>
+      <c r="O67" s="640"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
         <f>SUM(R5:R66)</f>
-        <v>960323.84000000008</v>
+        <v>2750395.84</v>
       </c>
       <c r="S67" s="7">
         <f>SUM(S5:S66)</f>
-        <v>14058.920000000013</v>
+        <v>17164.920000000013</v>
       </c>
       <c r="T67" s="97"/>
       <c r="W67" s="210"/>
@@ -39683,7 +39828,7 @@
       <c r="J69" s="101"/>
       <c r="K69" s="541">
         <f>I67+L67</f>
-        <v>47615.130000000005</v>
+        <v>113409.13</v>
       </c>
       <c r="L69" s="542"/>
       <c r="M69" s="470"/>
@@ -39708,34 +39853,34 @@
       <c r="E70" s="551"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
-        <v>379891.08</v>
+        <v>1137881.08</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="530">
+      <c r="R70" s="552">
         <f>R67+S67</f>
-        <v>974382.76000000013</v>
-      </c>
-      <c r="S70" s="531"/>
+        <v>2767560.76</v>
+      </c>
+      <c r="S70" s="553"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="532" t="s">
+      <c r="D71" s="554" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="532"/>
+      <c r="E71" s="554"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="533" t="s">
+      <c r="I71" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="534"/>
-      <c r="K71" s="535">
+      <c r="J71" s="556"/>
+      <c r="K71" s="557">
         <f>F73+F74+F75</f>
-        <v>-2000822</v>
-      </c>
-      <c r="L71" s="536"/>
+        <v>-1242832</v>
+      </c>
+      <c r="L71" s="558"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -39762,18 +39907,18 @@
       </c>
       <c r="F73" s="95">
         <f>SUM(F70:F72)</f>
-        <v>-2000822</v>
+        <v>-1242832</v>
       </c>
       <c r="H73" s="34"/>
       <c r="I73" s="114" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="537">
+      <c r="K73" s="559">
         <f>-C4</f>
         <v>-365611.59</v>
       </c>
-      <c r="L73" s="619"/>
+      <c r="L73" s="603"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -39807,7 +39952,7 @@
       <c r="J75" s="548"/>
       <c r="K75" s="549">
         <f>K71+K73</f>
-        <v>-2366433.59</v>
+        <v>-1608443.59</v>
       </c>
       <c r="L75" s="549"/>
       <c r="R75" s="50"/>
@@ -39824,14 +39969,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="644" t="s">
+      <c r="I77" s="629" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="645"/>
-      <c r="K77" s="640">
-        <v>0</v>
-      </c>
-      <c r="L77" s="641"/>
+      <c r="J77" s="630"/>
+      <c r="K77" s="633">
+        <v>0</v>
+      </c>
+      <c r="L77" s="634"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -39840,10 +39985,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="646"/>
-      <c r="J78" s="647"/>
-      <c r="K78" s="642"/>
-      <c r="L78" s="643"/>
+      <c r="I78" s="631"/>
+      <c r="J78" s="632"/>
+      <c r="K78" s="635"/>
+      <c r="L78" s="636"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -39895,7 +40040,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="599"/>
+      <c r="AC81" s="576"/>
       <c r="AD81" s="526"/>
       <c r="AE81" s="526"/>
       <c r="AF81" s="526"/>
@@ -39908,7 +40053,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="599"/>
+      <c r="AC82" s="576"/>
       <c r="AD82" s="526"/>
       <c r="AE82" s="526"/>
       <c r="AF82" s="526"/>
@@ -40002,16 +40147,24 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="AB2:AG3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
     <mergeCell ref="M62:N63"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AE4:AG4"/>
@@ -40025,24 +40178,16 @@
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="M58:M59"/>
     <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="AB2:AG3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -42585,10 +42730,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A46:G63"/>
+  <dimension ref="A43:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42596,42 +42741,96 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="32"/>
-      <c r="B47" s="648" t="s">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="649" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="649"/>
-      <c r="D47" s="649"/>
-      <c r="E47" s="650"/>
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
-        <v>44443</v>
-      </c>
+      <c r="C44" s="650"/>
+      <c r="D44" s="650"/>
+      <c r="E44" s="651"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="19">
+        <v>44451</v>
+      </c>
+      <c r="B45" s="196" t="s">
+        <v>886</v>
+      </c>
+      <c r="C45" s="197">
+        <v>162.4</v>
+      </c>
+      <c r="D45" s="198" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="199" t="s">
+        <v>887</v>
+      </c>
+      <c r="F45" s="72">
+        <v>81</v>
+      </c>
+      <c r="G45" s="530"/>
+    </row>
+    <row r="46" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="196" t="s">
+        <v>885</v>
+      </c>
+      <c r="C46" s="197">
+        <v>0</v>
+      </c>
+      <c r="D46" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F46" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="196" t="s">
+        <v>885</v>
+      </c>
+      <c r="C47" s="197">
+        <v>0</v>
+      </c>
+      <c r="D47" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F47" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
       <c r="B48" s="196" t="s">
-        <v>872</v>
+        <v>885</v>
       </c>
       <c r="C48" s="197">
-        <v>2201.65</v>
-      </c>
-      <c r="D48" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E48" s="199" t="s">
-        <v>873</v>
+        <v>611</v>
       </c>
       <c r="F48" s="72">
-        <v>47</v>
-      </c>
-      <c r="G48" s="662"/>
-    </row>
-    <row r="49" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C49" s="197">
         <v>0</v>
@@ -42640,16 +42839,16 @@
         <v>33</v>
       </c>
       <c r="E49" s="199" t="s">
-        <v>27</v>
+        <v>611</v>
       </c>
       <c r="F49" s="72">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
       <c r="B50" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C50" s="197">
         <v>0</v>
@@ -42667,7 +42866,7 @@
     <row r="51" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C51" s="197">
         <v>0</v>
@@ -42682,15 +42881,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+    <row r="52" spans="1:6" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="330"/>
       <c r="B52" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C52" s="197">
         <v>0</v>
       </c>
-      <c r="D52" s="200" t="s">
+      <c r="D52" s="331" t="s">
         <v>33</v>
       </c>
       <c r="E52" s="199" t="s">
@@ -42701,14 +42900,14 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="329"/>
       <c r="B53" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C53" s="197">
         <v>0</v>
       </c>
-      <c r="D53" s="200" t="s">
+      <c r="D53" s="198" t="s">
         <v>33</v>
       </c>
       <c r="E53" s="199" t="s">
@@ -42721,7 +42920,7 @@
     <row r="54" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C54" s="197">
         <v>0</v>
@@ -42736,15 +42935,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="330"/>
+    <row r="55" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="19"/>
       <c r="B55" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C55" s="197">
         <v>0</v>
       </c>
-      <c r="D55" s="331" t="s">
+      <c r="D55" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E55" s="199" t="s">
@@ -42755,14 +42954,14 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="329"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C56" s="197">
         <v>0</v>
       </c>
-      <c r="D56" s="198" t="s">
+      <c r="D56" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E56" s="199" t="s">
@@ -42775,7 +42974,7 @@
     <row r="57" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C57" s="197">
         <v>0</v>
@@ -42793,7 +42992,7 @@
     <row r="58" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="19"/>
       <c r="B58" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C58" s="197">
         <v>0</v>
@@ -42811,7 +43010,7 @@
     <row r="59" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="196" t="s">
-        <v>611</v>
+        <v>885</v>
       </c>
       <c r="C59" s="197">
         <v>0</v>
@@ -42826,62 +43025,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
-      <c r="B60" s="196" t="s">
-        <v>611</v>
-      </c>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C60" s="197">
-        <v>0</v>
-      </c>
-      <c r="D60" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E60" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F60" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
-      <c r="B61" s="196" t="s">
-        <v>611</v>
-      </c>
-      <c r="C61" s="197">
-        <v>0</v>
-      </c>
-      <c r="D61" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E61" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F61" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
-      <c r="B62" s="196" t="s">
-        <v>611</v>
-      </c>
-      <c r="C62" s="197">
-        <v>0</v>
-      </c>
-      <c r="D62" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E62" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F62" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="197">
         <v>0</v>
       </c>
     </row>
@@ -42890,7 +43035,7 @@
     <sortCondition ref="B45:B46"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B44:E44"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -42928,32 +43073,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="657" t="s">
+      <c r="B1" s="653" t="s">
         <v>726</v>
       </c>
-      <c r="C1" s="657"/>
-      <c r="D1" s="657"/>
-      <c r="E1" s="657"/>
-      <c r="H1" s="658" t="s">
+      <c r="C1" s="653"/>
+      <c r="D1" s="653"/>
+      <c r="E1" s="653"/>
+      <c r="H1" s="656" t="s">
         <v>726</v>
       </c>
-      <c r="I1" s="658"/>
-      <c r="J1" s="658"/>
+      <c r="I1" s="656"/>
+      <c r="J1" s="656"/>
       <c r="K1" s="205"/>
       <c r="L1" s="205"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="657" t="s">
+      <c r="O1" s="653" t="s">
         <v>725</v>
       </c>
-      <c r="P1" s="657"/>
+      <c r="P1" s="653"/>
     </row>
     <row r="2" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="573" t="s">
+      <c r="E2" s="577" t="s">
         <v>562</v>
       </c>
       <c r="F2" s="496"/>
@@ -42979,7 +43124,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="365"/>
-      <c r="E3" s="573"/>
+      <c r="E3" s="577"/>
       <c r="F3" s="496"/>
       <c r="H3" s="444">
         <v>126476.5</v>
@@ -42991,10 +43136,10 @@
         <v>44378</v>
       </c>
       <c r="K3" s="495"/>
-      <c r="L3" s="618" t="s">
+      <c r="L3" s="624" t="s">
         <v>567</v>
       </c>
-      <c r="M3" s="618"/>
+      <c r="M3" s="624"/>
       <c r="O3" s="444">
         <v>64006</v>
       </c>
@@ -43538,7 +43683,7 @@
         <v>44391</v>
       </c>
       <c r="K16" s="495"/>
-      <c r="L16" s="606">
+      <c r="L16" s="612">
         <f>SUM(L4:L15)</f>
         <v>3606750</v>
       </c>
@@ -43579,7 +43724,7 @@
         <v>44392</v>
       </c>
       <c r="K17" s="495"/>
-      <c r="L17" s="607"/>
+      <c r="L17" s="613"/>
       <c r="M17" s="475"/>
       <c r="O17" s="444">
         <v>0</v>
@@ -43652,10 +43797,10 @@
         <v>44394</v>
       </c>
       <c r="K19" s="495"/>
-      <c r="L19" s="608" t="s">
+      <c r="L19" s="614" t="s">
         <v>719</v>
       </c>
-      <c r="M19" s="609"/>
+      <c r="M19" s="615"/>
       <c r="O19" s="444">
         <v>0</v>
       </c>
@@ -43725,11 +43870,11 @@
         <v>44396</v>
       </c>
       <c r="K21" s="495"/>
-      <c r="L21" s="651">
+      <c r="L21" s="657">
         <f>L16-H37</f>
         <v>-383122.2200000002</v>
       </c>
-      <c r="M21" s="652"/>
+      <c r="M21" s="658"/>
       <c r="O21" s="444">
         <v>0</v>
       </c>
@@ -43763,8 +43908,8 @@
         <v>44397</v>
       </c>
       <c r="K22" s="495"/>
-      <c r="L22" s="653"/>
-      <c r="M22" s="654"/>
+      <c r="L22" s="659"/>
+      <c r="M22" s="660"/>
       <c r="O22" s="444">
         <v>0</v>
       </c>
@@ -44162,35 +44307,35 @@
       <c r="Q36" s="392"/>
     </row>
     <row r="37" spans="7:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H37" s="614">
+      <c r="H37" s="620">
         <f>SUM(H3:H36)</f>
         <v>3989872.22</v>
       </c>
-      <c r="I37" s="616">
+      <c r="I37" s="622">
         <f>SUM(I3:I36)</f>
         <v>688820.5</v>
       </c>
       <c r="J37" s="495"/>
       <c r="K37" s="495"/>
       <c r="L37" s="495"/>
-      <c r="O37" s="614">
+      <c r="O37" s="620">
         <f>SUM(O3:O36)</f>
         <v>1464800.09</v>
       </c>
-      <c r="P37" s="616">
+      <c r="P37" s="622">
         <f>SUM(P3:P36)</f>
         <v>121896</v>
       </c>
       <c r="Q37" s="392"/>
     </row>
     <row r="38" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H38" s="615"/>
-      <c r="I38" s="617"/>
+      <c r="H38" s="621"/>
+      <c r="I38" s="623"/>
       <c r="J38" s="495"/>
       <c r="K38" s="495"/>
       <c r="L38" s="495"/>
-      <c r="O38" s="615"/>
-      <c r="P38" s="617"/>
+      <c r="O38" s="621"/>
+      <c r="P38" s="623"/>
       <c r="Q38" s="392"/>
     </row>
     <row r="39" spans="7:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -44202,12 +44347,12 @@
     </row>
     <row r="40" spans="7:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G40" s="272"/>
-      <c r="H40" s="660"/>
-      <c r="I40" s="660"/>
-      <c r="O40" s="618" t="s">
+      <c r="H40" s="654"/>
+      <c r="I40" s="654"/>
+      <c r="O40" s="624" t="s">
         <v>567</v>
       </c>
-      <c r="P40" s="618"/>
+      <c r="P40" s="624"/>
       <c r="Q40" s="392"/>
     </row>
     <row r="41" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -44354,9 +44499,9 @@
     </row>
     <row r="53" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G53" s="272"/>
-      <c r="H53" s="661"/>
+      <c r="H53" s="655"/>
       <c r="I53" s="7"/>
-      <c r="O53" s="606">
+      <c r="O53" s="612">
         <f>SUM(O41:O52)</f>
         <v>1682687</v>
       </c>
@@ -44365,9 +44510,9 @@
     </row>
     <row r="54" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G54" s="272"/>
-      <c r="H54" s="661"/>
+      <c r="H54" s="655"/>
       <c r="I54" s="7"/>
-      <c r="O54" s="607"/>
+      <c r="O54" s="613"/>
       <c r="P54" s="475"/>
       <c r="Q54" s="392"/>
     </row>
@@ -44381,12 +44526,12 @@
     </row>
     <row r="56" spans="7:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="G56" s="272"/>
-      <c r="H56" s="660"/>
-      <c r="I56" s="660"/>
-      <c r="O56" s="608" t="s">
+      <c r="H56" s="654"/>
+      <c r="I56" s="654"/>
+      <c r="O56" s="614" t="s">
         <v>719</v>
       </c>
-      <c r="P56" s="609"/>
+      <c r="P56" s="615"/>
       <c r="Q56" s="392"/>
     </row>
     <row r="57" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -44399,8 +44544,8 @@
     </row>
     <row r="58" spans="7:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="272"/>
-      <c r="H58" s="659"/>
-      <c r="I58" s="659"/>
+      <c r="H58" s="652"/>
+      <c r="I58" s="652"/>
       <c r="O58" s="492">
         <f>O53-O37</f>
         <v>217886.90999999992</v>
@@ -44412,8 +44557,8 @@
     </row>
     <row r="59" spans="7:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="272"/>
-      <c r="H59" s="659"/>
-      <c r="I59" s="659"/>
+      <c r="H59" s="652"/>
+      <c r="I59" s="652"/>
       <c r="O59" s="505">
         <v>-383122.22</v>
       </c>
@@ -44441,14 +44586,20 @@
       <c r="P61" s="506"/>
     </row>
     <row r="62" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="O62" s="655">
+      <c r="O62" s="661">
         <f>SUM(O58:O61)</f>
         <v>-328961.31000000006</v>
       </c>
-      <c r="P62" s="656"/>
+      <c r="P62" s="662"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L16:L17"/>
     <mergeCell ref="H58:I59"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O37:O38"/>
@@ -44459,16 +44610,10 @@
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H53:H54"/>
     <mergeCell ref="H56:I56"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L16:L17"/>
     <mergeCell ref="O53:O54"/>
     <mergeCell ref="O56:P56"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L21:M22"/>
-    <mergeCell ref="O62:P62"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.13" top="0.43" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44490,12 +44635,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32"/>
-      <c r="B1" s="648" t="s">
+      <c r="B1" s="649" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="649"/>
-      <c r="D1" s="649"/>
-      <c r="E1" s="650"/>
+      <c r="C1" s="650"/>
+      <c r="D1" s="650"/>
+      <c r="E1" s="651"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -44577,12 +44722,12 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32"/>
-      <c r="B9" s="648" t="s">
+      <c r="B9" s="649" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="649"/>
-      <c r="D9" s="649"/>
-      <c r="E9" s="650"/>
+      <c r="C9" s="650"/>
+      <c r="D9" s="650"/>
+      <c r="E9" s="651"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -44738,12 +44883,12 @@
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32"/>
-      <c r="B20" s="648" t="s">
+      <c r="B20" s="649" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="649"/>
-      <c r="D20" s="649"/>
-      <c r="E20" s="650"/>
+      <c r="C20" s="650"/>
+      <c r="D20" s="650"/>
+      <c r="E20" s="651"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -44901,12 +45046,12 @@
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
-      <c r="B31" s="648" t="s">
+      <c r="B31" s="649" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="649"/>
-      <c r="D31" s="649"/>
-      <c r="E31" s="650"/>
+      <c r="C31" s="650"/>
+      <c r="D31" s="650"/>
+      <c r="E31" s="651"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -45060,12 +45205,12 @@
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32"/>
-      <c r="B42" s="648" t="s">
+      <c r="B42" s="649" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="649"/>
-      <c r="D42" s="649"/>
-      <c r="E42" s="650"/>
+      <c r="C42" s="650"/>
+      <c r="D42" s="650"/>
+      <c r="E42" s="651"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -45219,12 +45364,12 @@
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="32"/>
-      <c r="B54" s="648" t="s">
+      <c r="B54" s="649" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="649"/>
-      <c r="D54" s="649"/>
-      <c r="E54" s="650"/>
+      <c r="C54" s="650"/>
+      <c r="D54" s="650"/>
+      <c r="E54" s="651"/>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -45465,17 +45610,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -45506,17 +45651,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -45545,14 +45690,14 @@
       <c r="D4" s="23">
         <v>44230</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="558" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="537" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -48122,30 +48267,30 @@
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="530">
+      <c r="P65" s="552">
         <f>P62+Q62</f>
         <v>3144691.75</v>
       </c>
-      <c r="Q65" s="531"/>
+      <c r="Q65" s="553"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="532" t="s">
+      <c r="D66" s="554" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="532"/>
+      <c r="E66" s="554"/>
       <c r="F66" s="95">
         <v>-2261593.1</v>
       </c>
-      <c r="I66" s="533" t="s">
+      <c r="I66" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="534"/>
-      <c r="K66" s="535">
+      <c r="J66" s="556"/>
+      <c r="K66" s="557">
         <f>F68+F69+F70</f>
         <v>355407.6199999997</v>
       </c>
-      <c r="L66" s="536"/>
+      <c r="L66" s="558"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -48182,11 +48327,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="537">
+      <c r="K68" s="559">
         <f>-C4</f>
         <v>-209541.1</v>
       </c>
-      <c r="L68" s="538"/>
+      <c r="L68" s="560"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -48326,6 +48471,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -48337,12 +48488,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -49613,17 +49758,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>429</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -49653,17 +49798,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -49692,14 +49837,14 @@
       <c r="D4" s="23">
         <v>44257</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="558" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="537" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -52332,30 +52477,30 @@
       </c>
       <c r="I63" s="104"/>
       <c r="J63" s="105"/>
-      <c r="P63" s="530">
+      <c r="P63" s="552">
         <f>P60+Q60</f>
         <v>4585432.34</v>
       </c>
-      <c r="Q63" s="531"/>
+      <c r="Q63" s="553"/>
       <c r="S63" s="50"/>
     </row>
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="532" t="s">
+      <c r="D64" s="554" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="532"/>
+      <c r="E64" s="554"/>
       <c r="F64" s="95">
         <v>-3579271.89</v>
       </c>
-      <c r="I64" s="533" t="s">
+      <c r="I64" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J64" s="534"/>
-      <c r="K64" s="535">
+      <c r="J64" s="556"/>
+      <c r="K64" s="557">
         <f>F66+F67+F68</f>
         <v>-110332.85000000047</v>
       </c>
-      <c r="L64" s="536"/>
+      <c r="L64" s="558"/>
       <c r="P64" s="50"/>
       <c r="S64" s="107"/>
     </row>
@@ -52389,11 +52534,11 @@
         <v>21</v>
       </c>
       <c r="J66" s="115"/>
-      <c r="K66" s="537">
+      <c r="K66" s="559">
         <f>-C4</f>
         <v>-223014.26</v>
       </c>
-      <c r="L66" s="538"/>
+      <c r="L66" s="560"/>
       <c r="M66" s="116"/>
       <c r="P66" s="50"/>
       <c r="Q66" s="7"/>
@@ -52424,15 +52569,15 @@
       <c r="F68" s="120">
         <v>215362.9</v>
       </c>
-      <c r="I68" s="560" t="s">
+      <c r="I68" s="561" t="s">
         <v>431</v>
       </c>
-      <c r="J68" s="561"/>
-      <c r="K68" s="562">
+      <c r="J68" s="562"/>
+      <c r="K68" s="563">
         <f>K64+K66</f>
         <v>-333347.11000000045</v>
       </c>
-      <c r="L68" s="563"/>
+      <c r="L68" s="564"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
       <c r="S68" s="121"/>
@@ -52588,6 +52733,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="D63:E63"/>
     <mergeCell ref="P63:Q63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="I64:J64"/>
@@ -52599,12 +52750,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H62:I62"/>
     <mergeCell ref="K62:L62"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="D63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -54036,17 +54181,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>430</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -54076,17 +54221,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -54115,11 +54260,11 @@
       <c r="D4" s="23">
         <v>44291</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="558" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="537" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="565"/>
@@ -56638,37 +56783,37 @@
       <c r="D59" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="564"/>
+      <c r="E59" s="567"/>
       <c r="F59" s="103">
         <f>F56-K58-C56</f>
         <v>3048717.54</v>
       </c>
       <c r="I59" s="104"/>
       <c r="J59" s="105"/>
-      <c r="P59" s="530">
+      <c r="P59" s="552">
         <f>P56+Q56</f>
         <v>8073324.3200000003</v>
       </c>
-      <c r="Q59" s="531"/>
+      <c r="Q59" s="553"/>
       <c r="S59" s="50"/>
     </row>
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="532" t="s">
+      <c r="D60" s="554" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="532"/>
+      <c r="E60" s="554"/>
       <c r="F60" s="95">
         <v>-3102716.28</v>
       </c>
-      <c r="I60" s="533" t="s">
+      <c r="I60" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J60" s="534"/>
-      <c r="K60" s="535">
+      <c r="J60" s="556"/>
+      <c r="K60" s="557">
         <f>F62+F63+F64</f>
         <v>216465.62000000023</v>
       </c>
-      <c r="L60" s="536"/>
+      <c r="L60" s="558"/>
       <c r="P60" s="50"/>
       <c r="S60" s="107"/>
     </row>
@@ -56702,11 +56847,11 @@
         <v>21</v>
       </c>
       <c r="J62" s="115"/>
-      <c r="K62" s="537">
+      <c r="K62" s="559">
         <f>-C4</f>
         <v>-215362.9</v>
       </c>
-      <c r="L62" s="538"/>
+      <c r="L62" s="560"/>
       <c r="M62" s="116"/>
       <c r="P62" s="50"/>
       <c r="Q62" s="7"/>
@@ -56901,6 +57046,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="P59:Q59"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="I60:J60"/>
@@ -56912,12 +57063,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -57800,17 +57945,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="552" t="s">
+      <c r="C1" s="531" t="s">
         <v>504</v>
       </c>
-      <c r="D1" s="552"/>
-      <c r="E1" s="552"/>
-      <c r="F1" s="552"/>
-      <c r="G1" s="552"/>
-      <c r="H1" s="552"/>
-      <c r="I1" s="552"/>
-      <c r="J1" s="552"/>
-      <c r="K1" s="552"/>
+      <c r="D1" s="531"/>
+      <c r="E1" s="531"/>
+      <c r="F1" s="531"/>
+      <c r="G1" s="531"/>
+      <c r="H1" s="531"/>
+      <c r="I1" s="531"/>
+      <c r="J1" s="531"/>
+      <c r="K1" s="531"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -57840,17 +57985,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="553" t="s">
+      <c r="B3" s="532" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="554"/>
+      <c r="C3" s="533"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="555" t="s">
+      <c r="H3" s="534" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="555"/>
+      <c r="I3" s="534"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -57879,14 +58024,14 @@
       <c r="D4" s="23">
         <v>44320</v>
       </c>
-      <c r="E4" s="556" t="s">
+      <c r="E4" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="557"/>
-      <c r="H4" s="558" t="s">
+      <c r="F4" s="536"/>
+      <c r="H4" s="537" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="559"/>
+      <c r="I4" s="538"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -60794,18 +60939,18 @@
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="530">
+      <c r="P65" s="552">
         <f>P62+Q62</f>
         <v>5004562.5599999996</v>
       </c>
-      <c r="Q65" s="531"/>
+      <c r="Q65" s="553"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="567" t="s">
+      <c r="B66" s="568" t="s">
         <v>528</v>
       </c>
-      <c r="C66" s="568"/>
+      <c r="C66" s="569"/>
       <c r="D66" s="551" t="s">
         <v>502</v>
       </c>
@@ -60813,21 +60958,21 @@
       <c r="F66" s="95">
         <v>-3854423.8</v>
       </c>
-      <c r="I66" s="533" t="s">
+      <c r="I66" s="555" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="534"/>
-      <c r="K66" s="535">
+      <c r="J66" s="556"/>
+      <c r="K66" s="557">
         <f>F68+F69+F70</f>
         <v>14998.430000000139</v>
       </c>
-      <c r="L66" s="536"/>
+      <c r="L66" s="558"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
     <row r="67" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="569"/>
-      <c r="C67" s="570"/>
+      <c r="B67" s="570"/>
+      <c r="C67" s="571"/>
       <c r="D67" s="108"/>
       <c r="E67" s="60"/>
       <c r="F67" s="109">
@@ -60842,8 +60987,8 @@
       <c r="S67" s="50"/>
     </row>
     <row r="68" spans="2:19" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="571"/>
-      <c r="C68" s="572"/>
+      <c r="B68" s="572"/>
+      <c r="C68" s="573"/>
       <c r="E68" s="60" t="s">
         <v>20</v>
       </c>
@@ -60856,11 +61001,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="537">
+      <c r="K68" s="559">
         <f>-C4</f>
         <v>-249311.35999999999</v>
       </c>
-      <c r="L68" s="538"/>
+      <c r="L68" s="560"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -61055,6 +61200,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -61068,11 +61218,6 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="B66:C68"/>
     <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
cierre del 30 sept 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="17" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="19" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O     2 0 2 1    " sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2382" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="903">
   <si>
     <t>MORRALLA EN CAJA DE 11 SUR   2,800.00  +  $ 1,200.00 Total    $  4,000.00</t>
   </si>
@@ -3290,10 +3290,55 @@
     <t xml:space="preserve">#  </t>
   </si>
   <si>
-    <t>#  300498</t>
-  </si>
-  <si>
-    <t># 300500</t>
+    <t>TOCINETA-CHISTORRA-QUESO-MANTECA-POLLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             </t>
+  </si>
+  <si>
+    <t>CECINA---CHORIZO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>#  301575</t>
+  </si>
+  <si>
+    <t>dejaron mercancia</t>
+  </si>
+  <si>
+    <t>#  301632</t>
+  </si>
+  <si>
+    <t>#  301879</t>
+  </si>
+  <si>
+    <t># 301885</t>
+  </si>
+  <si>
+    <t>#  301883</t>
+  </si>
+  <si>
+    <t># 301884</t>
+  </si>
+  <si>
+    <t>#  301900</t>
+  </si>
+  <si>
+    <t>#  301904</t>
+  </si>
+  <si>
+    <t># 301905</t>
+  </si>
+  <si>
+    <t>#  301949</t>
+  </si>
+  <si>
+    <t>#  301974</t>
+  </si>
+  <si>
+    <t>#  301985</t>
   </si>
 </sst>
 </file>
@@ -3309,7 +3354,7 @@
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="58" x14ac:knownFonts="1">
+  <fonts count="59" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3760,6 +3805,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5180,7 +5232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="667">
+  <cellXfs count="672">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6326,6 +6378,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="24" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="13" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="90" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="92" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6642,12 +6716,6 @@
     <xf numFmtId="166" fontId="35" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="8" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6678,6 +6746,12 @@
     <xf numFmtId="44" fontId="35" fillId="7" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6685,21 +6759,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6720,16 +6779,22 @@
     <xf numFmtId="7" fontId="35" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="13" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="58" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -6739,9 +6804,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FF9966FF"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FF66FFFF"/>
       <color rgb="FFFF3300"/>
       <color rgb="FF00FF00"/>
@@ -12923,17 +12988,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -12964,17 +13029,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -13003,14 +13068,14 @@
       <c r="D4" s="23">
         <v>44201</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="537" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -15621,61 +15686,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="539" t="s">
+      <c r="H64" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="540"/>
+      <c r="I64" s="548"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="541">
+      <c r="K64" s="549">
         <f>I62+L62</f>
         <v>360753.85</v>
       </c>
-      <c r="L64" s="542"/>
-      <c r="M64" s="543">
+      <c r="L64" s="550"/>
+      <c r="M64" s="551">
         <f>M62+N62</f>
         <v>2886514.7</v>
       </c>
-      <c r="N64" s="544"/>
+      <c r="N64" s="552"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="551" t="s">
+      <c r="D65" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="551"/>
+      <c r="E65" s="559"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2365880.5699999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="552">
+      <c r="P65" s="560">
         <f>P62+Q62</f>
         <v>3321521.28</v>
       </c>
-      <c r="Q65" s="553"/>
+      <c r="Q65" s="561"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="554" t="s">
+      <c r="D66" s="562" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="554"/>
+      <c r="E66" s="562"/>
       <c r="F66" s="95">
         <v>-2276696.6800000002</v>
       </c>
-      <c r="I66" s="555" t="s">
+      <c r="I66" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="556"/>
-      <c r="K66" s="557">
+      <c r="J66" s="564"/>
+      <c r="K66" s="565">
         <f>F68+F69+F70</f>
         <v>344253.98999999964</v>
       </c>
-      <c r="L66" s="558"/>
+      <c r="L66" s="566"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -15709,11 +15774,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="559">
+      <c r="K68" s="567">
         <f>-C4</f>
         <v>-250864.68</v>
       </c>
-      <c r="L68" s="560"/>
+      <c r="L68" s="568"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -15737,22 +15802,22 @@
       <c r="C70" s="119">
         <v>44230</v>
       </c>
-      <c r="D70" s="545" t="s">
+      <c r="D70" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="546"/>
+      <c r="E70" s="554"/>
       <c r="F70" s="120">
         <v>209541.1</v>
       </c>
-      <c r="I70" s="547" t="s">
+      <c r="I70" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="548"/>
-      <c r="K70" s="549">
+      <c r="J70" s="556"/>
+      <c r="K70" s="557">
         <f>K66+K68</f>
         <v>93389.309999999648</v>
       </c>
-      <c r="L70" s="550"/>
+      <c r="L70" s="558"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -17297,20 +17362,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="574" t="s">
+      <c r="B1" s="582" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -17320,7 +17385,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="575"/>
+      <c r="B2" s="583"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -17339,27 +17404,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="587" t="s">
+      <c r="AB2" s="595" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="587"/>
-      <c r="AD2" s="587"/>
-      <c r="AE2" s="587"/>
-      <c r="AF2" s="587"/>
-      <c r="AG2" s="587"/>
+      <c r="AC2" s="595"/>
+      <c r="AD2" s="595"/>
+      <c r="AE2" s="595"/>
+      <c r="AF2" s="595"/>
+      <c r="AG2" s="595"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -17367,7 +17432,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="577" t="s">
+      <c r="P3" s="585" t="s">
         <v>562</v>
       </c>
       <c r="Q3" s="393"/>
@@ -17380,12 +17445,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="587"/>
-      <c r="AC3" s="587"/>
-      <c r="AD3" s="587"/>
-      <c r="AE3" s="587"/>
-      <c r="AF3" s="587"/>
-      <c r="AG3" s="587"/>
+      <c r="AB3" s="595"/>
+      <c r="AC3" s="595"/>
+      <c r="AD3" s="595"/>
+      <c r="AE3" s="595"/>
+      <c r="AF3" s="595"/>
+      <c r="AG3" s="595"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -17398,14 +17463,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="537" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -17416,7 +17481,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="577"/>
+      <c r="P4" s="585"/>
       <c r="Q4" s="393"/>
       <c r="R4" s="30"/>
       <c r="S4" s="31"/>
@@ -17431,16 +17496,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="588" t="s">
+      <c r="AB4" s="596" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="589"/>
+      <c r="AC4" s="597"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="590" t="s">
+      <c r="AE4" s="598" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="590"/>
-      <c r="AG4" s="590"/>
+      <c r="AF4" s="598"/>
+      <c r="AG4" s="598"/>
     </row>
     <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
@@ -18852,10 +18917,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="595" t="s">
+      <c r="AE23" s="603" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="596"/>
+      <c r="AF23" s="604"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -18999,11 +19064,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="597" t="s">
+      <c r="AE25" s="605" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="598"/>
-      <c r="AG25" s="601">
+      <c r="AF25" s="606"/>
+      <c r="AG25" s="609">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -19074,9 +19139,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="599"/>
-      <c r="AF26" s="600"/>
-      <c r="AG26" s="602"/>
+      <c r="AE26" s="607"/>
+      <c r="AF26" s="608"/>
+      <c r="AG26" s="610"/>
     </row>
     <row r="27" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
@@ -19251,10 +19316,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="591" t="s">
+      <c r="AB29" s="599" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="593">
+      <c r="AC29" s="601">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -19290,11 +19355,11 @@
         <v>0</v>
       </c>
       <c r="O30" s="7"/>
-      <c r="P30" s="578">
+      <c r="P30" s="586">
         <f>SUM(P5:P29)</f>
         <v>-163726</v>
       </c>
-      <c r="Q30" s="578"/>
+      <c r="Q30" s="586"/>
       <c r="R30" s="7">
         <v>0</v>
       </c>
@@ -19308,8 +19373,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="592"/>
-      <c r="AC30" s="594"/>
+      <c r="AB30" s="600"/>
+      <c r="AC30" s="602"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -20671,21 +20736,21 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="539" t="s">
+      <c r="H64" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="540"/>
+      <c r="I64" s="548"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="541">
+      <c r="K64" s="549">
         <f>I62+L62</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L64" s="542"/>
-      <c r="M64" s="543">
+      <c r="L64" s="550"/>
+      <c r="M64" s="551">
         <f>M62+N62</f>
         <v>2936130</v>
       </c>
-      <c r="N64" s="544"/>
+      <c r="N64" s="552"/>
       <c r="O64" s="367"/>
       <c r="P64" s="367"/>
       <c r="Q64" s="367"/>
@@ -20700,40 +20765,40 @@
       <c r="AG64" s="327"/>
     </row>
     <row r="65" spans="2:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="551" t="s">
+      <c r="D65" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="551"/>
+      <c r="E65" s="559"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2702101.7199999997</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="R65" s="552">
+      <c r="R65" s="560">
         <f>R62+S62</f>
         <v>3138957.44</v>
       </c>
-      <c r="S65" s="553"/>
+      <c r="S65" s="561"/>
       <c r="U65" s="50"/>
     </row>
     <row r="66" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="554" t="s">
+      <c r="D66" s="562" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="554"/>
+      <c r="E66" s="562"/>
       <c r="F66" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I66" s="555" t="s">
+      <c r="I66" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="556"/>
-      <c r="K66" s="557">
+      <c r="J66" s="564"/>
+      <c r="K66" s="565">
         <f>F68+F69+F70</f>
         <v>381077.48999999953</v>
       </c>
-      <c r="L66" s="558"/>
+      <c r="L66" s="566"/>
       <c r="R66" s="50"/>
       <c r="U66" s="107"/>
     </row>
@@ -20767,11 +20832,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="559">
+      <c r="K68" s="567">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L68" s="560"/>
+      <c r="L68" s="568"/>
       <c r="M68" s="116"/>
       <c r="R68" s="50"/>
       <c r="S68" s="7"/>
@@ -20795,22 +20860,22 @@
       <c r="C70" s="119">
         <v>44377</v>
       </c>
-      <c r="D70" s="545" t="s">
+      <c r="D70" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="546"/>
+      <c r="E70" s="554"/>
       <c r="F70" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I70" s="547" t="s">
+      <c r="I70" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="548"/>
-      <c r="K70" s="549">
+      <c r="J70" s="556"/>
+      <c r="K70" s="557">
         <f>K66+K68</f>
         <v>125313.09999999951</v>
       </c>
-      <c r="L70" s="550"/>
+      <c r="L70" s="558"/>
       <c r="R70" s="50"/>
       <c r="S70" s="7"/>
       <c r="U70" s="121"/>
@@ -20826,14 +20891,14 @@
       <c r="S71" s="7"/>
     </row>
     <row r="72" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I72" s="579" t="s">
+      <c r="I72" s="587" t="s">
         <v>610</v>
       </c>
-      <c r="J72" s="580"/>
-      <c r="K72" s="583">
+      <c r="J72" s="588"/>
+      <c r="K72" s="591">
         <v>163726</v>
       </c>
-      <c r="L72" s="584"/>
+      <c r="L72" s="592"/>
       <c r="R72" s="7"/>
       <c r="S72" s="7"/>
     </row>
@@ -20842,10 +20907,10 @@
       <c r="C73" s="128"/>
       <c r="D73" s="129"/>
       <c r="E73" s="7"/>
-      <c r="I73" s="581"/>
-      <c r="J73" s="582"/>
-      <c r="K73" s="585"/>
-      <c r="L73" s="586"/>
+      <c r="I73" s="589"/>
+      <c r="J73" s="590"/>
+      <c r="K73" s="593"/>
+      <c r="L73" s="594"/>
       <c r="M73" s="2"/>
       <c r="N73" s="60"/>
       <c r="O73" s="165"/>
@@ -20897,7 +20962,7 @@
       <c r="C76" s="130"/>
       <c r="E76" s="7"/>
       <c r="M76" s="4"/>
-      <c r="AC76" s="576"/>
+      <c r="AC76" s="584"/>
       <c r="AD76" s="342"/>
       <c r="AE76" s="342"/>
       <c r="AF76" s="342"/>
@@ -20910,7 +20975,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="273"/>
       <c r="M77" s="4"/>
-      <c r="AC77" s="576"/>
+      <c r="AC77" s="584"/>
       <c r="AD77" s="342"/>
       <c r="AE77" s="342"/>
       <c r="AF77" s="342"/>
@@ -22372,25 +22437,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="574" t="s">
+      <c r="B1" s="582" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="575"/>
+      <c r="B2" s="583"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -22400,27 +22465,27 @@
       <c r="L2" s="12"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="Q2" s="587" t="s">
+      <c r="Q2" s="595" t="s">
         <v>596</v>
       </c>
-      <c r="R2" s="587"/>
-      <c r="S2" s="587"/>
-      <c r="T2" s="587"/>
-      <c r="U2" s="587"/>
-      <c r="V2" s="587"/>
+      <c r="R2" s="595"/>
+      <c r="S2" s="595"/>
+      <c r="T2" s="595"/>
+      <c r="U2" s="595"/>
+      <c r="V2" s="595"/>
     </row>
     <row r="3" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -22428,12 +22493,12 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="Q3" s="587"/>
-      <c r="R3" s="587"/>
-      <c r="S3" s="587"/>
-      <c r="T3" s="587"/>
-      <c r="U3" s="587"/>
-      <c r="V3" s="587"/>
+      <c r="Q3" s="595"/>
+      <c r="R3" s="595"/>
+      <c r="S3" s="595"/>
+      <c r="T3" s="595"/>
+      <c r="U3" s="595"/>
+      <c r="V3" s="595"/>
     </row>
     <row r="4" spans="1:23" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -22446,14 +22511,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="537" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -22465,16 +22530,16 @@
       </c>
       <c r="O4" s="365"/>
       <c r="P4" s="29"/>
-      <c r="Q4" s="588" t="s">
+      <c r="Q4" s="596" t="s">
         <v>527</v>
       </c>
-      <c r="R4" s="589"/>
+      <c r="R4" s="597"/>
       <c r="S4" s="99"/>
-      <c r="T4" s="590" t="s">
+      <c r="T4" s="598" t="s">
         <v>567</v>
       </c>
-      <c r="U4" s="590"/>
-      <c r="V4" s="590"/>
+      <c r="U4" s="598"/>
+      <c r="V4" s="598"/>
       <c r="W4" s="99"/>
     </row>
     <row r="5" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23473,10 +23538,10 @@
         <v>0</v>
       </c>
       <c r="S23" s="99"/>
-      <c r="T23" s="595" t="s">
+      <c r="T23" s="603" t="s">
         <v>564</v>
       </c>
-      <c r="U23" s="596"/>
+      <c r="U23" s="604"/>
       <c r="V23" s="339">
         <f>SUM(V6:V22)</f>
         <v>2323600</v>
@@ -23580,11 +23645,11 @@
         <v>138607</v>
       </c>
       <c r="S25" s="99"/>
-      <c r="T25" s="597" t="s">
+      <c r="T25" s="605" t="s">
         <v>565</v>
       </c>
-      <c r="U25" s="598"/>
-      <c r="V25" s="601">
+      <c r="U25" s="606"/>
+      <c r="V25" s="609">
         <f>R29-V23</f>
         <v>163726</v>
       </c>
@@ -23633,9 +23698,9 @@
         <v>107480</v>
       </c>
       <c r="S26" s="99"/>
-      <c r="T26" s="599"/>
-      <c r="U26" s="600"/>
-      <c r="V26" s="602"/>
+      <c r="T26" s="607"/>
+      <c r="U26" s="608"/>
+      <c r="V26" s="610"/>
       <c r="W26" s="99"/>
     </row>
     <row r="27" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23758,10 +23823,10 @@
       </c>
       <c r="O29" s="7"/>
       <c r="P29" s="29"/>
-      <c r="Q29" s="591" t="s">
+      <c r="Q29" s="599" t="s">
         <v>562</v>
       </c>
-      <c r="R29" s="593">
+      <c r="R29" s="601">
         <f>SUM(R5:R28)</f>
         <v>2487326</v>
       </c>
@@ -23798,8 +23863,8 @@
       </c>
       <c r="O30" s="7"/>
       <c r="P30" s="373"/>
-      <c r="Q30" s="592"/>
-      <c r="R30" s="594"/>
+      <c r="Q30" s="600"/>
+      <c r="R30" s="602"/>
       <c r="S30" s="99"/>
       <c r="T30" s="99"/>
       <c r="U30" s="99"/>
@@ -24424,21 +24489,21 @@
       <c r="A50" s="60"/>
       <c r="B50" s="100"/>
       <c r="C50" s="4"/>
-      <c r="H50" s="539" t="s">
+      <c r="H50" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="540"/>
+      <c r="I50" s="548"/>
       <c r="J50" s="101"/>
-      <c r="K50" s="541">
+      <c r="K50" s="549">
         <f>I48+L48</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L50" s="542"/>
-      <c r="M50" s="543">
+      <c r="L50" s="550"/>
+      <c r="M50" s="551">
         <f>M48+N48</f>
         <v>612530</v>
       </c>
-      <c r="N50" s="544"/>
+      <c r="N50" s="552"/>
       <c r="O50" s="367"/>
       <c r="P50" s="102"/>
       <c r="Q50" s="320"/>
@@ -24450,10 +24515,10 @@
       <c r="W50" s="327"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D51" s="551" t="s">
+      <c r="D51" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="551"/>
+      <c r="E51" s="559"/>
       <c r="F51" s="103">
         <f>F48-K50-C48</f>
         <v>2702101.7199999997</v>
@@ -24462,22 +24527,22 @@
       <c r="J51" s="105"/>
     </row>
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D52" s="554" t="s">
+      <c r="D52" s="562" t="s">
         <v>502</v>
       </c>
-      <c r="E52" s="554"/>
+      <c r="E52" s="562"/>
       <c r="F52" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I52" s="555" t="s">
+      <c r="I52" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J52" s="556"/>
-      <c r="K52" s="557">
+      <c r="J52" s="564"/>
+      <c r="K52" s="565">
         <f>F54+F55+F56</f>
         <v>381077.72999999952</v>
       </c>
-      <c r="L52" s="558"/>
+      <c r="L52" s="566"/>
     </row>
     <row r="53" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="108"/>
@@ -24506,11 +24571,11 @@
         <v>21</v>
       </c>
       <c r="J54" s="115"/>
-      <c r="K54" s="559">
+      <c r="K54" s="567">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L54" s="560"/>
+      <c r="L54" s="568"/>
       <c r="M54" s="116"/>
     </row>
     <row r="55" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24528,22 +24593,22 @@
       <c r="C56" s="119">
         <v>44377</v>
       </c>
-      <c r="D56" s="545" t="s">
+      <c r="D56" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="546"/>
+      <c r="E56" s="554"/>
       <c r="F56" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I56" s="547" t="s">
+      <c r="I56" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J56" s="548"/>
-      <c r="K56" s="549">
+      <c r="J56" s="556"/>
+      <c r="K56" s="557">
         <f>K52+K54</f>
         <v>125313.3399999995</v>
       </c>
-      <c r="L56" s="550"/>
+      <c r="L56" s="558"/>
     </row>
     <row r="57" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C57" s="122"/>
@@ -24599,7 +24664,7 @@
       <c r="C62" s="130"/>
       <c r="E62" s="7"/>
       <c r="M62" s="4"/>
-      <c r="R62" s="576"/>
+      <c r="R62" s="584"/>
       <c r="S62" s="379"/>
       <c r="T62" s="379"/>
       <c r="U62" s="379"/>
@@ -24612,7 +24677,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="273"/>
       <c r="M63" s="4"/>
-      <c r="R63" s="576"/>
+      <c r="R63" s="584"/>
       <c r="S63" s="379"/>
       <c r="T63" s="379"/>
       <c r="U63" s="379"/>
@@ -24768,20 +24833,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="574" t="s">
+      <c r="B1" s="582" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -24791,7 +24856,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="575"/>
+      <c r="B2" s="583"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -24810,27 +24875,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="587" t="s">
+      <c r="AB2" s="595" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="587"/>
-      <c r="AD2" s="587"/>
-      <c r="AE2" s="587"/>
-      <c r="AF2" s="587"/>
-      <c r="AG2" s="587"/>
+      <c r="AC2" s="595"/>
+      <c r="AD2" s="595"/>
+      <c r="AE2" s="595"/>
+      <c r="AF2" s="595"/>
+      <c r="AG2" s="595"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -24838,13 +24903,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="625" t="s">
+      <c r="P3" s="633" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="627" t="s">
+      <c r="Q3" s="635" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="628"/>
+      <c r="S3" s="636"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -24854,12 +24919,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="587"/>
-      <c r="AC3" s="587"/>
-      <c r="AD3" s="587"/>
-      <c r="AE3" s="587"/>
-      <c r="AF3" s="587"/>
-      <c r="AG3" s="587"/>
+      <c r="AB3" s="595"/>
+      <c r="AC3" s="595"/>
+      <c r="AD3" s="595"/>
+      <c r="AE3" s="595"/>
+      <c r="AF3" s="595"/>
+      <c r="AG3" s="595"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -24872,14 +24937,14 @@
       <c r="D4" s="23">
         <v>44377</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="626" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="634" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -24890,10 +24955,10 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="625"/>
-      <c r="Q4" s="627"/>
+      <c r="P4" s="633"/>
+      <c r="Q4" s="635"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="628"/>
+      <c r="S4" s="636"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -24905,16 +24970,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="588" t="s">
+      <c r="AB4" s="596" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="589"/>
+      <c r="AC4" s="597"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="590" t="s">
+      <c r="AE4" s="598" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="590"/>
-      <c r="AG4" s="590"/>
+      <c r="AF4" s="598"/>
+      <c r="AG4" s="598"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -26351,10 +26416,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="595" t="s">
+      <c r="AE23" s="603" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="596"/>
+      <c r="AF23" s="604"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -26486,11 +26551,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="597" t="s">
+      <c r="AE25" s="605" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="598"/>
-      <c r="AG25" s="601">
+      <c r="AF25" s="606"/>
+      <c r="AG25" s="609">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -26559,9 +26624,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="599"/>
-      <c r="AF26" s="600"/>
-      <c r="AG26" s="602"/>
+      <c r="AE26" s="607"/>
+      <c r="AF26" s="608"/>
+      <c r="AG26" s="610"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -26760,10 +26825,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="591" t="s">
+      <c r="AB29" s="599" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="593">
+      <c r="AC29" s="601">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -26826,8 +26891,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="592"/>
-      <c r="AC30" s="594"/>
+      <c r="AB30" s="600"/>
+      <c r="AC30" s="602"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -27320,11 +27385,11 @@
       <c r="J39" s="233"/>
       <c r="K39" s="361"/>
       <c r="L39" s="357"/>
-      <c r="M39" s="620">
+      <c r="M39" s="628">
         <f>SUM(M5:M38)</f>
         <v>3989472.22</v>
       </c>
-      <c r="N39" s="622">
+      <c r="N39" s="630">
         <f>SUM(N5:N38)</f>
         <v>689220.5</v>
       </c>
@@ -27373,8 +27438,8 @@
         <f>1145.91+398.99+423.94+498.99+398.99</f>
         <v>2866.8199999999997</v>
       </c>
-      <c r="M40" s="621"/>
-      <c r="N40" s="623"/>
+      <c r="M40" s="629"/>
+      <c r="N40" s="631"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -27567,10 +27632,10 @@
       <c r="L44" s="358">
         <v>73526</v>
       </c>
-      <c r="M44" s="624" t="s">
+      <c r="M44" s="632" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="624"/>
+      <c r="N44" s="632"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -28158,7 +28223,7 @@
       <c r="L57" s="458">
         <v>7482</v>
       </c>
-      <c r="M57" s="612">
+      <c r="M57" s="620">
         <f>SUM(M45:M56)</f>
         <v>3606750</v>
       </c>
@@ -28198,7 +28263,7 @@
       <c r="L58" s="458">
         <v>986</v>
       </c>
-      <c r="M58" s="613"/>
+      <c r="M58" s="621"/>
       <c r="N58" s="475"/>
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
@@ -28273,10 +28338,10 @@
         <f>1033.33+165.33</f>
         <v>1198.6599999999999</v>
       </c>
-      <c r="M60" s="614" t="s">
+      <c r="M60" s="622" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="615"/>
+      <c r="N60" s="623"/>
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -28349,11 +28414,11 @@
       <c r="L62" s="458">
         <v>22595.71</v>
       </c>
-      <c r="M62" s="616">
+      <c r="M62" s="624">
         <f>M57-M39</f>
         <v>-382722.2200000002</v>
       </c>
-      <c r="N62" s="617"/>
+      <c r="N62" s="625"/>
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -28389,8 +28454,8 @@
       <c r="L63" s="458">
         <v>1064</v>
       </c>
-      <c r="M63" s="618"/>
-      <c r="N63" s="619"/>
+      <c r="M63" s="626"/>
+      <c r="N63" s="627"/>
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -28580,16 +28645,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="539" t="s">
+      <c r="H69" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="540"/>
+      <c r="I69" s="548"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="541">
+      <c r="K69" s="549">
         <f>I67+L67</f>
         <v>587206.12</v>
       </c>
-      <c r="L69" s="542"/>
+      <c r="L69" s="550"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="367"/>
@@ -28606,40 +28671,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="551" t="s">
+      <c r="D70" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="551"/>
+      <c r="E70" s="559"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>3436910.52</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="552">
+      <c r="R70" s="560">
         <f>R67+S67</f>
         <v>10503773.959999999</v>
       </c>
-      <c r="S70" s="553"/>
+      <c r="S70" s="561"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="554" t="s">
+      <c r="D71" s="562" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="554"/>
+      <c r="E71" s="562"/>
       <c r="F71" s="95">
         <v>-3290264.27</v>
       </c>
-      <c r="I71" s="555" t="s">
+      <c r="I71" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="556"/>
-      <c r="K71" s="557">
+      <c r="J71" s="564"/>
+      <c r="K71" s="565">
         <f>F73+F74+F75</f>
         <v>426565.1</v>
       </c>
-      <c r="L71" s="558"/>
+      <c r="L71" s="566"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -28673,11 +28738,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="559">
+      <c r="K73" s="567">
         <f>-C4</f>
         <v>-308642.71999999997</v>
       </c>
-      <c r="L73" s="603"/>
+      <c r="L73" s="611"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -28700,22 +28765,22 @@
       <c r="C75" s="119">
         <v>44410</v>
       </c>
-      <c r="D75" s="545" t="s">
+      <c r="D75" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="546"/>
+      <c r="E75" s="554"/>
       <c r="F75" s="120">
         <v>250140.85</v>
       </c>
-      <c r="I75" s="547" t="s">
+      <c r="I75" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="548"/>
-      <c r="K75" s="549">
+      <c r="J75" s="556"/>
+      <c r="K75" s="557">
         <f>K71+K73</f>
         <v>117922.38</v>
       </c>
-      <c r="L75" s="549"/>
+      <c r="L75" s="557"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -28730,14 +28795,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="604" t="s">
+      <c r="I77" s="612" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="605"/>
-      <c r="K77" s="608">
+      <c r="J77" s="613"/>
+      <c r="K77" s="616">
         <v>-383122.22</v>
       </c>
-      <c r="L77" s="609"/>
+      <c r="L77" s="617"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -28746,10 +28811,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="606"/>
-      <c r="J78" s="607"/>
-      <c r="K78" s="610"/>
-      <c r="L78" s="611"/>
+      <c r="I78" s="614"/>
+      <c r="J78" s="615"/>
+      <c r="K78" s="618"/>
+      <c r="L78" s="619"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="165"/>
@@ -28801,7 +28866,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="576"/>
+      <c r="AC81" s="584"/>
       <c r="AD81" s="440"/>
       <c r="AE81" s="440"/>
       <c r="AF81" s="440"/>
@@ -28814,7 +28879,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="576"/>
+      <c r="AC82" s="584"/>
       <c r="AD82" s="440"/>
       <c r="AE82" s="440"/>
       <c r="AF82" s="440"/>
@@ -30591,8 +30656,8 @@
   </sheetPr>
   <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -30627,20 +30692,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="574" t="s">
+      <c r="B1" s="582" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>721</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -30650,7 +30715,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="575"/>
+      <c r="B2" s="583"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -30669,27 +30734,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="587" t="s">
+      <c r="AB2" s="595" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="587"/>
-      <c r="AD2" s="587"/>
-      <c r="AE2" s="587"/>
-      <c r="AF2" s="587"/>
-      <c r="AG2" s="587"/>
+      <c r="AC2" s="595"/>
+      <c r="AD2" s="595"/>
+      <c r="AE2" s="595"/>
+      <c r="AF2" s="595"/>
+      <c r="AG2" s="595"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -30700,13 +30765,13 @@
       <c r="O3" s="366" t="s">
         <v>753</v>
       </c>
-      <c r="P3" s="625" t="s">
+      <c r="P3" s="633" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="627" t="s">
+      <c r="Q3" s="635" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="628"/>
+      <c r="S3" s="636"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -30716,12 +30781,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="587"/>
-      <c r="AC3" s="587"/>
-      <c r="AD3" s="587"/>
-      <c r="AE3" s="587"/>
-      <c r="AF3" s="587"/>
-      <c r="AG3" s="587"/>
+      <c r="AB3" s="595"/>
+      <c r="AC3" s="595"/>
+      <c r="AD3" s="595"/>
+      <c r="AE3" s="595"/>
+      <c r="AF3" s="595"/>
+      <c r="AG3" s="595"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -30734,14 +30799,14 @@
       <c r="D4" s="23">
         <v>44411</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="626" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="634" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -30752,10 +30817,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="625"/>
-      <c r="Q4" s="627"/>
+      <c r="P4" s="633"/>
+      <c r="Q4" s="635"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="628"/>
+      <c r="S4" s="636"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -30767,16 +30832,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="588" t="s">
+      <c r="AB4" s="596" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="589"/>
+      <c r="AC4" s="597"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="590" t="s">
+      <c r="AE4" s="598" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="590"/>
-      <c r="AG4" s="590"/>
+      <c r="AF4" s="598"/>
+      <c r="AG4" s="598"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -32264,10 +32329,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="595" t="s">
+      <c r="AE23" s="603" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="596"/>
+      <c r="AF23" s="604"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -32407,11 +32472,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="597" t="s">
+      <c r="AE25" s="605" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="598"/>
-      <c r="AG25" s="601">
+      <c r="AF25" s="606"/>
+      <c r="AG25" s="609">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -32483,9 +32548,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="599"/>
-      <c r="AF26" s="600"/>
-      <c r="AG26" s="602"/>
+      <c r="AE26" s="607"/>
+      <c r="AF26" s="608"/>
+      <c r="AG26" s="610"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -32695,10 +32760,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="591" t="s">
+      <c r="AB29" s="599" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="593">
+      <c r="AC29" s="601">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -32763,8 +32828,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="592"/>
-      <c r="AC30" s="594"/>
+      <c r="AB30" s="600"/>
+      <c r="AC30" s="602"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -33277,11 +33342,11 @@
       <c r="L39" s="357">
         <v>11500</v>
       </c>
-      <c r="M39" s="620">
+      <c r="M39" s="537">
         <f>SUM(M5:M38)</f>
         <v>2842451</v>
       </c>
-      <c r="N39" s="622">
+      <c r="N39" s="630">
         <f>SUM(N5:N38)</f>
         <v>271503</v>
       </c>
@@ -33332,8 +33397,8 @@
       <c r="L40" s="357">
         <v>20880</v>
       </c>
-      <c r="M40" s="621"/>
-      <c r="N40" s="623"/>
+      <c r="M40" s="538"/>
+      <c r="N40" s="631"/>
       <c r="O40" s="392"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -33527,10 +33592,10 @@
       <c r="L44" s="358">
         <v>986</v>
       </c>
-      <c r="M44" s="624" t="s">
+      <c r="M44" s="632" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="624"/>
+      <c r="N44" s="632"/>
       <c r="O44" s="392"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -34104,8 +34169,8 @@
         <f>968.75+155</f>
         <v>1123.75</v>
       </c>
-      <c r="M58" s="637">
-        <f ca="1">SUM(M45:M58)</f>
+      <c r="M58" s="535">
+        <f>SUM(M45:M57)</f>
         <v>2805120</v>
       </c>
       <c r="N58" s="475"/>
@@ -34142,7 +34207,7 @@
       <c r="L59" s="458">
         <v>1480.06</v>
       </c>
-      <c r="M59" s="638"/>
+      <c r="M59" s="536"/>
       <c r="N59" s="42"/>
       <c r="O59" s="392"/>
       <c r="P59" s="7"/>
@@ -34177,10 +34242,10 @@
       <c r="L60" s="458">
         <v>2479.5</v>
       </c>
-      <c r="M60" s="614" t="s">
+      <c r="M60" s="622" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="615"/>
+      <c r="N60" s="623"/>
       <c r="O60" s="392"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -34247,11 +34312,11 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="633">
-        <f ca="1">M58-M39</f>
-        <v>-37331</v>
-      </c>
-      <c r="N62" s="634"/>
+      <c r="M62" s="641">
+        <f>M39-M58</f>
+        <v>37331</v>
+      </c>
+      <c r="N62" s="642"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -34283,8 +34348,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="635"/>
-      <c r="N63" s="636"/>
+      <c r="M63" s="643"/>
+      <c r="N63" s="644"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -34316,10 +34381,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="641">
+      <c r="M64" s="647">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="642"/>
+      <c r="N64" s="648"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -34350,10 +34415,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="643">
+      <c r="M65" s="649">
         <v>-163726</v>
       </c>
-      <c r="N65" s="644"/>
+      <c r="N65" s="650"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -34384,12 +34449,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="645">
-        <f ca="1">SUM(M65+M64+M62)</f>
-        <v>-583779.22</v>
-      </c>
-      <c r="N66" s="646"/>
-      <c r="O66" s="639" t="s">
+      <c r="M66" s="651">
+        <f>SUM(M65+M64+M62)</f>
+        <v>-509117.22</v>
+      </c>
+      <c r="N66" s="652"/>
+      <c r="O66" s="645" t="s">
         <v>821</v>
       </c>
       <c r="P66" s="7"/>
@@ -34443,9 +34508,9 @@
         <f>SUM(L5:L66)</f>
         <v>482695.31000000006</v>
       </c>
-      <c r="M67" s="647"/>
-      <c r="N67" s="648"/>
-      <c r="O67" s="640"/>
+      <c r="M67" s="653"/>
+      <c r="N67" s="654"/>
+      <c r="O67" s="646"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
@@ -34477,16 +34542,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="539" t="s">
+      <c r="H69" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="540"/>
+      <c r="I69" s="548"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="541">
+      <c r="K69" s="549">
         <f>I67+L67</f>
         <v>518841.31000000006</v>
       </c>
-      <c r="L69" s="542"/>
+      <c r="L69" s="550"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="489"/>
@@ -34503,40 +34568,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="551" t="s">
+      <c r="D70" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="551"/>
+      <c r="E70" s="559"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>2539226.3499999996</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="552">
+      <c r="R70" s="560">
         <f>R67+S67</f>
         <v>7378939.6599999992</v>
       </c>
-      <c r="S70" s="553"/>
+      <c r="S70" s="561"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="554" t="s">
+      <c r="D71" s="562" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="554"/>
+      <c r="E71" s="562"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="555" t="s">
+      <c r="I71" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="556"/>
-      <c r="K71" s="557">
+      <c r="J71" s="564"/>
+      <c r="K71" s="565">
         <f>F73+F74+F75</f>
         <v>536310.85999999964</v>
       </c>
-      <c r="L71" s="558"/>
+      <c r="L71" s="566"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -34570,11 +34635,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="559">
+      <c r="K73" s="567">
         <f>-C4</f>
         <v>-250140.85</v>
       </c>
-      <c r="L73" s="603"/>
+      <c r="L73" s="611"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -34597,22 +34662,22 @@
       <c r="C75" s="119">
         <v>44439</v>
       </c>
-      <c r="D75" s="545" t="s">
+      <c r="D75" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="546"/>
+      <c r="E75" s="554"/>
       <c r="F75" s="120">
         <v>365611.59</v>
       </c>
-      <c r="I75" s="547" t="s">
+      <c r="I75" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="548"/>
-      <c r="K75" s="549">
+      <c r="J75" s="556"/>
+      <c r="K75" s="557">
         <f>K71+K73</f>
         <v>286170.00999999966</v>
       </c>
-      <c r="L75" s="549"/>
+      <c r="L75" s="557"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -34627,14 +34692,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="629" t="s">
+      <c r="I77" s="637" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="630"/>
-      <c r="K77" s="633">
+      <c r="J77" s="638"/>
+      <c r="K77" s="641">
         <v>37331</v>
       </c>
-      <c r="L77" s="634"/>
+      <c r="L77" s="642"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -34643,10 +34708,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="631"/>
-      <c r="J78" s="632"/>
-      <c r="K78" s="635"/>
-      <c r="L78" s="636"/>
+      <c r="I78" s="639"/>
+      <c r="J78" s="640"/>
+      <c r="K78" s="643"/>
+      <c r="L78" s="644"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -34698,7 +34763,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="576"/>
+      <c r="AC81" s="584"/>
       <c r="AD81" s="486"/>
       <c r="AE81" s="486"/>
       <c r="AF81" s="486"/>
@@ -34711,7 +34776,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="576"/>
+      <c r="AC82" s="584"/>
       <c r="AD82" s="486"/>
       <c r="AE82" s="486"/>
       <c r="AF82" s="486"/>
@@ -34807,7 +34872,7 @@
   <sortState ref="M45:N55">
     <sortCondition ref="N45:N55"/>
   </sortState>
-  <mergeCells count="41">
+  <mergeCells count="39">
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
@@ -34824,11 +34889,9 @@
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="M39:M40"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="R70:S70"/>
-    <mergeCell ref="M58:M59"/>
     <mergeCell ref="O66:O67"/>
     <mergeCell ref="M62:N63"/>
     <mergeCell ref="M60:N60"/>
@@ -36388,8 +36451,8 @@
   </sheetPr>
   <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36424,20 +36487,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="574" t="s">
+      <c r="B1" s="582" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>836</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -36447,7 +36510,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="575"/>
+      <c r="B2" s="583"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -36466,27 +36529,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="587" t="s">
+      <c r="AB2" s="595" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="587"/>
-      <c r="AD2" s="587"/>
-      <c r="AE2" s="587"/>
-      <c r="AF2" s="587"/>
-      <c r="AG2" s="587"/>
+      <c r="AC2" s="595"/>
+      <c r="AD2" s="595"/>
+      <c r="AE2" s="595"/>
+      <c r="AF2" s="595"/>
+      <c r="AG2" s="595"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -36494,13 +36557,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="625" t="s">
+      <c r="P3" s="633" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="627" t="s">
+      <c r="Q3" s="635" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="628" t="s">
+      <c r="S3" s="636" t="s">
         <v>868</v>
       </c>
       <c r="W3" s="213" t="s">
@@ -36512,12 +36575,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="587"/>
-      <c r="AC3" s="587"/>
-      <c r="AD3" s="587"/>
-      <c r="AE3" s="587"/>
-      <c r="AF3" s="587"/>
-      <c r="AG3" s="587"/>
+      <c r="AB3" s="595"/>
+      <c r="AC3" s="595"/>
+      <c r="AD3" s="595"/>
+      <c r="AE3" s="595"/>
+      <c r="AF3" s="595"/>
+      <c r="AG3" s="595"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -36530,14 +36593,14 @@
       <c r="D4" s="23">
         <v>44439</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="626" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="634" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -36548,10 +36611,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="625"/>
-      <c r="Q4" s="627"/>
+      <c r="P4" s="633"/>
+      <c r="Q4" s="635"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="628"/>
+      <c r="S4" s="636"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -36563,16 +36626,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="588" t="s">
+      <c r="AB4" s="596" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="589"/>
+      <c r="AC4" s="597"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="590" t="s">
+      <c r="AE4" s="598" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="590"/>
-      <c r="AG4" s="590"/>
+      <c r="AF4" s="598"/>
+      <c r="AG4" s="598"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -36988,7 +37051,7 @@
       <c r="J10" s="52">
         <v>44445</v>
       </c>
-      <c r="K10" s="663" t="s">
+      <c r="K10" s="531" t="s">
         <v>876</v>
       </c>
       <c r="L10" s="53">
@@ -37070,7 +37133,7 @@
       <c r="J11" s="292">
         <v>44446</v>
       </c>
-      <c r="K11" s="665" t="s">
+      <c r="K11" s="533" t="s">
         <v>878</v>
       </c>
       <c r="L11" s="46">
@@ -37150,7 +37213,7 @@
         <v>4495</v>
       </c>
       <c r="J12" s="52"/>
-      <c r="K12" s="664"/>
+      <c r="K12" s="532"/>
       <c r="L12" s="46"/>
       <c r="M12" s="444">
         <v>124239</v>
@@ -37392,7 +37455,7 @@
       <c r="K15" s="158" t="s">
         <v>884</v>
       </c>
-      <c r="L15" s="666">
+      <c r="L15" s="534">
         <f>23427+400</f>
         <v>23827</v>
       </c>
@@ -37446,25 +37509,33 @@
       <c r="B16" s="134">
         <v>44451</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="139"/>
+      <c r="C16" s="36">
+        <v>29731</v>
+      </c>
+      <c r="D16" s="139" t="s">
+        <v>886</v>
+      </c>
       <c r="E16" s="136">
         <v>44451</v>
       </c>
-      <c r="F16" s="37"/>
+      <c r="F16" s="37">
+        <v>143478</v>
+      </c>
       <c r="G16" s="137"/>
       <c r="H16" s="138">
         <v>44451</v>
       </c>
-      <c r="I16" s="38"/>
+      <c r="I16" s="38">
+        <v>700</v>
+      </c>
       <c r="J16" s="52"/>
       <c r="K16" s="158"/>
       <c r="L16" s="6"/>
       <c r="M16" s="444">
-        <v>0</v>
+        <v>105634</v>
       </c>
       <c r="N16" s="334">
-        <v>0</v>
+        <v>7413</v>
       </c>
       <c r="O16" s="491"/>
       <c r="P16" s="389">
@@ -37475,7 +37546,7 @@
       </c>
       <c r="R16" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>143478</v>
       </c>
       <c r="S16" s="6">
         <f t="shared" si="0"/>
@@ -37513,25 +37584,33 @@
       <c r="B17" s="134">
         <v>44452</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="141"/>
+      <c r="C17" s="36">
+        <v>8641</v>
+      </c>
+      <c r="D17" s="141" t="s">
+        <v>804</v>
+      </c>
       <c r="E17" s="136">
         <v>44452</v>
       </c>
-      <c r="F17" s="37"/>
+      <c r="F17" s="37">
+        <v>138908</v>
+      </c>
       <c r="G17" s="137"/>
       <c r="H17" s="138">
         <v>44452</v>
       </c>
-      <c r="I17" s="38"/>
+      <c r="I17" s="38">
+        <v>7440</v>
+      </c>
       <c r="J17" s="52"/>
       <c r="K17" s="158"/>
       <c r="L17" s="53"/>
       <c r="M17" s="444">
-        <v>0</v>
+        <v>114973</v>
       </c>
       <c r="N17" s="334">
-        <v>0</v>
+        <v>7854</v>
       </c>
       <c r="O17" s="491"/>
       <c r="P17" s="389">
@@ -37542,13 +37621,15 @@
       </c>
       <c r="R17" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>138908</v>
       </c>
       <c r="S17" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T17" s="48"/>
+      <c r="T17" s="48" t="s">
+        <v>887</v>
+      </c>
       <c r="W17" s="213" t="s">
         <v>68</v>
       </c>
@@ -37580,25 +37661,34 @@
       <c r="B18" s="134">
         <v>44453</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="139"/>
+      <c r="C18" s="36">
+        <v>2167.5</v>
+      </c>
+      <c r="D18" s="139" t="s">
+        <v>888</v>
+      </c>
       <c r="E18" s="136">
         <v>44453</v>
       </c>
-      <c r="F18" s="37"/>
+      <c r="F18" s="37">
+        <v>194262</v>
+      </c>
       <c r="G18" s="137"/>
       <c r="H18" s="138">
         <v>44453</v>
       </c>
-      <c r="I18" s="38"/>
+      <c r="I18" s="38">
+        <v>660</v>
+      </c>
       <c r="J18" s="52"/>
       <c r="K18" s="452"/>
       <c r="L18" s="46"/>
       <c r="M18" s="444">
-        <v>0</v>
-      </c>
-      <c r="N18" s="334">
-        <v>0</v>
+        <v>166499.5</v>
+      </c>
+      <c r="N18" s="456">
+        <f>24860+75</f>
+        <v>24935</v>
       </c>
       <c r="O18" s="491"/>
       <c r="P18" s="389">
@@ -37609,11 +37699,10 @@
       </c>
       <c r="R18" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S18" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>194262</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>889</v>
       </c>
       <c r="T18" s="48"/>
       <c r="W18" s="213" t="s">
@@ -37959,10 +38048,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="595" t="s">
+      <c r="AE23" s="603" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="596"/>
+      <c r="AF23" s="604"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -38082,11 +38171,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="597" t="s">
+      <c r="AE25" s="605" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="598"/>
-      <c r="AG25" s="601">
+      <c r="AF25" s="606"/>
+      <c r="AG25" s="609">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -38148,9 +38237,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="599"/>
-      <c r="AF26" s="600"/>
-      <c r="AG26" s="602"/>
+      <c r="AE26" s="607"/>
+      <c r="AF26" s="608"/>
+      <c r="AG26" s="610"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -38316,10 +38405,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="591" t="s">
+      <c r="AB29" s="599" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="593">
+      <c r="AC29" s="601">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -38374,8 +38463,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="592"/>
-      <c r="AC30" s="594"/>
+      <c r="AB30" s="600"/>
+      <c r="AC30" s="602"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -38808,20 +38897,20 @@
       <c r="J39" s="299"/>
       <c r="K39" s="246"/>
       <c r="L39" s="46"/>
-      <c r="M39" s="620">
+      <c r="M39" s="628">
         <f>SUM(M5:M38)</f>
-        <v>1062599</v>
-      </c>
-      <c r="N39" s="622">
+        <v>1449705.5</v>
+      </c>
+      <c r="N39" s="630">
         <f>SUM(N5:N38)</f>
-        <v>92447</v>
+        <v>132649</v>
       </c>
       <c r="O39" s="392"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <f>SUM(R5:R38)</f>
-        <v>1375197.92</v>
+        <v>1851845.92</v>
       </c>
       <c r="T39" s="48"/>
       <c r="W39" s="213" t="s">
@@ -38851,8 +38940,8 @@
       <c r="J40" s="299"/>
       <c r="K40" s="172"/>
       <c r="L40" s="46"/>
-      <c r="M40" s="621"/>
-      <c r="N40" s="623"/>
+      <c r="M40" s="629"/>
+      <c r="N40" s="631"/>
       <c r="O40" s="392"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -38996,10 +39085,10 @@
       <c r="J44" s="299"/>
       <c r="K44" s="528"/>
       <c r="L44" s="71"/>
-      <c r="M44" s="624" t="s">
+      <c r="M44" s="632" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="624"/>
+      <c r="N44" s="632"/>
       <c r="O44" s="392"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -39465,7 +39554,7 @@
       <c r="J58" s="529"/>
       <c r="K58" s="468"/>
       <c r="L58" s="50"/>
-      <c r="M58" s="637">
+      <c r="M58" s="655">
         <f t="shared" ref="M58" si="2">SUM(M45:M57)</f>
         <v>0</v>
       </c>
@@ -39499,7 +39588,7 @@
       <c r="J59" s="529"/>
       <c r="K59" s="243"/>
       <c r="L59" s="50"/>
-      <c r="M59" s="638"/>
+      <c r="M59" s="656"/>
       <c r="N59" s="42"/>
       <c r="O59" s="392"/>
       <c r="P59" s="7"/>
@@ -39530,10 +39619,10 @@
       <c r="J60" s="529"/>
       <c r="K60" s="468"/>
       <c r="L60" s="50"/>
-      <c r="M60" s="614" t="s">
+      <c r="M60" s="622" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="615"/>
+      <c r="N60" s="623"/>
       <c r="O60" s="392"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -39594,10 +39683,10 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="633">
+      <c r="M62" s="641">
         <v>-37331</v>
       </c>
-      <c r="N62" s="634"/>
+      <c r="N62" s="642"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -39629,8 +39718,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="635"/>
-      <c r="N63" s="636"/>
+      <c r="M63" s="643"/>
+      <c r="N63" s="644"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -39662,10 +39751,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="641">
+      <c r="M64" s="647">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="642"/>
+      <c r="N64" s="648"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -39696,10 +39785,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="643">
+      <c r="M65" s="649">
         <v>-163726</v>
       </c>
-      <c r="N65" s="644"/>
+      <c r="N65" s="650"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -39730,12 +39819,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="645">
+      <c r="M66" s="651">
         <f>SUM(M65+M64+M62)</f>
         <v>-583779.22</v>
       </c>
-      <c r="N66" s="646"/>
-      <c r="O66" s="639"/>
+      <c r="N66" s="652"/>
+      <c r="O66" s="645"/>
       <c r="P66" s="7"/>
       <c r="Q66" s="7"/>
       <c r="R66" s="84">
@@ -39761,7 +39850,7 @@
       </c>
       <c r="C67" s="86">
         <f>SUM(C5:C66)</f>
-        <v>106742.79000000001</v>
+        <v>147282.29</v>
       </c>
       <c r="D67" s="87"/>
       <c r="E67" s="88" t="s">
@@ -39769,7 +39858,7 @@
       </c>
       <c r="F67" s="89">
         <f>SUM(F5:F66)</f>
-        <v>1358033</v>
+        <v>1834681</v>
       </c>
       <c r="G67" s="87"/>
       <c r="H67" s="90" t="s">
@@ -39777,7 +39866,7 @@
       </c>
       <c r="I67" s="91">
         <f>SUM(I5:I66)</f>
-        <v>14748</v>
+        <v>23548</v>
       </c>
       <c r="J67" s="92"/>
       <c r="K67" s="93" t="s">
@@ -39787,14 +39876,14 @@
         <f>SUM(L5:L66)</f>
         <v>98661.13</v>
       </c>
-      <c r="M67" s="647"/>
-      <c r="N67" s="648"/>
-      <c r="O67" s="640"/>
+      <c r="M67" s="653"/>
+      <c r="N67" s="654"/>
+      <c r="O67" s="646"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
         <f>SUM(R5:R66)</f>
-        <v>2750395.84</v>
+        <v>3703691.84</v>
       </c>
       <c r="S67" s="7">
         <f>SUM(S5:S66)</f>
@@ -39821,16 +39910,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="539" t="s">
+      <c r="H69" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="540"/>
+      <c r="I69" s="548"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="541">
+      <c r="K69" s="549">
         <f>I67+L67</f>
-        <v>113409.13</v>
-      </c>
-      <c r="L69" s="542"/>
+        <v>122209.13</v>
+      </c>
+      <c r="L69" s="550"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="489"/>
@@ -39847,40 +39936,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="551" t="s">
+      <c r="D70" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="551"/>
+      <c r="E70" s="559"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
-        <v>1137881.08</v>
+        <v>1565189.58</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="552">
+      <c r="R70" s="560">
         <f>R67+S67</f>
-        <v>2767560.76</v>
-      </c>
-      <c r="S70" s="553"/>
+        <v>3720856.76</v>
+      </c>
+      <c r="S70" s="561"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="554" t="s">
+      <c r="D71" s="562" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="554"/>
+      <c r="E71" s="562"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="555" t="s">
+      <c r="I71" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="556"/>
-      <c r="K71" s="557">
+      <c r="J71" s="564"/>
+      <c r="K71" s="565">
         <f>F73+F74+F75</f>
-        <v>-1242832</v>
-      </c>
-      <c r="L71" s="558"/>
+        <v>-815523.5</v>
+      </c>
+      <c r="L71" s="566"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -39907,18 +39996,18 @@
       </c>
       <c r="F73" s="95">
         <f>SUM(F70:F72)</f>
-        <v>-1242832</v>
+        <v>-815523.5</v>
       </c>
       <c r="H73" s="34"/>
       <c r="I73" s="114" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="559">
+      <c r="K73" s="567">
         <f>-C4</f>
         <v>-365611.59</v>
       </c>
-      <c r="L73" s="603"/>
+      <c r="L73" s="611"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -39939,22 +40028,22 @@
     </row>
     <row r="75" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="119"/>
-      <c r="D75" s="545" t="s">
+      <c r="D75" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="546"/>
+      <c r="E75" s="554"/>
       <c r="F75" s="120">
         <v>0</v>
       </c>
-      <c r="I75" s="547" t="s">
+      <c r="I75" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="548"/>
-      <c r="K75" s="549">
+      <c r="J75" s="556"/>
+      <c r="K75" s="557">
         <f>K71+K73</f>
-        <v>-1608443.59</v>
-      </c>
-      <c r="L75" s="549"/>
+        <v>-1181135.0900000001</v>
+      </c>
+      <c r="L75" s="557"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -39969,14 +40058,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="629" t="s">
+      <c r="I77" s="637" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="630"/>
-      <c r="K77" s="633">
-        <v>0</v>
-      </c>
-      <c r="L77" s="634"/>
+      <c r="J77" s="638"/>
+      <c r="K77" s="641">
+        <v>0</v>
+      </c>
+      <c r="L77" s="642"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -39985,10 +40074,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="631"/>
-      <c r="J78" s="632"/>
-      <c r="K78" s="635"/>
-      <c r="L78" s="636"/>
+      <c r="I78" s="639"/>
+      <c r="J78" s="640"/>
+      <c r="K78" s="643"/>
+      <c r="L78" s="644"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -40040,7 +40129,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="576"/>
+      <c r="AC81" s="584"/>
       <c r="AD81" s="526"/>
       <c r="AE81" s="526"/>
       <c r="AF81" s="526"/>
@@ -40053,7 +40142,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="576"/>
+      <c r="AC82" s="584"/>
       <c r="AD82" s="526"/>
       <c r="AE82" s="526"/>
       <c r="AF82" s="526"/>
@@ -42730,10 +42819,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A43:G60"/>
+  <dimension ref="A37:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42741,45 +42830,152 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="649" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="32"/>
+      <c r="B39" s="657" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="650"/>
-      <c r="D44" s="650"/>
-      <c r="E44" s="651"/>
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="658"/>
+      <c r="D39" s="658"/>
+      <c r="E39" s="659"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="19">
+        <v>44454</v>
+      </c>
+      <c r="B40" s="196" t="s">
+        <v>890</v>
+      </c>
+      <c r="C40" s="197">
+        <v>267.95</v>
+      </c>
+      <c r="D40" s="198" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F40" s="671" t="s">
+        <v>891</v>
+      </c>
+      <c r="G40" s="530"/>
+    </row>
+    <row r="41" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="19">
+        <v>44454</v>
+      </c>
+      <c r="B41" s="196" t="s">
+        <v>892</v>
+      </c>
+      <c r="C41" s="197">
+        <v>322.33999999999997</v>
+      </c>
+      <c r="D41" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F41" s="671" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="19">
+        <v>44454</v>
+      </c>
+      <c r="B42" s="196" t="s">
+        <v>893</v>
+      </c>
+      <c r="C42" s="197">
+        <v>48</v>
+      </c>
+      <c r="D42" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="199" t="s">
+        <v>894</v>
+      </c>
+      <c r="F42" s="72">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="19">
+        <v>44454</v>
+      </c>
+      <c r="B43" s="196" t="s">
+        <v>895</v>
+      </c>
+      <c r="C43" s="197">
+        <v>338.89</v>
+      </c>
+      <c r="D43" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="199" t="s">
+        <v>896</v>
+      </c>
+      <c r="F43" s="72">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="19">
+        <v>44454</v>
+      </c>
+      <c r="B44" s="196" t="s">
+        <v>897</v>
+      </c>
+      <c r="C44" s="197">
+        <v>162.77000000000001</v>
+      </c>
+      <c r="D44" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F44" s="671" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
-        <v>44451</v>
+        <v>44454</v>
       </c>
       <c r="B45" s="196" t="s">
-        <v>886</v>
+        <v>898</v>
       </c>
       <c r="C45" s="197">
-        <v>162.4</v>
-      </c>
-      <c r="D45" s="198" t="s">
+        <v>188.42</v>
+      </c>
+      <c r="D45" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E45" s="199" t="s">
-        <v>887</v>
+        <v>899</v>
       </c>
       <c r="F45" s="72">
-        <v>81</v>
-      </c>
-      <c r="G45" s="530"/>
-    </row>
-    <row r="46" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19">
+        <v>44454</v>
+      </c>
       <c r="B46" s="196" t="s">
-        <v>885</v>
+        <v>900</v>
       </c>
       <c r="C46" s="197">
-        <v>0</v>
+        <v>154.36000000000001</v>
       </c>
       <c r="D46" s="200" t="s">
         <v>33</v>
@@ -42787,47 +42983,51 @@
       <c r="E46" s="199" t="s">
         <v>611</v>
       </c>
-      <c r="F46" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="F46" s="671" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="330">
+        <v>44454</v>
+      </c>
       <c r="B47" s="196" t="s">
-        <v>885</v>
+        <v>901</v>
       </c>
       <c r="C47" s="197">
-        <v>0</v>
-      </c>
-      <c r="D47" s="200" t="s">
+        <v>212.04</v>
+      </c>
+      <c r="D47" s="331" t="s">
         <v>33</v>
       </c>
       <c r="E47" s="199" t="s">
         <v>611</v>
       </c>
-      <c r="F47" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="F47" s="671" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="329">
+        <v>44454</v>
+      </c>
       <c r="B48" s="196" t="s">
-        <v>885</v>
+        <v>902</v>
       </c>
       <c r="C48" s="197">
-        <v>0</v>
-      </c>
-      <c r="D48" s="200" t="s">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="D48" s="198" t="s">
         <v>33</v>
       </c>
       <c r="E48" s="199" t="s">
         <v>611</v>
       </c>
-      <c r="F48" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F48" s="671" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="196" t="s">
         <v>885</v>
@@ -42881,15 +43081,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="330"/>
+    <row r="52" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
       <c r="B52" s="196" t="s">
         <v>885</v>
       </c>
       <c r="C52" s="197">
         <v>0</v>
       </c>
-      <c r="D52" s="331" t="s">
+      <c r="D52" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E52" s="199" t="s">
@@ -42900,14 +43100,14 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="329"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="196" t="s">
         <v>885</v>
       </c>
       <c r="C53" s="197">
         <v>0</v>
       </c>
-      <c r="D53" s="198" t="s">
+      <c r="D53" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E53" s="199" t="s">
@@ -42935,98 +43135,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
-      <c r="B55" s="196" t="s">
-        <v>885</v>
-      </c>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C55" s="197">
-        <v>0</v>
-      </c>
-      <c r="D55" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E55" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F55" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="196" t="s">
-        <v>885</v>
-      </c>
-      <c r="C56" s="197">
-        <v>0</v>
-      </c>
-      <c r="D56" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E56" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F56" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
-      <c r="B57" s="196" t="s">
-        <v>885</v>
-      </c>
-      <c r="C57" s="197">
-        <v>0</v>
-      </c>
-      <c r="D57" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E57" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F57" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="B58" s="196" t="s">
-        <v>885</v>
-      </c>
-      <c r="C58" s="197">
-        <v>0</v>
-      </c>
-      <c r="D58" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E58" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F58" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="196" t="s">
-        <v>885</v>
-      </c>
-      <c r="C59" s="197">
-        <v>0</v>
-      </c>
-      <c r="D59" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" s="199" t="s">
-        <v>611</v>
-      </c>
-      <c r="F59" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="197">
         <v>0</v>
       </c>
     </row>
@@ -43035,7 +43145,7 @@
     <sortCondition ref="B45:B46"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B39:E39"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -43073,32 +43183,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="653" t="s">
+      <c r="B1" s="666" t="s">
         <v>726</v>
       </c>
-      <c r="C1" s="653"/>
-      <c r="D1" s="653"/>
-      <c r="E1" s="653"/>
-      <c r="H1" s="656" t="s">
+      <c r="C1" s="666"/>
+      <c r="D1" s="666"/>
+      <c r="E1" s="666"/>
+      <c r="H1" s="667" t="s">
         <v>726</v>
       </c>
-      <c r="I1" s="656"/>
-      <c r="J1" s="656"/>
+      <c r="I1" s="667"/>
+      <c r="J1" s="667"/>
       <c r="K1" s="205"/>
       <c r="L1" s="205"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="653" t="s">
+      <c r="O1" s="666" t="s">
         <v>725</v>
       </c>
-      <c r="P1" s="653"/>
+      <c r="P1" s="666"/>
     </row>
     <row r="2" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="577" t="s">
+      <c r="E2" s="585" t="s">
         <v>562</v>
       </c>
       <c r="F2" s="496"/>
@@ -43124,7 +43234,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="365"/>
-      <c r="E3" s="577"/>
+      <c r="E3" s="585"/>
       <c r="F3" s="496"/>
       <c r="H3" s="444">
         <v>126476.5</v>
@@ -43136,10 +43246,10 @@
         <v>44378</v>
       </c>
       <c r="K3" s="495"/>
-      <c r="L3" s="624" t="s">
+      <c r="L3" s="632" t="s">
         <v>567</v>
       </c>
-      <c r="M3" s="624"/>
+      <c r="M3" s="632"/>
       <c r="O3" s="444">
         <v>64006</v>
       </c>
@@ -43683,7 +43793,7 @@
         <v>44391</v>
       </c>
       <c r="K16" s="495"/>
-      <c r="L16" s="612">
+      <c r="L16" s="620">
         <f>SUM(L4:L15)</f>
         <v>3606750</v>
       </c>
@@ -43724,7 +43834,7 @@
         <v>44392</v>
       </c>
       <c r="K17" s="495"/>
-      <c r="L17" s="613"/>
+      <c r="L17" s="621"/>
       <c r="M17" s="475"/>
       <c r="O17" s="444">
         <v>0</v>
@@ -43797,10 +43907,10 @@
         <v>44394</v>
       </c>
       <c r="K19" s="495"/>
-      <c r="L19" s="614" t="s">
+      <c r="L19" s="622" t="s">
         <v>719</v>
       </c>
-      <c r="M19" s="615"/>
+      <c r="M19" s="623"/>
       <c r="O19" s="444">
         <v>0</v>
       </c>
@@ -43870,11 +43980,11 @@
         <v>44396</v>
       </c>
       <c r="K21" s="495"/>
-      <c r="L21" s="657">
+      <c r="L21" s="660">
         <f>L16-H37</f>
         <v>-383122.2200000002</v>
       </c>
-      <c r="M21" s="658"/>
+      <c r="M21" s="661"/>
       <c r="O21" s="444">
         <v>0</v>
       </c>
@@ -43908,8 +44018,8 @@
         <v>44397</v>
       </c>
       <c r="K22" s="495"/>
-      <c r="L22" s="659"/>
-      <c r="M22" s="660"/>
+      <c r="L22" s="662"/>
+      <c r="M22" s="663"/>
       <c r="O22" s="444">
         <v>0</v>
       </c>
@@ -44307,35 +44417,35 @@
       <c r="Q36" s="392"/>
     </row>
     <row r="37" spans="7:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H37" s="620">
+      <c r="H37" s="628">
         <f>SUM(H3:H36)</f>
         <v>3989872.22</v>
       </c>
-      <c r="I37" s="622">
+      <c r="I37" s="630">
         <f>SUM(I3:I36)</f>
         <v>688820.5</v>
       </c>
       <c r="J37" s="495"/>
       <c r="K37" s="495"/>
       <c r="L37" s="495"/>
-      <c r="O37" s="620">
+      <c r="O37" s="628">
         <f>SUM(O3:O36)</f>
         <v>1464800.09</v>
       </c>
-      <c r="P37" s="622">
+      <c r="P37" s="630">
         <f>SUM(P3:P36)</f>
         <v>121896</v>
       </c>
       <c r="Q37" s="392"/>
     </row>
     <row r="38" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H38" s="621"/>
-      <c r="I38" s="623"/>
+      <c r="H38" s="629"/>
+      <c r="I38" s="631"/>
       <c r="J38" s="495"/>
       <c r="K38" s="495"/>
       <c r="L38" s="495"/>
-      <c r="O38" s="621"/>
-      <c r="P38" s="623"/>
+      <c r="O38" s="629"/>
+      <c r="P38" s="631"/>
       <c r="Q38" s="392"/>
     </row>
     <row r="39" spans="7:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -44347,12 +44457,12 @@
     </row>
     <row r="40" spans="7:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G40" s="272"/>
-      <c r="H40" s="654"/>
-      <c r="I40" s="654"/>
-      <c r="O40" s="624" t="s">
+      <c r="H40" s="669"/>
+      <c r="I40" s="669"/>
+      <c r="O40" s="632" t="s">
         <v>567</v>
       </c>
-      <c r="P40" s="624"/>
+      <c r="P40" s="632"/>
       <c r="Q40" s="392"/>
     </row>
     <row r="41" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -44499,9 +44609,9 @@
     </row>
     <row r="53" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G53" s="272"/>
-      <c r="H53" s="655"/>
+      <c r="H53" s="670"/>
       <c r="I53" s="7"/>
-      <c r="O53" s="612">
+      <c r="O53" s="620">
         <f>SUM(O41:O52)</f>
         <v>1682687</v>
       </c>
@@ -44510,9 +44620,9 @@
     </row>
     <row r="54" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G54" s="272"/>
-      <c r="H54" s="655"/>
+      <c r="H54" s="670"/>
       <c r="I54" s="7"/>
-      <c r="O54" s="613"/>
+      <c r="O54" s="621"/>
       <c r="P54" s="475"/>
       <c r="Q54" s="392"/>
     </row>
@@ -44526,12 +44636,12 @@
     </row>
     <row r="56" spans="7:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="G56" s="272"/>
-      <c r="H56" s="654"/>
-      <c r="I56" s="654"/>
-      <c r="O56" s="614" t="s">
+      <c r="H56" s="669"/>
+      <c r="I56" s="669"/>
+      <c r="O56" s="622" t="s">
         <v>719</v>
       </c>
-      <c r="P56" s="615"/>
+      <c r="P56" s="623"/>
       <c r="Q56" s="392"/>
     </row>
     <row r="57" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -44544,8 +44654,8 @@
     </row>
     <row r="58" spans="7:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="272"/>
-      <c r="H58" s="652"/>
-      <c r="I58" s="652"/>
+      <c r="H58" s="668"/>
+      <c r="I58" s="668"/>
       <c r="O58" s="492">
         <f>O53-O37</f>
         <v>217886.90999999992</v>
@@ -44557,8 +44667,8 @@
     </row>
     <row r="59" spans="7:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="272"/>
-      <c r="H59" s="652"/>
-      <c r="I59" s="652"/>
+      <c r="H59" s="668"/>
+      <c r="I59" s="668"/>
       <c r="O59" s="505">
         <v>-383122.22</v>
       </c>
@@ -44586,20 +44696,14 @@
       <c r="P61" s="506"/>
     </row>
     <row r="62" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="O62" s="661">
+      <c r="O62" s="664">
         <f>SUM(O58:O61)</f>
         <v>-328961.31000000006</v>
       </c>
-      <c r="P62" s="662"/>
+      <c r="P62" s="665"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L16:L17"/>
     <mergeCell ref="H58:I59"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O37:O38"/>
@@ -44610,10 +44714,16 @@
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H53:H54"/>
     <mergeCell ref="H56:I56"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L16:L17"/>
     <mergeCell ref="O53:O54"/>
     <mergeCell ref="O56:P56"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L21:M22"/>
+    <mergeCell ref="O62:P62"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.13" top="0.43" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44635,12 +44745,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32"/>
-      <c r="B1" s="649" t="s">
+      <c r="B1" s="657" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="650"/>
-      <c r="D1" s="650"/>
-      <c r="E1" s="651"/>
+      <c r="C1" s="658"/>
+      <c r="D1" s="658"/>
+      <c r="E1" s="659"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -44722,12 +44832,12 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32"/>
-      <c r="B9" s="649" t="s">
+      <c r="B9" s="657" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="650"/>
-      <c r="D9" s="650"/>
-      <c r="E9" s="651"/>
+      <c r="C9" s="658"/>
+      <c r="D9" s="658"/>
+      <c r="E9" s="659"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -44883,12 +44993,12 @@
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32"/>
-      <c r="B20" s="649" t="s">
+      <c r="B20" s="657" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="650"/>
-      <c r="D20" s="650"/>
-      <c r="E20" s="651"/>
+      <c r="C20" s="658"/>
+      <c r="D20" s="658"/>
+      <c r="E20" s="659"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -45046,12 +45156,12 @@
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
-      <c r="B31" s="649" t="s">
+      <c r="B31" s="657" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="650"/>
-      <c r="D31" s="650"/>
-      <c r="E31" s="651"/>
+      <c r="C31" s="658"/>
+      <c r="D31" s="658"/>
+      <c r="E31" s="659"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -45205,12 +45315,12 @@
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32"/>
-      <c r="B42" s="649" t="s">
+      <c r="B42" s="657" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="650"/>
-      <c r="D42" s="650"/>
-      <c r="E42" s="651"/>
+      <c r="C42" s="658"/>
+      <c r="D42" s="658"/>
+      <c r="E42" s="659"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -45364,12 +45474,12 @@
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="32"/>
-      <c r="B54" s="649" t="s">
+      <c r="B54" s="657" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="650"/>
-      <c r="D54" s="650"/>
-      <c r="E54" s="651"/>
+      <c r="C54" s="658"/>
+      <c r="D54" s="658"/>
+      <c r="E54" s="659"/>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -45610,17 +45720,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -45651,17 +45761,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -45690,14 +45800,14 @@
       <c r="D4" s="23">
         <v>44230</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="537" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -48236,61 +48346,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="539" t="s">
+      <c r="H64" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="540"/>
+      <c r="I64" s="548"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="541">
+      <c r="K64" s="549">
         <f>I62+L62</f>
         <v>259947.00000000003</v>
       </c>
-      <c r="L64" s="542"/>
-      <c r="M64" s="543">
+      <c r="L64" s="550"/>
+      <c r="M64" s="551">
         <f>M62+N62</f>
         <v>2744320</v>
       </c>
-      <c r="N64" s="544"/>
+      <c r="N64" s="552"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="551" t="s">
+      <c r="D65" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="551"/>
+      <c r="E65" s="559"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2374814.2599999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="552">
+      <c r="P65" s="560">
         <f>P62+Q62</f>
         <v>3144691.75</v>
       </c>
-      <c r="Q65" s="553"/>
+      <c r="Q65" s="561"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="554" t="s">
+      <c r="D66" s="562" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="554"/>
+      <c r="E66" s="562"/>
       <c r="F66" s="95">
         <v>-2261593.1</v>
       </c>
-      <c r="I66" s="555" t="s">
+      <c r="I66" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="556"/>
-      <c r="K66" s="557">
+      <c r="J66" s="564"/>
+      <c r="K66" s="565">
         <f>F68+F69+F70</f>
         <v>355407.6199999997</v>
       </c>
-      <c r="L66" s="558"/>
+      <c r="L66" s="566"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -48327,11 +48437,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="559">
+      <c r="K68" s="567">
         <f>-C4</f>
         <v>-209541.1</v>
       </c>
-      <c r="L68" s="560"/>
+      <c r="L68" s="568"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -48355,22 +48465,22 @@
       <c r="C70" s="119">
         <v>44257</v>
       </c>
-      <c r="D70" s="545" t="s">
+      <c r="D70" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="546"/>
+      <c r="E70" s="554"/>
       <c r="F70" s="120">
         <v>223014.26</v>
       </c>
-      <c r="I70" s="547" t="s">
+      <c r="I70" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="548"/>
-      <c r="K70" s="549">
+      <c r="J70" s="556"/>
+      <c r="K70" s="557">
         <f>K66+K68</f>
         <v>145866.5199999997</v>
       </c>
-      <c r="L70" s="550"/>
+      <c r="L70" s="558"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -49758,17 +49868,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>429</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -49798,17 +49908,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -49837,14 +49947,14 @@
       <c r="D4" s="23">
         <v>44257</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="537" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -52446,61 +52556,61 @@
       <c r="A62" s="60"/>
       <c r="B62" s="100"/>
       <c r="C62" s="4"/>
-      <c r="H62" s="539" t="s">
+      <c r="H62" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="540"/>
+      <c r="I62" s="548"/>
       <c r="J62" s="101"/>
-      <c r="K62" s="541">
+      <c r="K62" s="549">
         <f>I60+L60</f>
         <v>781851.32000000007</v>
       </c>
-      <c r="L62" s="542"/>
-      <c r="M62" s="543">
+      <c r="L62" s="550"/>
+      <c r="M62" s="551">
         <f>M60+N60</f>
         <v>4064802.5</v>
       </c>
-      <c r="N62" s="544"/>
+      <c r="N62" s="552"/>
       <c r="O62" s="102"/>
       <c r="P62" s="99"/>
       <c r="Q62" s="99"/>
       <c r="S62" s="174"/>
     </row>
     <row r="63" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="551" t="s">
+      <c r="D63" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="551"/>
+      <c r="E63" s="559"/>
       <c r="F63" s="103">
         <f>F60-K62-C60</f>
         <v>3177878.1399999997</v>
       </c>
       <c r="I63" s="104"/>
       <c r="J63" s="105"/>
-      <c r="P63" s="552">
+      <c r="P63" s="560">
         <f>P60+Q60</f>
         <v>4585432.34</v>
       </c>
-      <c r="Q63" s="553"/>
+      <c r="Q63" s="561"/>
       <c r="S63" s="50"/>
     </row>
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="554" t="s">
+      <c r="D64" s="562" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="554"/>
+      <c r="E64" s="562"/>
       <c r="F64" s="95">
         <v>-3579271.89</v>
       </c>
-      <c r="I64" s="555" t="s">
+      <c r="I64" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J64" s="556"/>
-      <c r="K64" s="557">
+      <c r="J64" s="564"/>
+      <c r="K64" s="565">
         <f>F66+F67+F68</f>
         <v>-110332.85000000047</v>
       </c>
-      <c r="L64" s="558"/>
+      <c r="L64" s="566"/>
       <c r="P64" s="50"/>
       <c r="S64" s="107"/>
     </row>
@@ -52534,11 +52644,11 @@
         <v>21</v>
       </c>
       <c r="J66" s="115"/>
-      <c r="K66" s="559">
+      <c r="K66" s="567">
         <f>-C4</f>
         <v>-223014.26</v>
       </c>
-      <c r="L66" s="560"/>
+      <c r="L66" s="568"/>
       <c r="M66" s="116"/>
       <c r="P66" s="50"/>
       <c r="Q66" s="7"/>
@@ -52562,22 +52672,22 @@
       <c r="C68" s="119">
         <v>44291</v>
       </c>
-      <c r="D68" s="545" t="s">
+      <c r="D68" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="546"/>
+      <c r="E68" s="554"/>
       <c r="F68" s="120">
         <v>215362.9</v>
       </c>
-      <c r="I68" s="561" t="s">
+      <c r="I68" s="569" t="s">
         <v>431</v>
       </c>
-      <c r="J68" s="562"/>
-      <c r="K68" s="563">
+      <c r="J68" s="570"/>
+      <c r="K68" s="571">
         <f>K64+K66</f>
         <v>-333347.11000000045</v>
       </c>
-      <c r="L68" s="564"/>
+      <c r="L68" s="572"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
       <c r="S68" s="121"/>
@@ -54181,17 +54291,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>430</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -54221,17 +54331,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -54260,14 +54370,14 @@
       <c r="D4" s="23">
         <v>44291</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="537" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="565"/>
+      <c r="I4" s="573"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -56759,61 +56869,61 @@
       <c r="A58" s="60"/>
       <c r="B58" s="100"/>
       <c r="C58" s="4"/>
-      <c r="H58" s="539" t="s">
+      <c r="H58" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I58" s="540"/>
+      <c r="I58" s="548"/>
       <c r="J58" s="101"/>
-      <c r="K58" s="541">
+      <c r="K58" s="549">
         <f>I56+L56</f>
         <v>370346.35000000003</v>
       </c>
-      <c r="L58" s="566"/>
-      <c r="M58" s="543">
+      <c r="L58" s="574"/>
+      <c r="M58" s="551">
         <f>M56+N56</f>
         <v>3537422</v>
       </c>
-      <c r="N58" s="544"/>
+      <c r="N58" s="552"/>
       <c r="O58" s="102"/>
       <c r="P58" s="99"/>
       <c r="Q58" s="99"/>
       <c r="S58" s="174"/>
     </row>
     <row r="59" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="551" t="s">
+      <c r="D59" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="567"/>
+      <c r="E59" s="575"/>
       <c r="F59" s="103">
         <f>F56-K58-C56</f>
         <v>3048717.54</v>
       </c>
       <c r="I59" s="104"/>
       <c r="J59" s="105"/>
-      <c r="P59" s="552">
+      <c r="P59" s="560">
         <f>P56+Q56</f>
         <v>8073324.3200000003</v>
       </c>
-      <c r="Q59" s="553"/>
+      <c r="Q59" s="561"/>
       <c r="S59" s="50"/>
     </row>
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="554" t="s">
+      <c r="D60" s="562" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="554"/>
+      <c r="E60" s="562"/>
       <c r="F60" s="95">
         <v>-3102716.28</v>
       </c>
-      <c r="I60" s="555" t="s">
+      <c r="I60" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J60" s="556"/>
-      <c r="K60" s="557">
+      <c r="J60" s="564"/>
+      <c r="K60" s="565">
         <f>F62+F63+F64</f>
         <v>216465.62000000023</v>
       </c>
-      <c r="L60" s="558"/>
+      <c r="L60" s="566"/>
       <c r="P60" s="50"/>
       <c r="S60" s="107"/>
     </row>
@@ -56847,11 +56957,11 @@
         <v>21</v>
       </c>
       <c r="J62" s="115"/>
-      <c r="K62" s="559">
+      <c r="K62" s="567">
         <f>-C4</f>
         <v>-215362.9</v>
       </c>
-      <c r="L62" s="560"/>
+      <c r="L62" s="568"/>
       <c r="M62" s="116"/>
       <c r="P62" s="50"/>
       <c r="Q62" s="7"/>
@@ -56875,22 +56985,22 @@
       <c r="C64" s="119">
         <v>44320</v>
       </c>
-      <c r="D64" s="545" t="s">
+      <c r="D64" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="546"/>
+      <c r="E64" s="554"/>
       <c r="F64" s="120">
         <v>249311.35999999999</v>
       </c>
-      <c r="I64" s="547" t="s">
+      <c r="I64" s="555" t="s">
         <v>25</v>
       </c>
-      <c r="J64" s="548"/>
-      <c r="K64" s="549">
+      <c r="J64" s="556"/>
+      <c r="K64" s="557">
         <f>K60+K62</f>
         <v>1102.720000000234</v>
       </c>
-      <c r="L64" s="550"/>
+      <c r="L64" s="558"/>
       <c r="P64" s="50"/>
       <c r="Q64" s="7"/>
       <c r="S64" s="121"/>
@@ -57945,17 +58055,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="531" t="s">
+      <c r="C1" s="539" t="s">
         <v>504</v>
       </c>
-      <c r="D1" s="531"/>
-      <c r="E1" s="531"/>
-      <c r="F1" s="531"/>
-      <c r="G1" s="531"/>
-      <c r="H1" s="531"/>
-      <c r="I1" s="531"/>
-      <c r="J1" s="531"/>
-      <c r="K1" s="531"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -57985,17 +58095,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="532" t="s">
+      <c r="B3" s="540" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="533"/>
+      <c r="C3" s="541"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="534" t="s">
+      <c r="H3" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="534"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -58024,14 +58134,14 @@
       <c r="D4" s="23">
         <v>44320</v>
       </c>
-      <c r="E4" s="535" t="s">
+      <c r="E4" s="543" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="536"/>
-      <c r="H4" s="537" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="538"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -60908,71 +61018,71 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="539" t="s">
+      <c r="H64" s="547" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="540"/>
+      <c r="I64" s="548"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="541">
+      <c r="K64" s="549">
         <f>I62+L62</f>
         <v>779034.56000000017</v>
       </c>
-      <c r="L64" s="542"/>
-      <c r="M64" s="543">
+      <c r="L64" s="550"/>
+      <c r="M64" s="551">
         <f>M62+N62</f>
         <v>4478181</v>
       </c>
-      <c r="N64" s="544"/>
+      <c r="N64" s="552"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="551" t="s">
+      <c r="D65" s="559" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="551"/>
+      <c r="E65" s="559"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>3602842.44</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="552">
+      <c r="P65" s="560">
         <f>P62+Q62</f>
         <v>5004562.5599999996</v>
       </c>
-      <c r="Q65" s="553"/>
+      <c r="Q65" s="561"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="568" t="s">
+      <c r="B66" s="576" t="s">
         <v>528</v>
       </c>
-      <c r="C66" s="569"/>
-      <c r="D66" s="551" t="s">
+      <c r="C66" s="577"/>
+      <c r="D66" s="559" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="551"/>
+      <c r="E66" s="559"/>
       <c r="F66" s="95">
         <v>-3854423.8</v>
       </c>
-      <c r="I66" s="555" t="s">
+      <c r="I66" s="563" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="556"/>
-      <c r="K66" s="557">
+      <c r="J66" s="564"/>
+      <c r="K66" s="565">
         <f>F68+F69+F70</f>
         <v>14998.430000000139</v>
       </c>
-      <c r="L66" s="558"/>
+      <c r="L66" s="566"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
     <row r="67" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="570"/>
-      <c r="C67" s="571"/>
+      <c r="B67" s="578"/>
+      <c r="C67" s="579"/>
       <c r="D67" s="108"/>
       <c r="E67" s="60"/>
       <c r="F67" s="109">
@@ -60987,8 +61097,8 @@
       <c r="S67" s="50"/>
     </row>
     <row r="68" spans="2:19" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="572"/>
-      <c r="C68" s="573"/>
+      <c r="B68" s="580"/>
+      <c r="C68" s="581"/>
       <c r="E68" s="60" t="s">
         <v>20</v>
       </c>
@@ -61001,11 +61111,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="559">
+      <c r="K68" s="567">
         <f>-C4</f>
         <v>-249311.35999999999</v>
       </c>
-      <c r="L68" s="560"/>
+      <c r="L68" s="568"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -61029,22 +61139,22 @@
       <c r="C70" s="119">
         <v>44353</v>
       </c>
-      <c r="D70" s="545" t="s">
+      <c r="D70" s="553" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="546"/>
+      <c r="E70" s="554"/>
       <c r="F70" s="120">
         <v>255764.39</v>
       </c>
-      <c r="I70" s="547" t="s">
+      <c r="I70" s="555" t="s">
         <v>431</v>
       </c>
-      <c r="J70" s="548"/>
-      <c r="K70" s="549">
+      <c r="J70" s="556"/>
+      <c r="K70" s="557">
         <f>K66+K68</f>
         <v>-234312.92999999985</v>
       </c>
-      <c r="L70" s="550"/>
+      <c r="L70" s="558"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>

</xml_diff>

<commit_message>
CIERRE 4 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
@@ -630,7 +630,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="899">
   <si>
     <t>MORRALLA EN CAJA DE 11 SUR   2,800.00  +  $ 1,200.00 Total    $  4,000.00</t>
   </si>
@@ -3311,19 +3311,22 @@
     <t>ELIS</t>
   </si>
   <si>
-    <t>#  302667</t>
-  </si>
-  <si>
-    <t># 302668</t>
-  </si>
-  <si>
-    <t>#  302638</t>
-  </si>
-  <si>
-    <t># 302641</t>
-  </si>
-  <si>
     <t>NOMINA # 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONGANIZA-POLLO   </t>
+  </si>
+  <si>
+    <t>#  303931</t>
+  </si>
+  <si>
+    <t># 303933</t>
+  </si>
+  <si>
+    <t>#  304080</t>
+  </si>
+  <si>
+    <t>LONGANIZA-QUESOS-MANTECA-POLLO</t>
   </si>
 </sst>
 </file>
@@ -6386,26 +6389,38 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="58" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6447,31 +6462,26 @@
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="15" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6486,14 +6496,14 @@
     <xf numFmtId="166" fontId="6" fillId="15" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6512,15 +6522,6 @@
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6600,32 +6601,26 @@
     <xf numFmtId="44" fontId="49" fillId="0" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="8" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6666,28 +6661,37 @@
     <xf numFmtId="44" fontId="16" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="35" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6701,12 +6705,6 @@
     </xf>
     <xf numFmtId="166" fontId="35" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="7" fontId="6" fillId="11" borderId="73" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6732,6 +6730,18 @@
     <xf numFmtId="44" fontId="35" fillId="7" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6746,6 +6756,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="7" fontId="35" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6768,25 +6790,6 @@
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -12980,17 +12983,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -13021,17 +13024,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -13060,14 +13063,14 @@
       <c r="D4" s="23">
         <v>44201</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="575" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -15678,61 +15681,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="557"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="558">
         <f>I62+L62</f>
         <v>360753.85</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="559"/>
+      <c r="M64" s="560">
         <f>M62+N62</f>
         <v>2886514.7</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="561"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="568"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2365880.5699999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="561">
+      <c r="P65" s="547">
         <f>P62+Q62</f>
         <v>3321521.28</v>
       </c>
-      <c r="Q65" s="562"/>
+      <c r="Q65" s="548"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="563" t="s">
+      <c r="D66" s="549" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="563"/>
+      <c r="E66" s="549"/>
       <c r="F66" s="95">
         <v>-2276696.6800000002</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="551"/>
+      <c r="K66" s="552">
         <f>F68+F69+F70</f>
         <v>344253.98999999964</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="553"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -15766,11 +15769,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="554">
         <f>-C4</f>
         <v>-250864.68</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="555"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -15794,22 +15797,22 @@
       <c r="C70" s="119">
         <v>44230</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="563"/>
       <c r="F70" s="120">
         <v>209541.1</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="565"/>
+      <c r="K70" s="566">
         <f>K66+K68</f>
         <v>93389.309999999648</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="567"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -15913,11 +15916,11 @@
     <sortCondition ref="J35:J54"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
@@ -15925,11 +15928,11 @@
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="K70:L70"/>
     <mergeCell ref="D65:E65"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.2" right="0.16" top="0.34" bottom="0.32" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -17354,20 +17357,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="617" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -17377,7 +17380,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="618"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -17396,27 +17399,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="600" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="600"/>
+      <c r="AD2" s="600"/>
+      <c r="AE2" s="600"/>
+      <c r="AF2" s="600"/>
+      <c r="AG2" s="600"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -17424,7 +17427,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="586" t="s">
+      <c r="P3" s="590" t="s">
         <v>562</v>
       </c>
       <c r="Q3" s="393"/>
@@ -17437,12 +17440,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="600"/>
+      <c r="AC3" s="600"/>
+      <c r="AD3" s="600"/>
+      <c r="AE3" s="600"/>
+      <c r="AF3" s="600"/>
+      <c r="AG3" s="600"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -17455,14 +17458,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="575" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -17473,7 +17476,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="586"/>
+      <c r="P4" s="590"/>
       <c r="Q4" s="393"/>
       <c r="R4" s="30"/>
       <c r="S4" s="31"/>
@@ -17488,16 +17491,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="601" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="602"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="603" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="603"/>
+      <c r="AG4" s="603"/>
     </row>
     <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
@@ -18909,10 +18912,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="608" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="609"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -19056,11 +19059,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="610" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="611"/>
+      <c r="AG25" s="614">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -19131,9 +19134,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="612"/>
+      <c r="AF26" s="613"/>
+      <c r="AG26" s="615"/>
     </row>
     <row r="27" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
@@ -19308,10 +19311,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="604" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="606">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -19347,11 +19350,11 @@
         <v>0</v>
       </c>
       <c r="O30" s="7"/>
-      <c r="P30" s="587">
+      <c r="P30" s="591">
         <f>SUM(P5:P29)</f>
         <v>-163726</v>
       </c>
-      <c r="Q30" s="587"/>
+      <c r="Q30" s="591"/>
       <c r="R30" s="7">
         <v>0</v>
       </c>
@@ -19365,8 +19368,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="605"/>
+      <c r="AC30" s="607"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -20728,21 +20731,21 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="557"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="558">
         <f>I62+L62</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="559"/>
+      <c r="M64" s="560">
         <f>M62+N62</f>
         <v>2936130</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="561"/>
       <c r="O64" s="367"/>
       <c r="P64" s="367"/>
       <c r="Q64" s="367"/>
@@ -20757,40 +20760,40 @@
       <c r="AG64" s="327"/>
     </row>
     <row r="65" spans="2:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="568"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2702101.7199999997</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="R65" s="561">
+      <c r="R65" s="547">
         <f>R62+S62</f>
         <v>3138957.44</v>
       </c>
-      <c r="S65" s="562"/>
+      <c r="S65" s="548"/>
       <c r="U65" s="50"/>
     </row>
     <row r="66" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="563" t="s">
+      <c r="D66" s="549" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="563"/>
+      <c r="E66" s="549"/>
       <c r="F66" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="551"/>
+      <c r="K66" s="552">
         <f>F68+F69+F70</f>
         <v>381077.48999999953</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="553"/>
       <c r="R66" s="50"/>
       <c r="U66" s="107"/>
     </row>
@@ -20824,11 +20827,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="554">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="555"/>
       <c r="M68" s="116"/>
       <c r="R68" s="50"/>
       <c r="S68" s="7"/>
@@ -20852,22 +20855,22 @@
       <c r="C70" s="119">
         <v>44377</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="563"/>
       <c r="F70" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="565"/>
+      <c r="K70" s="566">
         <f>K66+K68</f>
         <v>125313.09999999951</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="567"/>
       <c r="R70" s="50"/>
       <c r="S70" s="7"/>
       <c r="U70" s="121"/>
@@ -20883,14 +20886,14 @@
       <c r="S71" s="7"/>
     </row>
     <row r="72" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I72" s="588" t="s">
+      <c r="I72" s="592" t="s">
         <v>610</v>
       </c>
-      <c r="J72" s="589"/>
-      <c r="K72" s="592">
+      <c r="J72" s="593"/>
+      <c r="K72" s="596">
         <v>163726</v>
       </c>
-      <c r="L72" s="593"/>
+      <c r="L72" s="597"/>
       <c r="R72" s="7"/>
       <c r="S72" s="7"/>
     </row>
@@ -20899,10 +20902,10 @@
       <c r="C73" s="128"/>
       <c r="D73" s="129"/>
       <c r="E73" s="7"/>
-      <c r="I73" s="590"/>
-      <c r="J73" s="591"/>
-      <c r="K73" s="594"/>
-      <c r="L73" s="595"/>
+      <c r="I73" s="594"/>
+      <c r="J73" s="595"/>
+      <c r="K73" s="598"/>
+      <c r="L73" s="599"/>
       <c r="M73" s="2"/>
       <c r="N73" s="60"/>
       <c r="O73" s="165"/>
@@ -20954,7 +20957,7 @@
       <c r="C76" s="130"/>
       <c r="E76" s="7"/>
       <c r="M76" s="4"/>
-      <c r="AC76" s="585"/>
+      <c r="AC76" s="616"/>
       <c r="AD76" s="342"/>
       <c r="AE76" s="342"/>
       <c r="AF76" s="342"/>
@@ -20967,7 +20970,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="273"/>
       <c r="M77" s="4"/>
-      <c r="AC77" s="585"/>
+      <c r="AC77" s="616"/>
       <c r="AD77" s="342"/>
       <c r="AE77" s="342"/>
       <c r="AF77" s="342"/>
@@ -21061,6 +21064,22 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AC76:AC77"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="I72:J73"/>
@@ -21076,22 +21095,6 @@
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
-    <mergeCell ref="AC76:AC77"/>
-    <mergeCell ref="R65:S65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.49" right="0.23622047244094491" top="0.47244094488188981" bottom="0.27559055118110237" header="0.70866141732283472" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22429,25 +22432,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="617" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="618"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -22457,27 +22460,27 @@
       <c r="L2" s="12"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="Q2" s="596" t="s">
+      <c r="Q2" s="600" t="s">
         <v>596</v>
       </c>
-      <c r="R2" s="596"/>
-      <c r="S2" s="596"/>
-      <c r="T2" s="596"/>
-      <c r="U2" s="596"/>
-      <c r="V2" s="596"/>
+      <c r="R2" s="600"/>
+      <c r="S2" s="600"/>
+      <c r="T2" s="600"/>
+      <c r="U2" s="600"/>
+      <c r="V2" s="600"/>
     </row>
     <row r="3" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -22485,12 +22488,12 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="Q3" s="596"/>
-      <c r="R3" s="596"/>
-      <c r="S3" s="596"/>
-      <c r="T3" s="596"/>
-      <c r="U3" s="596"/>
-      <c r="V3" s="596"/>
+      <c r="Q3" s="600"/>
+      <c r="R3" s="600"/>
+      <c r="S3" s="600"/>
+      <c r="T3" s="600"/>
+      <c r="U3" s="600"/>
+      <c r="V3" s="600"/>
     </row>
     <row r="4" spans="1:23" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -22503,14 +22506,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="575" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -22522,16 +22525,16 @@
       </c>
       <c r="O4" s="365"/>
       <c r="P4" s="29"/>
-      <c r="Q4" s="597" t="s">
+      <c r="Q4" s="601" t="s">
         <v>527</v>
       </c>
-      <c r="R4" s="598"/>
+      <c r="R4" s="602"/>
       <c r="S4" s="99"/>
-      <c r="T4" s="599" t="s">
+      <c r="T4" s="603" t="s">
         <v>567</v>
       </c>
-      <c r="U4" s="599"/>
-      <c r="V4" s="599"/>
+      <c r="U4" s="603"/>
+      <c r="V4" s="603"/>
       <c r="W4" s="99"/>
     </row>
     <row r="5" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23530,10 +23533,10 @@
         <v>0</v>
       </c>
       <c r="S23" s="99"/>
-      <c r="T23" s="604" t="s">
+      <c r="T23" s="608" t="s">
         <v>564</v>
       </c>
-      <c r="U23" s="605"/>
+      <c r="U23" s="609"/>
       <c r="V23" s="339">
         <f>SUM(V6:V22)</f>
         <v>2323600</v>
@@ -23637,11 +23640,11 @@
         <v>138607</v>
       </c>
       <c r="S25" s="99"/>
-      <c r="T25" s="606" t="s">
+      <c r="T25" s="610" t="s">
         <v>565</v>
       </c>
-      <c r="U25" s="607"/>
-      <c r="V25" s="610">
+      <c r="U25" s="611"/>
+      <c r="V25" s="614">
         <f>R29-V23</f>
         <v>163726</v>
       </c>
@@ -23690,9 +23693,9 @@
         <v>107480</v>
       </c>
       <c r="S26" s="99"/>
-      <c r="T26" s="608"/>
-      <c r="U26" s="609"/>
-      <c r="V26" s="611"/>
+      <c r="T26" s="612"/>
+      <c r="U26" s="613"/>
+      <c r="V26" s="615"/>
       <c r="W26" s="99"/>
     </row>
     <row r="27" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23815,10 +23818,10 @@
       </c>
       <c r="O29" s="7"/>
       <c r="P29" s="29"/>
-      <c r="Q29" s="600" t="s">
+      <c r="Q29" s="604" t="s">
         <v>562</v>
       </c>
-      <c r="R29" s="602">
+      <c r="R29" s="606">
         <f>SUM(R5:R28)</f>
         <v>2487326</v>
       </c>
@@ -23855,8 +23858,8 @@
       </c>
       <c r="O30" s="7"/>
       <c r="P30" s="373"/>
-      <c r="Q30" s="601"/>
-      <c r="R30" s="603"/>
+      <c r="Q30" s="605"/>
+      <c r="R30" s="607"/>
       <c r="S30" s="99"/>
       <c r="T30" s="99"/>
       <c r="U30" s="99"/>
@@ -24481,21 +24484,21 @@
       <c r="A50" s="60"/>
       <c r="B50" s="100"/>
       <c r="C50" s="4"/>
-      <c r="H50" s="548" t="s">
+      <c r="H50" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="549"/>
+      <c r="I50" s="557"/>
       <c r="J50" s="101"/>
-      <c r="K50" s="550">
+      <c r="K50" s="558">
         <f>I48+L48</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L50" s="551"/>
-      <c r="M50" s="552">
+      <c r="L50" s="559"/>
+      <c r="M50" s="560">
         <f>M48+N48</f>
         <v>612530</v>
       </c>
-      <c r="N50" s="553"/>
+      <c r="N50" s="561"/>
       <c r="O50" s="367"/>
       <c r="P50" s="102"/>
       <c r="Q50" s="320"/>
@@ -24507,10 +24510,10 @@
       <c r="W50" s="327"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D51" s="560" t="s">
+      <c r="D51" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="560"/>
+      <c r="E51" s="568"/>
       <c r="F51" s="103">
         <f>F48-K50-C48</f>
         <v>2702101.7199999997</v>
@@ -24519,22 +24522,22 @@
       <c r="J51" s="105"/>
     </row>
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D52" s="563" t="s">
+      <c r="D52" s="549" t="s">
         <v>502</v>
       </c>
-      <c r="E52" s="563"/>
+      <c r="E52" s="549"/>
       <c r="F52" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I52" s="564" t="s">
+      <c r="I52" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J52" s="565"/>
-      <c r="K52" s="566">
+      <c r="J52" s="551"/>
+      <c r="K52" s="552">
         <f>F54+F55+F56</f>
         <v>381077.72999999952</v>
       </c>
-      <c r="L52" s="567"/>
+      <c r="L52" s="553"/>
     </row>
     <row r="53" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="108"/>
@@ -24563,11 +24566,11 @@
         <v>21</v>
       </c>
       <c r="J54" s="115"/>
-      <c r="K54" s="568">
+      <c r="K54" s="554">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L54" s="569"/>
+      <c r="L54" s="555"/>
       <c r="M54" s="116"/>
     </row>
     <row r="55" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24585,22 +24588,22 @@
       <c r="C56" s="119">
         <v>44377</v>
       </c>
-      <c r="D56" s="554" t="s">
+      <c r="D56" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="555"/>
+      <c r="E56" s="563"/>
       <c r="F56" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I56" s="556" t="s">
+      <c r="I56" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J56" s="557"/>
-      <c r="K56" s="558">
+      <c r="J56" s="565"/>
+      <c r="K56" s="566">
         <f>K52+K54</f>
         <v>125313.3399999995</v>
       </c>
-      <c r="L56" s="559"/>
+      <c r="L56" s="567"/>
     </row>
     <row r="57" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C57" s="122"/>
@@ -24656,7 +24659,7 @@
       <c r="C62" s="130"/>
       <c r="E62" s="7"/>
       <c r="M62" s="4"/>
-      <c r="R62" s="585"/>
+      <c r="R62" s="616"/>
       <c r="S62" s="379"/>
       <c r="T62" s="379"/>
       <c r="U62" s="379"/>
@@ -24669,7 +24672,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="273"/>
       <c r="M63" s="4"/>
-      <c r="R63" s="585"/>
+      <c r="R63" s="616"/>
       <c r="S63" s="379"/>
       <c r="T63" s="379"/>
       <c r="U63" s="379"/>
@@ -24746,6 +24749,23 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="Q2:V3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T25:U26"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="Q29:Q30"/>
+    <mergeCell ref="R29:R30"/>
     <mergeCell ref="R62:R63"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
@@ -24755,23 +24775,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="I56:J56"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T25:U26"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="Q29:Q30"/>
-    <mergeCell ref="R29:R30"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="Q2:V3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24825,20 +24828,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="617" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -24848,7 +24851,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="618"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -24867,27 +24870,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="600" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="600"/>
+      <c r="AD2" s="600"/>
+      <c r="AE2" s="600"/>
+      <c r="AF2" s="600"/>
+      <c r="AG2" s="600"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -24895,13 +24898,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="634" t="s">
+      <c r="P3" s="619" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="636" t="s">
+      <c r="Q3" s="621" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="637"/>
+      <c r="S3" s="622"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -24911,12 +24914,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="600"/>
+      <c r="AC3" s="600"/>
+      <c r="AD3" s="600"/>
+      <c r="AE3" s="600"/>
+      <c r="AF3" s="600"/>
+      <c r="AG3" s="600"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -24929,14 +24932,14 @@
       <c r="D4" s="23">
         <v>44377</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="635" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="620" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -24947,10 +24950,10 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="634"/>
-      <c r="Q4" s="636"/>
+      <c r="P4" s="619"/>
+      <c r="Q4" s="621"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="637"/>
+      <c r="S4" s="622"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -24962,16 +24965,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="601" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="602"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="603" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="603"/>
+      <c r="AG4" s="603"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -26408,10 +26411,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="608" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="609"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -26543,11 +26546,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="610" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="611"/>
+      <c r="AG25" s="614">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -26616,9 +26619,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="612"/>
+      <c r="AF26" s="613"/>
+      <c r="AG26" s="615"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -26817,10 +26820,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="604" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="606">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -26883,8 +26886,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="605"/>
+      <c r="AC30" s="607"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -27377,11 +27380,11 @@
       <c r="J39" s="233"/>
       <c r="K39" s="361"/>
       <c r="L39" s="357"/>
-      <c r="M39" s="629">
+      <c r="M39" s="631">
         <f>SUM(M5:M38)</f>
         <v>3989472.22</v>
       </c>
-      <c r="N39" s="631">
+      <c r="N39" s="633">
         <f>SUM(N5:N38)</f>
         <v>689220.5</v>
       </c>
@@ -27430,8 +27433,8 @@
         <f>1145.91+398.99+423.94+498.99+398.99</f>
         <v>2866.8199999999997</v>
       </c>
-      <c r="M40" s="630"/>
-      <c r="N40" s="632"/>
+      <c r="M40" s="632"/>
+      <c r="N40" s="634"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -27624,10 +27627,10 @@
       <c r="L44" s="358">
         <v>73526</v>
       </c>
-      <c r="M44" s="633" t="s">
+      <c r="M44" s="635" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="633"/>
+      <c r="N44" s="635"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -28215,7 +28218,7 @@
       <c r="L57" s="458">
         <v>7482</v>
       </c>
-      <c r="M57" s="621">
+      <c r="M57" s="623">
         <f>SUM(M45:M56)</f>
         <v>3606750</v>
       </c>
@@ -28255,7 +28258,7 @@
       <c r="L58" s="458">
         <v>986</v>
       </c>
-      <c r="M58" s="622"/>
+      <c r="M58" s="624"/>
       <c r="N58" s="475"/>
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
@@ -28330,10 +28333,10 @@
         <f>1033.33+165.33</f>
         <v>1198.6599999999999</v>
       </c>
-      <c r="M60" s="623" t="s">
+      <c r="M60" s="625" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="624"/>
+      <c r="N60" s="626"/>
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -28406,11 +28409,11 @@
       <c r="L62" s="458">
         <v>22595.71</v>
       </c>
-      <c r="M62" s="625">
+      <c r="M62" s="627">
         <f>M57-M39</f>
         <v>-382722.2200000002</v>
       </c>
-      <c r="N62" s="626"/>
+      <c r="N62" s="628"/>
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -28446,8 +28449,8 @@
       <c r="L63" s="458">
         <v>1064</v>
       </c>
-      <c r="M63" s="627"/>
-      <c r="N63" s="628"/>
+      <c r="M63" s="629"/>
+      <c r="N63" s="630"/>
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -28637,16 +28640,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="548" t="s">
+      <c r="H69" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="549"/>
+      <c r="I69" s="557"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="550">
+      <c r="K69" s="558">
         <f>I67+L67</f>
         <v>587206.12</v>
       </c>
-      <c r="L69" s="551"/>
+      <c r="L69" s="559"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="367"/>
@@ -28663,40 +28666,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="560" t="s">
+      <c r="D70" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="560"/>
+      <c r="E70" s="568"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>3436910.52</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="561">
+      <c r="R70" s="547">
         <f>R67+S67</f>
         <v>10503773.959999999</v>
       </c>
-      <c r="S70" s="562"/>
+      <c r="S70" s="548"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="563" t="s">
+      <c r="D71" s="549" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="563"/>
+      <c r="E71" s="549"/>
       <c r="F71" s="95">
         <v>-3290264.27</v>
       </c>
-      <c r="I71" s="564" t="s">
+      <c r="I71" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="565"/>
-      <c r="K71" s="566">
+      <c r="J71" s="551"/>
+      <c r="K71" s="552">
         <f>F73+F74+F75</f>
         <v>426565.1</v>
       </c>
-      <c r="L71" s="567"/>
+      <c r="L71" s="553"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -28730,11 +28733,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="568">
+      <c r="K73" s="554">
         <f>-C4</f>
         <v>-308642.71999999997</v>
       </c>
-      <c r="L73" s="612"/>
+      <c r="L73" s="636"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -28757,22 +28760,22 @@
       <c r="C75" s="119">
         <v>44410</v>
       </c>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="563"/>
       <c r="F75" s="120">
         <v>250140.85</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="565"/>
+      <c r="K75" s="566">
         <f>K71+K73</f>
         <v>117922.38</v>
       </c>
-      <c r="L75" s="558"/>
+      <c r="L75" s="566"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -28787,14 +28790,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="613" t="s">
+      <c r="I77" s="637" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="614"/>
-      <c r="K77" s="617">
+      <c r="J77" s="638"/>
+      <c r="K77" s="641">
         <v>-383122.22</v>
       </c>
-      <c r="L77" s="618"/>
+      <c r="L77" s="642"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -28803,10 +28806,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="615"/>
-      <c r="J78" s="616"/>
-      <c r="K78" s="619"/>
-      <c r="L78" s="620"/>
+      <c r="I78" s="639"/>
+      <c r="J78" s="640"/>
+      <c r="K78" s="643"/>
+      <c r="L78" s="644"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="165"/>
@@ -28858,7 +28861,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="585"/>
+      <c r="AC81" s="616"/>
       <c r="AD81" s="440"/>
       <c r="AE81" s="440"/>
       <c r="AF81" s="440"/>
@@ -28871,7 +28874,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="585"/>
+      <c r="AC82" s="616"/>
       <c r="AD82" s="440"/>
       <c r="AE82" s="440"/>
       <c r="AF82" s="440"/>
@@ -28965,6 +28968,28 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AE25:AF26"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="M57:M58"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="M62:N63"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="M44:N44"/>
     <mergeCell ref="AG25:AG26"/>
     <mergeCell ref="AB29:AB30"/>
     <mergeCell ref="AC29:AC30"/>
@@ -28980,28 +29005,6 @@
     <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AE25:AF26"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="M57:M58"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M62:N63"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.27559055118110237" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30684,20 +30687,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="617" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>721</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -30707,7 +30710,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="618"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -30726,27 +30729,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="600" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="600"/>
+      <c r="AD2" s="600"/>
+      <c r="AE2" s="600"/>
+      <c r="AF2" s="600"/>
+      <c r="AG2" s="600"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -30757,13 +30760,13 @@
       <c r="O3" s="366" t="s">
         <v>753</v>
       </c>
-      <c r="P3" s="634" t="s">
+      <c r="P3" s="619" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="636" t="s">
+      <c r="Q3" s="621" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="637"/>
+      <c r="S3" s="622"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -30773,12 +30776,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="600"/>
+      <c r="AC3" s="600"/>
+      <c r="AD3" s="600"/>
+      <c r="AE3" s="600"/>
+      <c r="AF3" s="600"/>
+      <c r="AG3" s="600"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -30791,14 +30794,14 @@
       <c r="D4" s="23">
         <v>44411</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="635" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="620" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -30809,10 +30812,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="634"/>
-      <c r="Q4" s="636"/>
+      <c r="P4" s="619"/>
+      <c r="Q4" s="621"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="637"/>
+      <c r="S4" s="622"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -30824,16 +30827,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="601" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="602"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="603" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="603"/>
+      <c r="AG4" s="603"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -32321,10 +32324,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="608" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="609"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -32464,11 +32467,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="610" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="611"/>
+      <c r="AG25" s="614">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -32540,9 +32543,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="612"/>
+      <c r="AF26" s="613"/>
+      <c r="AG26" s="615"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -32752,10 +32755,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="604" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="606">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -32820,8 +32823,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="605"/>
+      <c r="AC30" s="607"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -33338,7 +33341,7 @@
         <f>SUM(M5:M38)</f>
         <v>2842451</v>
       </c>
-      <c r="N39" s="631">
+      <c r="N39" s="633">
         <f>SUM(N5:N38)</f>
         <v>271503</v>
       </c>
@@ -33390,7 +33393,7 @@
         <v>20880</v>
       </c>
       <c r="M40" s="538"/>
-      <c r="N40" s="632"/>
+      <c r="N40" s="634"/>
       <c r="O40" s="392"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -33584,10 +33587,10 @@
       <c r="L44" s="358">
         <v>986</v>
       </c>
-      <c r="M44" s="633" t="s">
+      <c r="M44" s="635" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="633"/>
+      <c r="N44" s="635"/>
       <c r="O44" s="392"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -34234,10 +34237,10 @@
       <c r="L60" s="458">
         <v>2479.5</v>
       </c>
-      <c r="M60" s="623" t="s">
+      <c r="M60" s="625" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="624"/>
+      <c r="N60" s="626"/>
       <c r="O60" s="392"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -34304,11 +34307,11 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="642">
+      <c r="M62" s="647">
         <f>M39-M58</f>
         <v>37331</v>
       </c>
-      <c r="N62" s="643"/>
+      <c r="N62" s="648"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -34340,8 +34343,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="644"/>
-      <c r="N63" s="645"/>
+      <c r="M63" s="649"/>
+      <c r="N63" s="650"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -34373,10 +34376,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="648">
+      <c r="M64" s="651">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="649"/>
+      <c r="N64" s="652"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -34407,10 +34410,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="650">
+      <c r="M65" s="653">
         <v>-163726</v>
       </c>
-      <c r="N65" s="651"/>
+      <c r="N65" s="654"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -34441,12 +34444,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="652">
+      <c r="M66" s="655">
         <f>SUM(M65+M64+M62)</f>
         <v>-509117.22</v>
       </c>
-      <c r="N66" s="653"/>
-      <c r="O66" s="646" t="s">
+      <c r="N66" s="656"/>
+      <c r="O66" s="645" t="s">
         <v>821</v>
       </c>
       <c r="P66" s="7"/>
@@ -34500,9 +34503,9 @@
         <f>SUM(L5:L66)</f>
         <v>482695.31000000006</v>
       </c>
-      <c r="M67" s="654"/>
-      <c r="N67" s="655"/>
-      <c r="O67" s="647"/>
+      <c r="M67" s="657"/>
+      <c r="N67" s="658"/>
+      <c r="O67" s="646"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
@@ -34534,16 +34537,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="548" t="s">
+      <c r="H69" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="549"/>
+      <c r="I69" s="557"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="550">
+      <c r="K69" s="558">
         <f>I67+L67</f>
         <v>518841.31000000006</v>
       </c>
-      <c r="L69" s="551"/>
+      <c r="L69" s="559"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="489"/>
@@ -34560,40 +34563,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="560" t="s">
+      <c r="D70" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="560"/>
+      <c r="E70" s="568"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>2539226.3499999996</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="561">
+      <c r="R70" s="547">
         <f>R67+S67</f>
         <v>7378939.6599999992</v>
       </c>
-      <c r="S70" s="562"/>
+      <c r="S70" s="548"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="563" t="s">
+      <c r="D71" s="549" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="563"/>
+      <c r="E71" s="549"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="564" t="s">
+      <c r="I71" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="565"/>
-      <c r="K71" s="566">
+      <c r="J71" s="551"/>
+      <c r="K71" s="552">
         <f>F73+F74+F75</f>
         <v>536310.85999999964</v>
       </c>
-      <c r="L71" s="567"/>
+      <c r="L71" s="553"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -34627,11 +34630,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="568">
+      <c r="K73" s="554">
         <f>-C4</f>
         <v>-250140.85</v>
       </c>
-      <c r="L73" s="612"/>
+      <c r="L73" s="636"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -34654,22 +34657,22 @@
       <c r="C75" s="119">
         <v>44439</v>
       </c>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="563"/>
       <c r="F75" s="120">
         <v>365611.59</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="565"/>
+      <c r="K75" s="566">
         <f>K71+K73</f>
         <v>286170.00999999966</v>
       </c>
-      <c r="L75" s="558"/>
+      <c r="L75" s="566"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -34684,14 +34687,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="638" t="s">
+      <c r="I77" s="659" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="639"/>
-      <c r="K77" s="642">
+      <c r="J77" s="660"/>
+      <c r="K77" s="647">
         <v>37331</v>
       </c>
-      <c r="L77" s="643"/>
+      <c r="L77" s="648"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -34700,10 +34703,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="640"/>
-      <c r="J78" s="641"/>
-      <c r="K78" s="644"/>
-      <c r="L78" s="645"/>
+      <c r="I78" s="661"/>
+      <c r="J78" s="662"/>
+      <c r="K78" s="649"/>
+      <c r="L78" s="650"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -34755,7 +34758,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="585"/>
+      <c r="AC81" s="616"/>
       <c r="AD81" s="486"/>
       <c r="AE81" s="486"/>
       <c r="AF81" s="486"/>
@@ -34768,7 +34771,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="585"/>
+      <c r="AC82" s="616"/>
       <c r="AD82" s="486"/>
       <c r="AE82" s="486"/>
       <c r="AF82" s="486"/>
@@ -34865,6 +34868,30 @@
     <sortCondition ref="N45:N55"/>
   </sortState>
   <mergeCells count="39">
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="M62:N63"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N67"/>
+    <mergeCell ref="M44:N44"/>
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
@@ -34880,30 +34907,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="M62:N63"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M66:N67"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36443,8 +36446,8 @@
   </sheetPr>
   <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36479,20 +36482,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="617" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>836</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -36502,7 +36505,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="618"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -36521,27 +36524,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="600" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="600"/>
+      <c r="AD2" s="600"/>
+      <c r="AE2" s="600"/>
+      <c r="AF2" s="600"/>
+      <c r="AG2" s="600"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -36549,13 +36552,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="634" t="s">
+      <c r="P3" s="619" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="636" t="s">
+      <c r="Q3" s="621" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="637" t="s">
+      <c r="S3" s="622" t="s">
         <v>868</v>
       </c>
       <c r="W3" s="213" t="s">
@@ -36567,12 +36570,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="600"/>
+      <c r="AC3" s="600"/>
+      <c r="AD3" s="600"/>
+      <c r="AE3" s="600"/>
+      <c r="AF3" s="600"/>
+      <c r="AG3" s="600"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -36585,14 +36588,14 @@
       <c r="D4" s="23">
         <v>44439</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="635" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="620" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -36603,10 +36606,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="634"/>
-      <c r="Q4" s="636"/>
+      <c r="P4" s="619"/>
+      <c r="Q4" s="621"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="637"/>
+      <c r="S4" s="622"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -36618,16 +36621,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="601" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="602"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="603" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="603"/>
+      <c r="AG4" s="603"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -37960,19 +37963,19 @@
       <c r="B22" s="134">
         <v>44457</v>
       </c>
-      <c r="C22" s="672"/>
-      <c r="D22" s="673"/>
-      <c r="E22" s="674">
+      <c r="C22" s="540"/>
+      <c r="D22" s="541"/>
+      <c r="E22" s="542">
         <v>44457</v>
       </c>
-      <c r="F22" s="675">
-        <v>0</v>
-      </c>
-      <c r="G22" s="676"/>
-      <c r="H22" s="677">
+      <c r="F22" s="543">
+        <v>0</v>
+      </c>
+      <c r="G22" s="544"/>
+      <c r="H22" s="545">
         <v>44457</v>
       </c>
-      <c r="I22" s="678"/>
+      <c r="I22" s="546"/>
       <c r="J22" s="52"/>
       <c r="K22" s="165"/>
       <c r="L22" s="61"/>
@@ -38048,7 +38051,7 @@
         <v>44457</v>
       </c>
       <c r="K23" s="279" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="L23" s="53">
         <f>27198.44+400</f>
@@ -38092,10 +38095,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="608" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="609"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -38106,25 +38109,33 @@
       <c r="B24" s="134">
         <v>44459</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="139"/>
+      <c r="C24" s="36">
+        <v>2895</v>
+      </c>
+      <c r="D24" s="139" t="s">
+        <v>106</v>
+      </c>
       <c r="E24" s="136">
         <v>44459</v>
       </c>
-      <c r="F24" s="37"/>
+      <c r="F24" s="37">
+        <v>117293</v>
+      </c>
       <c r="G24" s="137"/>
       <c r="H24" s="138">
         <v>44459</v>
       </c>
-      <c r="I24" s="38"/>
+      <c r="I24" s="38">
+        <v>440</v>
+      </c>
       <c r="J24" s="294"/>
       <c r="K24" s="295"/>
       <c r="L24" s="296"/>
       <c r="M24" s="444">
-        <v>0</v>
+        <v>109275</v>
       </c>
       <c r="N24" s="334">
-        <v>0</v>
+        <v>6616</v>
       </c>
       <c r="O24" s="491"/>
       <c r="P24" s="389">
@@ -38135,11 +38146,11 @@
       </c>
       <c r="R24" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S24" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>119226</v>
+      </c>
+      <c r="S24" s="201">
+        <f t="shared" si="0"/>
+        <v>1933</v>
       </c>
       <c r="T24" s="48"/>
       <c r="W24" s="213" t="s">
@@ -38163,25 +38174,33 @@
       <c r="B25" s="134">
         <v>44460</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="139"/>
+      <c r="C25" s="36">
+        <v>5471</v>
+      </c>
+      <c r="D25" s="139" t="s">
+        <v>894</v>
+      </c>
       <c r="E25" s="136">
         <v>44460</v>
       </c>
-      <c r="F25" s="37"/>
+      <c r="F25" s="37">
+        <v>82166</v>
+      </c>
       <c r="G25" s="137"/>
       <c r="H25" s="138">
         <v>44460</v>
       </c>
-      <c r="I25" s="38"/>
+      <c r="I25" s="38">
+        <v>440</v>
+      </c>
       <c r="J25" s="297"/>
       <c r="K25" s="172"/>
       <c r="L25" s="75"/>
       <c r="M25" s="444">
-        <v>0</v>
+        <v>66730</v>
       </c>
       <c r="N25" s="334">
-        <v>0</v>
+        <v>9525</v>
       </c>
       <c r="O25" s="491"/>
       <c r="P25" s="389">
@@ -38192,7 +38211,7 @@
       </c>
       <c r="R25" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>82166</v>
       </c>
       <c r="S25" s="6">
         <f t="shared" si="0"/>
@@ -38215,11 +38234,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="610" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="611"/>
+      <c r="AG25" s="614">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -38229,25 +38248,33 @@
       <c r="B26" s="134">
         <v>44461</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="139"/>
+      <c r="C26" s="36">
+        <v>16172</v>
+      </c>
+      <c r="D26" s="139" t="s">
+        <v>898</v>
+      </c>
       <c r="E26" s="136">
         <v>44461</v>
       </c>
-      <c r="F26" s="37"/>
+      <c r="F26" s="37">
+        <v>107611</v>
+      </c>
       <c r="G26" s="137"/>
       <c r="H26" s="138">
         <v>44461</v>
       </c>
-      <c r="I26" s="38"/>
+      <c r="I26" s="38">
+        <v>3618</v>
+      </c>
       <c r="J26" s="52"/>
       <c r="K26" s="295"/>
       <c r="L26" s="53"/>
       <c r="M26" s="444">
-        <v>0</v>
+        <v>81416</v>
       </c>
       <c r="N26" s="334">
-        <v>0</v>
+        <v>6405</v>
       </c>
       <c r="O26" s="491"/>
       <c r="P26" s="389">
@@ -38258,7 +38285,7 @@
       </c>
       <c r="R26" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>107611</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" si="0"/>
@@ -38281,9 +38308,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="612"/>
+      <c r="AF26" s="613"/>
+      <c r="AG26" s="615"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -38449,10 +38476,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="604" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="606">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -38507,8 +38534,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="605"/>
+      <c r="AC30" s="607"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -38941,20 +38968,20 @@
       <c r="J39" s="299"/>
       <c r="K39" s="246"/>
       <c r="L39" s="46"/>
-      <c r="M39" s="629">
+      <c r="M39" s="631">
         <f>SUM(M5:M38)</f>
-        <v>1945472.02</v>
-      </c>
-      <c r="N39" s="631">
+        <v>2202893.02</v>
+      </c>
+      <c r="N39" s="633">
         <f>SUM(N5:N38)</f>
-        <v>169534</v>
+        <v>192080</v>
       </c>
       <c r="O39" s="392"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <f>SUM(R5:R38)</f>
-        <v>2472816.88</v>
+        <v>2781819.88</v>
       </c>
       <c r="T39" s="48"/>
       <c r="W39" s="213" t="s">
@@ -38984,8 +39011,8 @@
       <c r="J40" s="299"/>
       <c r="K40" s="172"/>
       <c r="L40" s="46"/>
-      <c r="M40" s="630"/>
-      <c r="N40" s="632"/>
+      <c r="M40" s="632"/>
+      <c r="N40" s="634"/>
       <c r="O40" s="392"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -39129,10 +39156,10 @@
       <c r="J44" s="299"/>
       <c r="K44" s="528"/>
       <c r="L44" s="71"/>
-      <c r="M44" s="633" t="s">
+      <c r="M44" s="635" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="633"/>
+      <c r="N44" s="635"/>
       <c r="O44" s="392"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -39598,7 +39625,7 @@
       <c r="J58" s="529"/>
       <c r="K58" s="468"/>
       <c r="L58" s="50"/>
-      <c r="M58" s="656">
+      <c r="M58" s="663">
         <f t="shared" ref="M58" si="2">SUM(M45:M57)</f>
         <v>0</v>
       </c>
@@ -39632,7 +39659,7 @@
       <c r="J59" s="529"/>
       <c r="K59" s="243"/>
       <c r="L59" s="50"/>
-      <c r="M59" s="657"/>
+      <c r="M59" s="664"/>
       <c r="N59" s="42"/>
       <c r="O59" s="392"/>
       <c r="P59" s="7"/>
@@ -39663,10 +39690,10 @@
       <c r="J60" s="529"/>
       <c r="K60" s="468"/>
       <c r="L60" s="50"/>
-      <c r="M60" s="623" t="s">
+      <c r="M60" s="625" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="624"/>
+      <c r="N60" s="626"/>
       <c r="O60" s="392"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -39727,10 +39754,10 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="642">
+      <c r="M62" s="647">
         <v>-37331</v>
       </c>
-      <c r="N62" s="643"/>
+      <c r="N62" s="648"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -39762,8 +39789,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="644"/>
-      <c r="N63" s="645"/>
+      <c r="M63" s="649"/>
+      <c r="N63" s="650"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -39795,10 +39822,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="648">
+      <c r="M64" s="651">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="649"/>
+      <c r="N64" s="652"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -39829,10 +39856,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="650">
+      <c r="M65" s="653">
         <v>-163726</v>
       </c>
-      <c r="N65" s="651"/>
+      <c r="N65" s="654"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -39863,12 +39890,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="652">
+      <c r="M66" s="655">
         <f>SUM(M65+M64+M62)</f>
         <v>-583779.22</v>
       </c>
-      <c r="N66" s="653"/>
-      <c r="O66" s="646"/>
+      <c r="N66" s="656"/>
+      <c r="O66" s="645"/>
       <c r="P66" s="7"/>
       <c r="Q66" s="7"/>
       <c r="R66" s="84">
@@ -39894,7 +39921,7 @@
       </c>
       <c r="C67" s="86">
         <f>SUM(C5:C66)</f>
-        <v>183493.29</v>
+        <v>208031.29</v>
       </c>
       <c r="D67" s="87"/>
       <c r="E67" s="88" t="s">
@@ -39902,7 +39929,7 @@
       </c>
       <c r="F67" s="89">
         <f>SUM(F5:F66)</f>
-        <v>2448739</v>
+        <v>2755809</v>
       </c>
       <c r="G67" s="87"/>
       <c r="H67" s="90" t="s">
@@ -39910,7 +39937,7 @@
       </c>
       <c r="I67" s="91">
         <f>SUM(I5:I66)</f>
-        <v>28058</v>
+        <v>32556</v>
       </c>
       <c r="J67" s="92"/>
       <c r="K67" s="93" t="s">
@@ -39920,18 +39947,18 @@
         <f>SUM(L5:L66)</f>
         <v>146259.57</v>
       </c>
-      <c r="M67" s="654"/>
-      <c r="N67" s="655"/>
-      <c r="O67" s="647"/>
+      <c r="M67" s="657"/>
+      <c r="N67" s="658"/>
+      <c r="O67" s="646"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
         <f>SUM(R5:R66)</f>
-        <v>4945633.76</v>
+        <v>5563639.7599999998</v>
       </c>
       <c r="S67" s="7">
         <f>SUM(S5:S66)</f>
-        <v>24077.880000000005</v>
+        <v>26010.880000000005</v>
       </c>
       <c r="T67" s="97"/>
       <c r="W67" s="210"/>
@@ -39954,16 +39981,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="548" t="s">
+      <c r="H69" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="549"/>
+      <c r="I69" s="557"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="550">
+      <c r="K69" s="558">
         <f>I67+L67</f>
-        <v>174317.57</v>
-      </c>
-      <c r="L69" s="551"/>
+        <v>178815.57</v>
+      </c>
+      <c r="L69" s="559"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="489"/>
@@ -39980,40 +40007,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="560" t="s">
+      <c r="D70" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="560"/>
+      <c r="E70" s="568"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
-        <v>2090928.1400000001</v>
+        <v>2368962.14</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="561">
+      <c r="R70" s="547">
         <f>R67+S67</f>
-        <v>4969711.6399999997</v>
-      </c>
-      <c r="S70" s="562"/>
+        <v>5589650.6399999997</v>
+      </c>
+      <c r="S70" s="548"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="563" t="s">
+      <c r="D71" s="549" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="563"/>
+      <c r="E71" s="549"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="564" t="s">
+      <c r="I71" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="565"/>
-      <c r="K71" s="566">
+      <c r="J71" s="551"/>
+      <c r="K71" s="552">
         <f>F73+F74+F75</f>
-        <v>-289784.93999999994</v>
-      </c>
-      <c r="L71" s="567"/>
+        <v>-11750.939999999944</v>
+      </c>
+      <c r="L71" s="553"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -40040,18 +40067,18 @@
       </c>
       <c r="F73" s="95">
         <f>SUM(F70:F72)</f>
-        <v>-289784.93999999994</v>
+        <v>-11750.939999999944</v>
       </c>
       <c r="H73" s="34"/>
       <c r="I73" s="114" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="568">
+      <c r="K73" s="554">
         <f>-C4</f>
         <v>-365611.59</v>
       </c>
-      <c r="L73" s="612"/>
+      <c r="L73" s="636"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -40072,22 +40099,22 @@
     </row>
     <row r="75" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="119"/>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="563"/>
       <c r="F75" s="120">
         <v>0</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="565"/>
+      <c r="K75" s="566">
         <f>K71+K73</f>
-        <v>-655396.53</v>
-      </c>
-      <c r="L75" s="558"/>
+        <v>-377362.52999999997</v>
+      </c>
+      <c r="L75" s="566"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -40102,14 +40129,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="638" t="s">
+      <c r="I77" s="659" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="639"/>
-      <c r="K77" s="642">
-        <v>0</v>
-      </c>
-      <c r="L77" s="643"/>
+      <c r="J77" s="660"/>
+      <c r="K77" s="647">
+        <v>0</v>
+      </c>
+      <c r="L77" s="648"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -40118,10 +40145,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="640"/>
-      <c r="J78" s="641"/>
-      <c r="K78" s="644"/>
-      <c r="L78" s="645"/>
+      <c r="I78" s="661"/>
+      <c r="J78" s="662"/>
+      <c r="K78" s="649"/>
+      <c r="L78" s="650"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -40173,7 +40200,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="585"/>
+      <c r="AC81" s="616"/>
       <c r="AD81" s="526"/>
       <c r="AE81" s="526"/>
       <c r="AF81" s="526"/>
@@ -40186,7 +40213,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="585"/>
+      <c r="AC82" s="616"/>
       <c r="AD82" s="526"/>
       <c r="AE82" s="526"/>
       <c r="AF82" s="526"/>
@@ -40280,24 +40307,16 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="AB2:AG3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="M62:N63"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AE4:AG4"/>
@@ -40311,16 +40330,24 @@
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="M58:M59"/>
     <mergeCell ref="M60:N60"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="AB2:AG3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -42865,8 +42892,8 @@
   </sheetPr>
   <dimension ref="A44:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42882,53 +42909,53 @@
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="32"/>
-      <c r="B46" s="658" t="s">
+      <c r="B46" s="665" t="s">
         <v>32</v>
       </c>
-      <c r="C46" s="659"/>
-      <c r="D46" s="659"/>
-      <c r="E46" s="660"/>
+      <c r="C46" s="666"/>
+      <c r="D46" s="666"/>
+      <c r="E46" s="667"/>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
-        <v>44457</v>
+        <v>44461</v>
       </c>
       <c r="B47" s="196" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C47" s="197">
-        <v>95</v>
+        <v>162.71</v>
       </c>
       <c r="D47" s="198" t="s">
         <v>33</v>
       </c>
       <c r="E47" s="199" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="F47" s="539">
-        <v>417</v>
+        <v>140</v>
       </c>
       <c r="G47" s="530"/>
     </row>
     <row r="48" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
-        <v>44457</v>
+        <v>44461</v>
       </c>
       <c r="B48" s="196" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C48" s="197">
-        <v>1365.91</v>
+        <v>32.04</v>
       </c>
       <c r="D48" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E48" s="199" t="s">
-        <v>896</v>
+        <v>611</v>
       </c>
       <c r="F48" s="539">
-        <v>1259</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -43177,7 +43204,7 @@
   <mergeCells count="1">
     <mergeCell ref="B46:E46"/>
   </mergeCells>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0" header="0.31496062992125984" footer="0.21"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -43213,32 +43240,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="663" t="s">
+      <c r="B1" s="674" t="s">
         <v>726</v>
       </c>
-      <c r="C1" s="663"/>
-      <c r="D1" s="663"/>
-      <c r="E1" s="663"/>
-      <c r="H1" s="664" t="s">
+      <c r="C1" s="674"/>
+      <c r="D1" s="674"/>
+      <c r="E1" s="674"/>
+      <c r="H1" s="675" t="s">
         <v>726</v>
       </c>
-      <c r="I1" s="664"/>
-      <c r="J1" s="664"/>
+      <c r="I1" s="675"/>
+      <c r="J1" s="675"/>
       <c r="K1" s="205"/>
       <c r="L1" s="205"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="663" t="s">
+      <c r="O1" s="674" t="s">
         <v>725</v>
       </c>
-      <c r="P1" s="663"/>
+      <c r="P1" s="674"/>
     </row>
     <row r="2" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="586" t="s">
+      <c r="E2" s="590" t="s">
         <v>562</v>
       </c>
       <c r="F2" s="496"/>
@@ -43264,7 +43291,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="365"/>
-      <c r="E3" s="586"/>
+      <c r="E3" s="590"/>
       <c r="F3" s="496"/>
       <c r="H3" s="444">
         <v>126476.5</v>
@@ -43276,10 +43303,10 @@
         <v>44378</v>
       </c>
       <c r="K3" s="495"/>
-      <c r="L3" s="633" t="s">
+      <c r="L3" s="635" t="s">
         <v>567</v>
       </c>
-      <c r="M3" s="633"/>
+      <c r="M3" s="635"/>
       <c r="O3" s="444">
         <v>64006</v>
       </c>
@@ -43823,7 +43850,7 @@
         <v>44391</v>
       </c>
       <c r="K16" s="495"/>
-      <c r="L16" s="621">
+      <c r="L16" s="623">
         <f>SUM(L4:L15)</f>
         <v>3606750</v>
       </c>
@@ -43864,7 +43891,7 @@
         <v>44392</v>
       </c>
       <c r="K17" s="495"/>
-      <c r="L17" s="622"/>
+      <c r="L17" s="624"/>
       <c r="M17" s="475"/>
       <c r="O17" s="444">
         <v>0</v>
@@ -43937,10 +43964,10 @@
         <v>44394</v>
       </c>
       <c r="K19" s="495"/>
-      <c r="L19" s="623" t="s">
+      <c r="L19" s="625" t="s">
         <v>719</v>
       </c>
-      <c r="M19" s="624"/>
+      <c r="M19" s="626"/>
       <c r="O19" s="444">
         <v>0</v>
       </c>
@@ -44447,35 +44474,35 @@
       <c r="Q36" s="392"/>
     </row>
     <row r="37" spans="7:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H37" s="629">
+      <c r="H37" s="631">
         <f>SUM(H3:H36)</f>
         <v>3989872.22</v>
       </c>
-      <c r="I37" s="631">
+      <c r="I37" s="633">
         <f>SUM(I3:I36)</f>
         <v>688820.5</v>
       </c>
       <c r="J37" s="495"/>
       <c r="K37" s="495"/>
       <c r="L37" s="495"/>
-      <c r="O37" s="629">
+      <c r="O37" s="631">
         <f>SUM(O3:O36)</f>
         <v>1464800.09</v>
       </c>
-      <c r="P37" s="631">
+      <c r="P37" s="633">
         <f>SUM(P3:P36)</f>
         <v>121896</v>
       </c>
       <c r="Q37" s="392"/>
     </row>
     <row r="38" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H38" s="630"/>
-      <c r="I38" s="632"/>
+      <c r="H38" s="632"/>
+      <c r="I38" s="634"/>
       <c r="J38" s="495"/>
       <c r="K38" s="495"/>
       <c r="L38" s="495"/>
-      <c r="O38" s="630"/>
-      <c r="P38" s="632"/>
+      <c r="O38" s="632"/>
+      <c r="P38" s="634"/>
       <c r="Q38" s="392"/>
     </row>
     <row r="39" spans="7:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -44487,12 +44514,12 @@
     </row>
     <row r="40" spans="7:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G40" s="272"/>
-      <c r="H40" s="666"/>
-      <c r="I40" s="666"/>
-      <c r="O40" s="633" t="s">
+      <c r="H40" s="677"/>
+      <c r="I40" s="677"/>
+      <c r="O40" s="635" t="s">
         <v>567</v>
       </c>
-      <c r="P40" s="633"/>
+      <c r="P40" s="635"/>
       <c r="Q40" s="392"/>
     </row>
     <row r="41" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -44639,9 +44666,9 @@
     </row>
     <row r="53" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G53" s="272"/>
-      <c r="H53" s="667"/>
+      <c r="H53" s="678"/>
       <c r="I53" s="7"/>
-      <c r="O53" s="621">
+      <c r="O53" s="623">
         <f>SUM(O41:O52)</f>
         <v>1682687</v>
       </c>
@@ -44650,9 +44677,9 @@
     </row>
     <row r="54" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G54" s="272"/>
-      <c r="H54" s="667"/>
+      <c r="H54" s="678"/>
       <c r="I54" s="7"/>
-      <c r="O54" s="622"/>
+      <c r="O54" s="624"/>
       <c r="P54" s="475"/>
       <c r="Q54" s="392"/>
     </row>
@@ -44666,12 +44693,12 @@
     </row>
     <row r="56" spans="7:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="G56" s="272"/>
-      <c r="H56" s="666"/>
-      <c r="I56" s="666"/>
-      <c r="O56" s="623" t="s">
+      <c r="H56" s="677"/>
+      <c r="I56" s="677"/>
+      <c r="O56" s="625" t="s">
         <v>719</v>
       </c>
-      <c r="P56" s="624"/>
+      <c r="P56" s="626"/>
       <c r="Q56" s="392"/>
     </row>
     <row r="57" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -44684,8 +44711,8 @@
     </row>
     <row r="58" spans="7:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="272"/>
-      <c r="H58" s="665"/>
-      <c r="I58" s="665"/>
+      <c r="H58" s="676"/>
+      <c r="I58" s="676"/>
       <c r="O58" s="492">
         <f>O53-O37</f>
         <v>217886.90999999992</v>
@@ -44697,8 +44724,8 @@
     </row>
     <row r="59" spans="7:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="272"/>
-      <c r="H59" s="665"/>
-      <c r="I59" s="665"/>
+      <c r="H59" s="676"/>
+      <c r="I59" s="676"/>
       <c r="O59" s="505">
         <v>-383122.22</v>
       </c>
@@ -44726,24 +44753,14 @@
       <c r="P61" s="506"/>
     </row>
     <row r="62" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="O62" s="661">
+      <c r="O62" s="672">
         <f>SUM(O58:O61)</f>
         <v>-328961.31000000006</v>
       </c>
-      <c r="P62" s="662"/>
+      <c r="P62" s="673"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L16:L17"/>
     <mergeCell ref="H58:I59"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O37:O38"/>
@@ -44754,6 +44771,16 @@
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H53:H54"/>
     <mergeCell ref="H56:I56"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="O62:P62"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.13" top="0.43" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44775,12 +44802,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32"/>
-      <c r="B1" s="658" t="s">
+      <c r="B1" s="665" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="659"/>
-      <c r="D1" s="659"/>
-      <c r="E1" s="660"/>
+      <c r="C1" s="666"/>
+      <c r="D1" s="666"/>
+      <c r="E1" s="667"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -44862,12 +44889,12 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32"/>
-      <c r="B9" s="658" t="s">
+      <c r="B9" s="665" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="659"/>
-      <c r="D9" s="659"/>
-      <c r="E9" s="660"/>
+      <c r="C9" s="666"/>
+      <c r="D9" s="666"/>
+      <c r="E9" s="667"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -45023,12 +45050,12 @@
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32"/>
-      <c r="B20" s="658" t="s">
+      <c r="B20" s="665" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="659"/>
-      <c r="D20" s="659"/>
-      <c r="E20" s="660"/>
+      <c r="C20" s="666"/>
+      <c r="D20" s="666"/>
+      <c r="E20" s="667"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -45186,12 +45213,12 @@
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
-      <c r="B31" s="658" t="s">
+      <c r="B31" s="665" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="659"/>
-      <c r="D31" s="659"/>
-      <c r="E31" s="660"/>
+      <c r="C31" s="666"/>
+      <c r="D31" s="666"/>
+      <c r="E31" s="667"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -45345,12 +45372,12 @@
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32"/>
-      <c r="B42" s="658" t="s">
+      <c r="B42" s="665" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="659"/>
-      <c r="D42" s="659"/>
-      <c r="E42" s="660"/>
+      <c r="C42" s="666"/>
+      <c r="D42" s="666"/>
+      <c r="E42" s="667"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -45504,12 +45531,12 @@
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="32"/>
-      <c r="B54" s="658" t="s">
+      <c r="B54" s="665" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="659"/>
-      <c r="D54" s="659"/>
-      <c r="E54" s="660"/>
+      <c r="C54" s="666"/>
+      <c r="D54" s="666"/>
+      <c r="E54" s="667"/>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -45750,17 +45777,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -45791,17 +45818,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -45830,14 +45857,14 @@
       <c r="D4" s="23">
         <v>44230</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="575" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -48376,61 +48403,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="557"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="558">
         <f>I62+L62</f>
         <v>259947.00000000003</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="559"/>
+      <c r="M64" s="560">
         <f>M62+N62</f>
         <v>2744320</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="561"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="568"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2374814.2599999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="561">
+      <c r="P65" s="547">
         <f>P62+Q62</f>
         <v>3144691.75</v>
       </c>
-      <c r="Q65" s="562"/>
+      <c r="Q65" s="548"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="563" t="s">
+      <c r="D66" s="549" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="563"/>
+      <c r="E66" s="549"/>
       <c r="F66" s="95">
         <v>-2261593.1</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="551"/>
+      <c r="K66" s="552">
         <f>F68+F69+F70</f>
         <v>355407.6199999997</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="553"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -48467,11 +48494,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="554">
         <f>-C4</f>
         <v>-209541.1</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="555"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -48495,22 +48522,22 @@
       <c r="C70" s="119">
         <v>44257</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="563"/>
       <c r="F70" s="120">
         <v>223014.26</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="565"/>
+      <c r="K70" s="566">
         <f>K66+K68</f>
         <v>145866.5199999997</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="567"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -48611,12 +48638,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -48628,6 +48649,12 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -49898,17 +49925,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>429</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -49938,17 +49965,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -49977,14 +50004,14 @@
       <c r="D4" s="23">
         <v>44257</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="575" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -52586,61 +52613,61 @@
       <c r="A62" s="60"/>
       <c r="B62" s="100"/>
       <c r="C62" s="4"/>
-      <c r="H62" s="548" t="s">
+      <c r="H62" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="549"/>
+      <c r="I62" s="557"/>
       <c r="J62" s="101"/>
-      <c r="K62" s="550">
+      <c r="K62" s="558">
         <f>I60+L60</f>
         <v>781851.32000000007</v>
       </c>
-      <c r="L62" s="551"/>
-      <c r="M62" s="552">
+      <c r="L62" s="559"/>
+      <c r="M62" s="560">
         <f>M60+N60</f>
         <v>4064802.5</v>
       </c>
-      <c r="N62" s="553"/>
+      <c r="N62" s="561"/>
       <c r="O62" s="102"/>
       <c r="P62" s="99"/>
       <c r="Q62" s="99"/>
       <c r="S62" s="174"/>
     </row>
     <row r="63" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="560" t="s">
+      <c r="D63" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="560"/>
+      <c r="E63" s="568"/>
       <c r="F63" s="103">
         <f>F60-K62-C60</f>
         <v>3177878.1399999997</v>
       </c>
       <c r="I63" s="104"/>
       <c r="J63" s="105"/>
-      <c r="P63" s="561">
+      <c r="P63" s="547">
         <f>P60+Q60</f>
         <v>4585432.34</v>
       </c>
-      <c r="Q63" s="562"/>
+      <c r="Q63" s="548"/>
       <c r="S63" s="50"/>
     </row>
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="563" t="s">
+      <c r="D64" s="549" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="563"/>
+      <c r="E64" s="549"/>
       <c r="F64" s="95">
         <v>-3579271.89</v>
       </c>
-      <c r="I64" s="564" t="s">
+      <c r="I64" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J64" s="565"/>
-      <c r="K64" s="566">
+      <c r="J64" s="551"/>
+      <c r="K64" s="552">
         <f>F66+F67+F68</f>
         <v>-110332.85000000047</v>
       </c>
-      <c r="L64" s="567"/>
+      <c r="L64" s="553"/>
       <c r="P64" s="50"/>
       <c r="S64" s="107"/>
     </row>
@@ -52674,11 +52701,11 @@
         <v>21</v>
       </c>
       <c r="J66" s="115"/>
-      <c r="K66" s="568">
+      <c r="K66" s="554">
         <f>-C4</f>
         <v>-223014.26</v>
       </c>
-      <c r="L66" s="569"/>
+      <c r="L66" s="555"/>
       <c r="M66" s="116"/>
       <c r="P66" s="50"/>
       <c r="Q66" s="7"/>
@@ -52702,22 +52729,22 @@
       <c r="C68" s="119">
         <v>44291</v>
       </c>
-      <c r="D68" s="554" t="s">
+      <c r="D68" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="555"/>
+      <c r="E68" s="563"/>
       <c r="F68" s="120">
         <v>215362.9</v>
       </c>
-      <c r="I68" s="570" t="s">
+      <c r="I68" s="577" t="s">
         <v>431</v>
       </c>
-      <c r="J68" s="571"/>
-      <c r="K68" s="572">
+      <c r="J68" s="578"/>
+      <c r="K68" s="579">
         <f>K64+K66</f>
         <v>-333347.11000000045</v>
       </c>
-      <c r="L68" s="573"/>
+      <c r="L68" s="580"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
       <c r="S68" s="121"/>
@@ -52873,12 +52900,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="D63:E63"/>
     <mergeCell ref="P63:Q63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="I64:J64"/>
@@ -52890,6 +52911,12 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H62:I62"/>
     <mergeCell ref="K62:L62"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="D63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -54321,17 +54348,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>430</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -54361,17 +54388,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -54400,14 +54427,14 @@
       <c r="D4" s="23">
         <v>44291</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="575" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="574"/>
+      <c r="I4" s="582"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -56899,61 +56926,61 @@
       <c r="A58" s="60"/>
       <c r="B58" s="100"/>
       <c r="C58" s="4"/>
-      <c r="H58" s="548" t="s">
+      <c r="H58" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I58" s="549"/>
+      <c r="I58" s="557"/>
       <c r="J58" s="101"/>
-      <c r="K58" s="550">
+      <c r="K58" s="558">
         <f>I56+L56</f>
         <v>370346.35000000003</v>
       </c>
-      <c r="L58" s="575"/>
-      <c r="M58" s="552">
+      <c r="L58" s="583"/>
+      <c r="M58" s="560">
         <f>M56+N56</f>
         <v>3537422</v>
       </c>
-      <c r="N58" s="553"/>
+      <c r="N58" s="561"/>
       <c r="O58" s="102"/>
       <c r="P58" s="99"/>
       <c r="Q58" s="99"/>
       <c r="S58" s="174"/>
     </row>
     <row r="59" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="560" t="s">
+      <c r="D59" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="576"/>
+      <c r="E59" s="581"/>
       <c r="F59" s="103">
         <f>F56-K58-C56</f>
         <v>3048717.54</v>
       </c>
       <c r="I59" s="104"/>
       <c r="J59" s="105"/>
-      <c r="P59" s="561">
+      <c r="P59" s="547">
         <f>P56+Q56</f>
         <v>8073324.3200000003</v>
       </c>
-      <c r="Q59" s="562"/>
+      <c r="Q59" s="548"/>
       <c r="S59" s="50"/>
     </row>
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="563" t="s">
+      <c r="D60" s="549" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="563"/>
+      <c r="E60" s="549"/>
       <c r="F60" s="95">
         <v>-3102716.28</v>
       </c>
-      <c r="I60" s="564" t="s">
+      <c r="I60" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J60" s="565"/>
-      <c r="K60" s="566">
+      <c r="J60" s="551"/>
+      <c r="K60" s="552">
         <f>F62+F63+F64</f>
         <v>216465.62000000023</v>
       </c>
-      <c r="L60" s="567"/>
+      <c r="L60" s="553"/>
       <c r="P60" s="50"/>
       <c r="S60" s="107"/>
     </row>
@@ -56987,11 +57014,11 @@
         <v>21</v>
       </c>
       <c r="J62" s="115"/>
-      <c r="K62" s="568">
+      <c r="K62" s="554">
         <f>-C4</f>
         <v>-215362.9</v>
       </c>
-      <c r="L62" s="569"/>
+      <c r="L62" s="555"/>
       <c r="M62" s="116"/>
       <c r="P62" s="50"/>
       <c r="Q62" s="7"/>
@@ -57015,22 +57042,22 @@
       <c r="C64" s="119">
         <v>44320</v>
       </c>
-      <c r="D64" s="554" t="s">
+      <c r="D64" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="555"/>
+      <c r="E64" s="563"/>
       <c r="F64" s="120">
         <v>249311.35999999999</v>
       </c>
-      <c r="I64" s="556" t="s">
+      <c r="I64" s="564" t="s">
         <v>25</v>
       </c>
-      <c r="J64" s="557"/>
-      <c r="K64" s="558">
+      <c r="J64" s="565"/>
+      <c r="K64" s="566">
         <f>K60+K62</f>
         <v>1102.720000000234</v>
       </c>
-      <c r="L64" s="559"/>
+      <c r="L64" s="567"/>
       <c r="P64" s="50"/>
       <c r="Q64" s="7"/>
       <c r="S64" s="121"/>
@@ -57186,12 +57213,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="D59:E59"/>
     <mergeCell ref="P59:Q59"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="I60:J60"/>
@@ -57203,6 +57224,12 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -58085,17 +58112,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="569" t="s">
         <v>504</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="569"/>
+      <c r="E1" s="569"/>
+      <c r="F1" s="569"/>
+      <c r="G1" s="569"/>
+      <c r="H1" s="569"/>
+      <c r="I1" s="569"/>
+      <c r="J1" s="569"/>
+      <c r="K1" s="569"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -58125,17 +58152,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="570" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="571"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="572" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="572"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -58164,14 +58191,14 @@
       <c r="D4" s="23">
         <v>44320</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="574"/>
+      <c r="H4" s="575" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="576"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -61048,71 +61075,71 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="556" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="557"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="558">
         <f>I62+L62</f>
         <v>779034.56000000017</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="559"/>
+      <c r="M64" s="560">
         <f>M62+N62</f>
         <v>4478181</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="561"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="568" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="568"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>3602842.44</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="561">
+      <c r="P65" s="547">
         <f>P62+Q62</f>
         <v>5004562.5599999996</v>
       </c>
-      <c r="Q65" s="562"/>
+      <c r="Q65" s="548"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="577" t="s">
+      <c r="B66" s="584" t="s">
         <v>528</v>
       </c>
-      <c r="C66" s="578"/>
-      <c r="D66" s="560" t="s">
+      <c r="C66" s="585"/>
+      <c r="D66" s="568" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="560"/>
+      <c r="E66" s="568"/>
       <c r="F66" s="95">
         <v>-3854423.8</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="550" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="551"/>
+      <c r="K66" s="552">
         <f>F68+F69+F70</f>
         <v>14998.430000000139</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="553"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
     <row r="67" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="579"/>
-      <c r="C67" s="580"/>
+      <c r="B67" s="586"/>
+      <c r="C67" s="587"/>
       <c r="D67" s="108"/>
       <c r="E67" s="60"/>
       <c r="F67" s="109">
@@ -61127,8 +61154,8 @@
       <c r="S67" s="50"/>
     </row>
     <row r="68" spans="2:19" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="581"/>
-      <c r="C68" s="582"/>
+      <c r="B68" s="588"/>
+      <c r="C68" s="589"/>
       <c r="E68" s="60" t="s">
         <v>20</v>
       </c>
@@ -61141,11 +61168,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="554">
         <f>-C4</f>
         <v>-249311.35999999999</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="555"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -61169,22 +61196,22 @@
       <c r="C70" s="119">
         <v>44353</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="562" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="563"/>
       <c r="F70" s="120">
         <v>255764.39</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="564" t="s">
         <v>431</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="565"/>
+      <c r="K70" s="566">
         <f>K66+K68</f>
         <v>-234312.92999999985</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="567"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -61340,11 +61367,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -61358,6 +61380,11 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="B66:C68"/>
     <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 11 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="17" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="19" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O     2 0 2 1    " sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="899">
   <si>
     <t>MORRALLA EN CAJA DE 11 SUR   2,800.00  +  $ 1,200.00 Total    $  4,000.00</t>
   </si>
@@ -3287,9 +3287,6 @@
     <t>NOMINA #  37</t>
   </si>
   <si>
-    <t xml:space="preserve">#  </t>
-  </si>
-  <si>
     <t>TOCINETA-CHISTORRA-QUESO-MANTECA-POLLO</t>
   </si>
   <si>
@@ -3323,25 +3320,13 @@
     <t>LONGANIZA--POLLO</t>
   </si>
   <si>
-    <t>#  304122</t>
-  </si>
-  <si>
-    <t># 304124</t>
-  </si>
-  <si>
-    <t>#  304142</t>
-  </si>
-  <si>
-    <t>#  304217</t>
-  </si>
-  <si>
-    <t># 304218</t>
-  </si>
-  <si>
-    <t>#  304342</t>
-  </si>
-  <si>
-    <t># 304343</t>
+    <t>LONGANIZA-QUESOS-POLLO-MAIZ</t>
+  </si>
+  <si>
+    <t>NOMINA # 39 +   PEPE</t>
+  </si>
+  <si>
+    <t>TOCINETA--LONGANIZA--POLLO</t>
   </si>
 </sst>
 </file>
@@ -5235,7 +5220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="672">
+  <cellXfs count="673">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6765,26 +6750,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="35" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="35" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="7" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6797,6 +6776,15 @@
     </xf>
     <xf numFmtId="166" fontId="6" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="35" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="35" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -36454,8 +36442,8 @@
   </sheetPr>
   <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="L25" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -37516,7 +37504,7 @@
         <v>29731</v>
       </c>
       <c r="D16" s="139" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E16" s="136">
         <v>44451</v>
@@ -37631,7 +37619,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="48" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="W17" s="213" t="s">
         <v>68</v>
@@ -37668,7 +37656,7 @@
         <v>2167.5</v>
       </c>
       <c r="D18" s="139" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E18" s="136">
         <v>44453</v>
@@ -37705,7 +37693,7 @@
         <v>194262</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="T18" s="48"/>
       <c r="W18" s="213" t="s">
@@ -37743,7 +37731,7 @@
         <v>22237</v>
       </c>
       <c r="D19" s="139" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E19" s="136">
         <v>44454</v>
@@ -37898,7 +37886,7 @@
         <v>12109</v>
       </c>
       <c r="D21" s="139" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E21" s="136">
         <v>44456</v>
@@ -37917,7 +37905,7 @@
         <v>44455</v>
       </c>
       <c r="K21" s="162" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="L21" s="53">
         <v>10000</v>
@@ -37994,7 +37982,7 @@
         <v>44457</v>
       </c>
       <c r="K22" s="165" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="L22" s="61">
         <f>27198.44+400</f>
@@ -38053,7 +38041,7 @@
         <v>4628</v>
       </c>
       <c r="D23" s="140" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E23" s="136">
         <v>44458</v>
@@ -38192,7 +38180,7 @@
         <v>5471</v>
       </c>
       <c r="D25" s="139" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E25" s="136">
         <v>44460</v>
@@ -38266,7 +38254,7 @@
         <v>16172</v>
       </c>
       <c r="D26" s="139" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E26" s="136">
         <v>44461</v>
@@ -38331,25 +38319,37 @@
       <c r="B27" s="134">
         <v>44462</v>
       </c>
-      <c r="C27" s="36"/>
+      <c r="C27" s="36">
+        <v>9477</v>
+      </c>
       <c r="D27" s="141"/>
       <c r="E27" s="136">
         <v>44462</v>
       </c>
-      <c r="F27" s="37"/>
+      <c r="F27" s="37">
+        <v>93196</v>
+      </c>
       <c r="G27" s="137"/>
       <c r="H27" s="138">
         <v>44462</v>
       </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="298"/>
-      <c r="K27" s="282"/>
-      <c r="L27" s="75"/>
+      <c r="I27" s="38">
+        <v>2135</v>
+      </c>
+      <c r="J27" s="298">
+        <v>44462</v>
+      </c>
+      <c r="K27" s="282" t="s">
+        <v>662</v>
+      </c>
+      <c r="L27" s="75">
+        <v>14000</v>
+      </c>
       <c r="M27" s="444">
-        <v>0</v>
+        <v>60026</v>
       </c>
       <c r="N27" s="334">
-        <v>0</v>
+        <v>7558</v>
       </c>
       <c r="O27" s="491"/>
       <c r="P27" s="389">
@@ -38360,7 +38360,7 @@
       </c>
       <c r="R27" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>93196</v>
       </c>
       <c r="S27" s="6">
         <f t="shared" si="0"/>
@@ -38392,25 +38392,33 @@
       <c r="B28" s="134">
         <v>44463</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="141"/>
+      <c r="C28" s="36">
+        <v>2253</v>
+      </c>
+      <c r="D28" s="141" t="s">
+        <v>45</v>
+      </c>
       <c r="E28" s="136">
         <v>44463</v>
       </c>
-      <c r="F28" s="37"/>
+      <c r="F28" s="37">
+        <v>163874</v>
+      </c>
       <c r="G28" s="137"/>
       <c r="H28" s="138">
         <v>44463</v>
       </c>
-      <c r="I28" s="38"/>
+      <c r="I28" s="38">
+        <v>600</v>
+      </c>
       <c r="J28" s="299"/>
       <c r="K28" s="151"/>
       <c r="L28" s="75"/>
       <c r="M28" s="444">
-        <v>0</v>
+        <v>141528</v>
       </c>
       <c r="N28" s="334">
-        <v>0</v>
+        <v>19493</v>
       </c>
       <c r="O28" s="491"/>
       <c r="P28" s="389">
@@ -38421,7 +38429,7 @@
       </c>
       <c r="R28" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>163874</v>
       </c>
       <c r="S28" s="6">
         <f t="shared" si="0"/>
@@ -38444,30 +38452,46 @@
       <c r="AF28" s="99"/>
       <c r="AG28" s="99"/>
     </row>
-    <row r="29" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" ht="33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="34"/>
       <c r="B29" s="134">
         <v>44464</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="143"/>
+      <c r="C29" s="36">
+        <v>14666</v>
+      </c>
+      <c r="D29" s="143" t="s">
+        <v>896</v>
+      </c>
       <c r="E29" s="136">
         <v>44464</v>
       </c>
-      <c r="F29" s="37"/>
+      <c r="F29" s="37">
+        <v>149350</v>
+      </c>
       <c r="G29" s="137"/>
       <c r="H29" s="138">
         <v>44464</v>
       </c>
-      <c r="I29" s="38"/>
-      <c r="J29" s="300"/>
-      <c r="K29" s="169"/>
-      <c r="L29" s="75"/>
+      <c r="I29" s="38">
+        <v>550</v>
+      </c>
+      <c r="J29" s="300">
+        <v>44464</v>
+      </c>
+      <c r="K29" s="672" t="s">
+        <v>897</v>
+      </c>
+      <c r="L29" s="75">
+        <f>23955.58+400+10000</f>
+        <v>34355.58</v>
+      </c>
       <c r="M29" s="444">
-        <v>0</v>
-      </c>
-      <c r="N29" s="334">
-        <v>0</v>
+        <v>95113</v>
+      </c>
+      <c r="N29" s="456">
+        <f>11325+ 45+90+120</f>
+        <v>11580</v>
       </c>
       <c r="O29" s="491"/>
       <c r="P29" s="389">
@@ -38478,11 +38502,11 @@
       </c>
       <c r="R29" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S29" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>156264.58000000002</v>
+      </c>
+      <c r="S29" s="202">
+        <f t="shared" si="0"/>
+        <v>6914.5800000000163</v>
       </c>
       <c r="T29" s="58"/>
       <c r="W29" s="213" t="s">
@@ -38507,25 +38531,33 @@
       <c r="B30" s="134">
         <v>44465</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="143"/>
+      <c r="C30" s="36">
+        <v>15280</v>
+      </c>
+      <c r="D30" s="143" t="s">
+        <v>898</v>
+      </c>
       <c r="E30" s="136">
         <v>44465</v>
       </c>
-      <c r="F30" s="37"/>
+      <c r="F30" s="37">
+        <v>168983</v>
+      </c>
       <c r="G30" s="137"/>
       <c r="H30" s="138">
         <v>44465</v>
       </c>
-      <c r="I30" s="38"/>
+      <c r="I30" s="38">
+        <v>600</v>
+      </c>
       <c r="J30" s="233"/>
       <c r="K30" s="356"/>
       <c r="L30" s="357"/>
       <c r="M30" s="444">
-        <v>0</v>
+        <v>140067</v>
       </c>
       <c r="N30" s="334">
-        <v>0</v>
+        <v>13036</v>
       </c>
       <c r="O30" s="491"/>
       <c r="P30" s="389">
@@ -38536,7 +38568,7 @@
       </c>
       <c r="R30" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>168983</v>
       </c>
       <c r="S30" s="6">
         <f t="shared" si="0"/>
@@ -38560,25 +38592,33 @@
       <c r="B31" s="134">
         <v>44466</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="266"/>
+      <c r="C31" s="36">
+        <v>2521</v>
+      </c>
+      <c r="D31" s="266" t="s">
+        <v>355</v>
+      </c>
       <c r="E31" s="136">
         <v>44466</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="37">
+        <v>105877</v>
+      </c>
       <c r="G31" s="137"/>
       <c r="H31" s="138">
         <v>44466</v>
       </c>
-      <c r="I31" s="38"/>
+      <c r="I31" s="38">
+        <v>930</v>
+      </c>
       <c r="J31" s="233"/>
       <c r="K31" s="144"/>
       <c r="L31" s="66"/>
       <c r="M31" s="444">
-        <v>0</v>
+        <v>89830</v>
       </c>
       <c r="N31" s="334">
-        <v>0</v>
+        <v>12596</v>
       </c>
       <c r="O31" s="491"/>
       <c r="P31" s="7"/>
@@ -38587,7 +38627,7 @@
       </c>
       <c r="R31" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>105877</v>
       </c>
       <c r="S31" s="6">
         <f t="shared" si="0"/>
@@ -38984,18 +39024,18 @@
       <c r="L39" s="46"/>
       <c r="M39" s="624">
         <f>SUM(M5:M38)</f>
-        <v>2332672</v>
+        <v>2859236</v>
       </c>
       <c r="N39" s="626">
         <f>SUM(N5:N38)</f>
-        <v>201666</v>
+        <v>265929</v>
       </c>
       <c r="O39" s="392"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <f>SUM(R5:R38)</f>
-        <v>2926612.86</v>
+        <v>3614807.44</v>
       </c>
       <c r="T39" s="48"/>
       <c r="W39" s="213" t="s">
@@ -39935,7 +39975,7 @@
       </c>
       <c r="C67" s="86">
         <f>SUM(C5:C66)</f>
-        <v>212659.29</v>
+        <v>256856.29</v>
       </c>
       <c r="D67" s="87"/>
       <c r="E67" s="88" t="s">
@@ -39943,7 +39983,7 @@
       </c>
       <c r="F67" s="89">
         <f>SUM(F5:F66)</f>
-        <v>2900602</v>
+        <v>3581882</v>
       </c>
       <c r="G67" s="87"/>
       <c r="H67" s="90" t="s">
@@ -39951,7 +39991,7 @@
       </c>
       <c r="I67" s="91">
         <f>SUM(I5:I66)</f>
-        <v>33356</v>
+        <v>38171</v>
       </c>
       <c r="J67" s="92"/>
       <c r="K67" s="93" t="s">
@@ -39959,7 +39999,7 @@
       </c>
       <c r="L67" s="522">
         <f>SUM(L5:L66)</f>
-        <v>146259.57</v>
+        <v>194615.15000000002</v>
       </c>
       <c r="M67" s="650"/>
       <c r="N67" s="651"/>
@@ -39968,11 +40008,11 @@
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
         <f>SUM(R5:R66)</f>
-        <v>5853225.7199999997</v>
+        <v>7229614.8799999999</v>
       </c>
       <c r="S67" s="7">
         <f>SUM(S5:S66)</f>
-        <v>26010.860000000015</v>
+        <v>32925.440000000031</v>
       </c>
       <c r="T67" s="97"/>
       <c r="W67" s="210"/>
@@ -40002,7 +40042,7 @@
       <c r="J69" s="101"/>
       <c r="K69" s="551">
         <f>I67+L67</f>
-        <v>179615.57</v>
+        <v>232786.15000000002</v>
       </c>
       <c r="L69" s="552"/>
       <c r="M69" s="470"/>
@@ -40027,13 +40067,13 @@
       <c r="E70" s="561"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
-        <v>2508327.14</v>
+        <v>3092239.56</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
       <c r="R70" s="540">
         <f>R67+S67</f>
-        <v>5879236.5800000001</v>
+        <v>7262540.3200000003</v>
       </c>
       <c r="S70" s="541"/>
       <c r="U70" s="50"/>
@@ -40052,7 +40092,7 @@
       <c r="J71" s="544"/>
       <c r="K71" s="545">
         <f>F73+F74+F75</f>
-        <v>127614.06000000006</v>
+        <v>711526.48</v>
       </c>
       <c r="L71" s="546"/>
       <c r="R71" s="50"/>
@@ -40081,7 +40121,7 @@
       </c>
       <c r="F73" s="95">
         <f>SUM(F70:F72)</f>
-        <v>127614.06000000006</v>
+        <v>711526.48</v>
       </c>
       <c r="H73" s="34"/>
       <c r="I73" s="114" t="s">
@@ -40126,7 +40166,7 @@
       <c r="J75" s="558"/>
       <c r="K75" s="559">
         <f>K71+K73</f>
-        <v>-237997.52999999997</v>
+        <v>345914.88999999996</v>
       </c>
       <c r="L75" s="559"/>
       <c r="R75" s="50"/>
@@ -42904,10 +42944,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A39:G57"/>
+  <dimension ref="A34:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42915,107 +42955,51 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="32"/>
-      <c r="B41" s="658" t="s">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="658" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="659"/>
-      <c r="D41" s="659"/>
-      <c r="E41" s="660"/>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19">
-        <v>44462</v>
-      </c>
-      <c r="B42" s="196" t="s">
-        <v>897</v>
-      </c>
-      <c r="C42" s="197">
-        <v>1859.13</v>
-      </c>
-      <c r="D42" s="198" t="s">
+      <c r="C44" s="659"/>
+      <c r="D44" s="659"/>
+      <c r="E44" s="660"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="196" t="s">
+        <v>611</v>
+      </c>
+      <c r="C45" s="197">
+        <v>0</v>
+      </c>
+      <c r="D45" s="198" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="199" t="s">
-        <v>898</v>
-      </c>
-      <c r="F42" s="539">
-        <v>1961</v>
-      </c>
-      <c r="G42" s="530"/>
-    </row>
-    <row r="43" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19">
-        <v>44462</v>
-      </c>
-      <c r="B43" s="196" t="s">
-        <v>899</v>
-      </c>
-      <c r="C43" s="197">
-        <v>20</v>
-      </c>
-      <c r="D43" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="199" t="s">
+      <c r="E45" s="199" t="s">
         <v>611</v>
       </c>
-      <c r="F43" s="539">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="19">
-        <v>44462</v>
-      </c>
-      <c r="B44" s="196" t="s">
-        <v>900</v>
-      </c>
-      <c r="C44" s="197">
-        <v>104.12</v>
-      </c>
-      <c r="D44" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="199" t="s">
-        <v>901</v>
-      </c>
-      <c r="F44" s="539">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19">
-        <v>44462</v>
-      </c>
-      <c r="B45" s="196" t="s">
-        <v>902</v>
-      </c>
-      <c r="C45" s="197">
-        <v>207.2</v>
-      </c>
-      <c r="D45" s="200" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="199" t="s">
-        <v>903</v>
-      </c>
       <c r="F45" s="539">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G45" s="530"/>
+    </row>
+    <row r="46" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="B46" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C46" s="197">
         <v>0</v>
@@ -43030,10 +43014,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C47" s="197">
         <v>0</v>
@@ -43051,7 +43035,7 @@
     <row r="48" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C48" s="197">
         <v>0</v>
@@ -43066,15 +43050,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="330"/>
+    <row r="49" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
       <c r="B49" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C49" s="197">
         <v>0</v>
       </c>
-      <c r="D49" s="331" t="s">
+      <c r="D49" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E49" s="199" t="s">
@@ -43085,14 +43069,14 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="329"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C50" s="197">
         <v>0</v>
       </c>
-      <c r="D50" s="198" t="s">
+      <c r="D50" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E50" s="199" t="s">
@@ -43105,7 +43089,7 @@
     <row r="51" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C51" s="197">
         <v>0</v>
@@ -43120,15 +43104,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+    <row r="52" spans="1:6" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="330"/>
       <c r="B52" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C52" s="197">
         <v>0</v>
       </c>
-      <c r="D52" s="200" t="s">
+      <c r="D52" s="331" t="s">
         <v>33</v>
       </c>
       <c r="E52" s="199" t="s">
@@ -43139,14 +43123,14 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="329"/>
       <c r="B53" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C53" s="197">
         <v>0</v>
       </c>
-      <c r="D53" s="200" t="s">
+      <c r="D53" s="198" t="s">
         <v>33</v>
       </c>
       <c r="E53" s="199" t="s">
@@ -43159,7 +43143,7 @@
     <row r="54" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C54" s="197">
         <v>0</v>
@@ -43177,7 +43161,7 @@
     <row r="55" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19"/>
       <c r="B55" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C55" s="197">
         <v>0</v>
@@ -43195,7 +43179,7 @@
     <row r="56" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="196" t="s">
-        <v>885</v>
+        <v>611</v>
       </c>
       <c r="C56" s="197">
         <v>0</v>
@@ -43210,8 +43194,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
+      <c r="B57" s="196" t="s">
+        <v>611</v>
+      </c>
       <c r="C57" s="197">
+        <v>0</v>
+      </c>
+      <c r="D57" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F57" s="539">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
+      <c r="B58" s="196" t="s">
+        <v>611</v>
+      </c>
+      <c r="C58" s="197">
+        <v>0</v>
+      </c>
+      <c r="D58" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F58" s="539">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="19"/>
+      <c r="B59" s="196" t="s">
+        <v>611</v>
+      </c>
+      <c r="C59" s="197">
+        <v>0</v>
+      </c>
+      <c r="D59" s="200" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="199" t="s">
+        <v>611</v>
+      </c>
+      <c r="F59" s="539">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="197">
         <v>0</v>
       </c>
     </row>
@@ -43220,7 +43258,7 @@
     <sortCondition ref="B45:B46"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B44:E44"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0" header="0.31496062992125984" footer="0.21"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -43258,26 +43296,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="663" t="s">
+      <c r="B1" s="662" t="s">
         <v>726</v>
       </c>
-      <c r="C1" s="663"/>
-      <c r="D1" s="663"/>
-      <c r="E1" s="663"/>
-      <c r="H1" s="664" t="s">
+      <c r="C1" s="662"/>
+      <c r="D1" s="662"/>
+      <c r="E1" s="662"/>
+      <c r="H1" s="665" t="s">
         <v>726</v>
       </c>
-      <c r="I1" s="664"/>
-      <c r="J1" s="664"/>
+      <c r="I1" s="665"/>
+      <c r="J1" s="665"/>
       <c r="K1" s="205"/>
       <c r="L1" s="205"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="663" t="s">
+      <c r="O1" s="662" t="s">
         <v>725</v>
       </c>
-      <c r="P1" s="663"/>
+      <c r="P1" s="662"/>
     </row>
     <row r="2" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
@@ -44055,11 +44093,11 @@
         <v>44396</v>
       </c>
       <c r="K21" s="495"/>
-      <c r="L21" s="668">
+      <c r="L21" s="666">
         <f>L16-H37</f>
         <v>-383122.2200000002</v>
       </c>
-      <c r="M21" s="669"/>
+      <c r="M21" s="667"/>
       <c r="O21" s="444">
         <v>0</v>
       </c>
@@ -44093,8 +44131,8 @@
         <v>44397</v>
       </c>
       <c r="K22" s="495"/>
-      <c r="L22" s="670"/>
-      <c r="M22" s="671"/>
+      <c r="L22" s="668"/>
+      <c r="M22" s="669"/>
       <c r="O22" s="444">
         <v>0</v>
       </c>
@@ -44532,8 +44570,8 @@
     </row>
     <row r="40" spans="7:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G40" s="272"/>
-      <c r="H40" s="666"/>
-      <c r="I40" s="666"/>
+      <c r="H40" s="663"/>
+      <c r="I40" s="663"/>
       <c r="O40" s="628" t="s">
         <v>567</v>
       </c>
@@ -44684,7 +44722,7 @@
     </row>
     <row r="53" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G53" s="272"/>
-      <c r="H53" s="667"/>
+      <c r="H53" s="664"/>
       <c r="I53" s="7"/>
       <c r="O53" s="616">
         <f>SUM(O41:O52)</f>
@@ -44695,7 +44733,7 @@
     </row>
     <row r="54" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G54" s="272"/>
-      <c r="H54" s="667"/>
+      <c r="H54" s="664"/>
       <c r="I54" s="7"/>
       <c r="O54" s="617"/>
       <c r="P54" s="475"/>
@@ -44711,8 +44749,8 @@
     </row>
     <row r="56" spans="7:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="G56" s="272"/>
-      <c r="H56" s="666"/>
-      <c r="I56" s="666"/>
+      <c r="H56" s="663"/>
+      <c r="I56" s="663"/>
       <c r="O56" s="618" t="s">
         <v>719</v>
       </c>
@@ -44729,8 +44767,8 @@
     </row>
     <row r="58" spans="7:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="272"/>
-      <c r="H58" s="665"/>
-      <c r="I58" s="665"/>
+      <c r="H58" s="661"/>
+      <c r="I58" s="661"/>
       <c r="O58" s="492">
         <f>O53-O37</f>
         <v>217886.90999999992</v>
@@ -44742,8 +44780,8 @@
     </row>
     <row r="59" spans="7:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="272"/>
-      <c r="H59" s="665"/>
-      <c r="I59" s="665"/>
+      <c r="H59" s="661"/>
+      <c r="I59" s="661"/>
       <c r="O59" s="505">
         <v>-383122.22</v>
       </c>
@@ -44771,18 +44809,14 @@
       <c r="P61" s="506"/>
     </row>
     <row r="62" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="O62" s="661">
+      <c r="O62" s="670">
         <f>SUM(O58:O61)</f>
         <v>-328961.31000000006</v>
       </c>
-      <c r="P62" s="662"/>
+      <c r="P62" s="671"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L21:M22"/>
     <mergeCell ref="O62:P62"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B1:E1"/>
@@ -44799,6 +44833,10 @@
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H53:H54"/>
     <mergeCell ref="H56:I56"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L21:M22"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.13" top="0.43" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 15 NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE ABASTOS  11 SUR   SEPTIEMBRE        2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="17" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="17" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O     2 0 2 1    " sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="REMISIONES  AGOSTO  2021  " sheetId="22" r:id="rId17"/>
     <sheet name="SEPTIEMBRE     2 0 2 1     " sheetId="27" r:id="rId18"/>
     <sheet name="REMISIONES  SEPTIEMBRE 2021 " sheetId="28" r:id="rId19"/>
-    <sheet name="Hoja6" sheetId="29" r:id="rId20"/>
+    <sheet name="pagos de octubre " sheetId="29" r:id="rId20"/>
     <sheet name="Hoja7" sheetId="30" r:id="rId21"/>
     <sheet name="C A N C E L A C I O N E S   " sheetId="5" r:id="rId22"/>
     <sheet name="REPORTE  JUNIO  JULIO  AGOSTO  " sheetId="23" r:id="rId23"/>
@@ -630,7 +630,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2470" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="932">
   <si>
     <t>MORRALLA EN CAJA DE 11 SUR   2,800.00  +  $ 1,200.00 Total    $  4,000.00</t>
   </si>
@@ -3402,6 +3402,30 @@
   </si>
   <si>
     <t>Impuesto Fed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAGO DE ABASTOS DE 4 CARNES  11 SUR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPORTE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transferencia </t>
+  </si>
+  <si>
+    <t>deposito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transferencia </t>
+  </si>
+  <si>
+    <t>depoisto</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deposito </t>
   </si>
 </sst>
 </file>
@@ -3417,7 +3441,7 @@
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="59" x14ac:knownFonts="1">
+  <fonts count="60" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3876,6 +3900,14 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5295,7 +5327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="677">
+  <cellXfs count="689">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6464,26 +6496,44 @@
     <xf numFmtId="16" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="18" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6525,31 +6575,26 @@
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="15" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6564,14 +6609,14 @@
     <xf numFmtId="166" fontId="6" fillId="15" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6590,15 +6635,6 @@
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6678,32 +6714,26 @@
     <xf numFmtId="44" fontId="49" fillId="0" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="8" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6744,28 +6774,37 @@
     <xf numFmtId="44" fontId="16" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="35" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6779,12 +6818,6 @@
     </xf>
     <xf numFmtId="166" fontId="35" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="7" fontId="6" fillId="11" borderId="73" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6810,6 +6843,18 @@
     <xf numFmtId="44" fontId="35" fillId="7" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6824,6 +6869,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="7" fontId="35" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6846,31 +6903,24 @@
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="6" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="18" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="59" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -6880,13 +6930,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF800000"/>
+      <color rgb="FF66FFFF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FF9966FF"/>
-      <color rgb="FF66FFFF"/>
       <color rgb="FFFF3300"/>
       <color rgb="FF00FF00"/>
-      <color rgb="FF800000"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FF990033"/>
       <color rgb="FFFF00FF"/>
@@ -13064,17 +13114,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -13105,17 +13155,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -13144,14 +13194,14 @@
       <c r="D4" s="23">
         <v>44201</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="573" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -15762,61 +15812,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="555"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="556">
         <f>I62+L62</f>
         <v>360753.85</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="557"/>
+      <c r="M64" s="558">
         <f>M62+N62</f>
         <v>2886514.7</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="559"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="566"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2365880.5699999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="561">
+      <c r="P65" s="545">
         <f>P62+Q62</f>
         <v>3321521.28</v>
       </c>
-      <c r="Q65" s="562"/>
+      <c r="Q65" s="546"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="563" t="s">
+      <c r="D66" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="563"/>
+      <c r="E66" s="547"/>
       <c r="F66" s="95">
         <v>-2276696.6800000002</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>344253.98999999964</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="551"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -15850,11 +15900,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-250864.68</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -15878,22 +15928,22 @@
       <c r="C70" s="119">
         <v>44230</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="120">
         <v>209541.1</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="563"/>
+      <c r="K70" s="564">
         <f>K66+K68</f>
         <v>93389.309999999648</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="565"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -15997,11 +16047,11 @@
     <sortCondition ref="J35:J54"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
@@ -16009,11 +16059,11 @@
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="K70:L70"/>
     <mergeCell ref="D65:E65"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.2" right="0.16" top="0.34" bottom="0.32" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -17438,20 +17488,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="615" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -17461,7 +17511,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="616"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -17480,27 +17530,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="598" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="598"/>
+      <c r="AD2" s="598"/>
+      <c r="AE2" s="598"/>
+      <c r="AF2" s="598"/>
+      <c r="AG2" s="598"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -17508,7 +17558,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="586" t="s">
+      <c r="P3" s="588" t="s">
         <v>562</v>
       </c>
       <c r="Q3" s="393"/>
@@ -17521,12 +17571,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="598"/>
+      <c r="AC3" s="598"/>
+      <c r="AD3" s="598"/>
+      <c r="AE3" s="598"/>
+      <c r="AF3" s="598"/>
+      <c r="AG3" s="598"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -17539,14 +17589,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="573" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -17557,7 +17607,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="586"/>
+      <c r="P4" s="588"/>
       <c r="Q4" s="393"/>
       <c r="R4" s="30"/>
       <c r="S4" s="31"/>
@@ -17572,16 +17622,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="599" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="600"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="601" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="601"/>
+      <c r="AG4" s="601"/>
     </row>
     <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
@@ -18993,10 +19043,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="606" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="607"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -19140,11 +19190,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="608" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="609"/>
+      <c r="AG25" s="612">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -19215,9 +19265,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="610"/>
+      <c r="AF26" s="611"/>
+      <c r="AG26" s="613"/>
     </row>
     <row r="27" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
@@ -19392,10 +19442,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="602" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="604">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -19431,11 +19481,11 @@
         <v>0</v>
       </c>
       <c r="O30" s="7"/>
-      <c r="P30" s="587">
+      <c r="P30" s="589">
         <f>SUM(P5:P29)</f>
         <v>-163726</v>
       </c>
-      <c r="Q30" s="587"/>
+      <c r="Q30" s="589"/>
       <c r="R30" s="7">
         <v>0</v>
       </c>
@@ -19449,8 +19499,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="603"/>
+      <c r="AC30" s="605"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -20812,21 +20862,21 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="555"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="556">
         <f>I62+L62</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="557"/>
+      <c r="M64" s="558">
         <f>M62+N62</f>
         <v>2936130</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="559"/>
       <c r="O64" s="367"/>
       <c r="P64" s="367"/>
       <c r="Q64" s="367"/>
@@ -20841,40 +20891,40 @@
       <c r="AG64" s="327"/>
     </row>
     <row r="65" spans="2:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="566"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2702101.7199999997</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="R65" s="561">
+      <c r="R65" s="545">
         <f>R62+S62</f>
         <v>3138957.44</v>
       </c>
-      <c r="S65" s="562"/>
+      <c r="S65" s="546"/>
       <c r="U65" s="50"/>
     </row>
     <row r="66" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="563" t="s">
+      <c r="D66" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="563"/>
+      <c r="E66" s="547"/>
       <c r="F66" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>381077.48999999953</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="551"/>
       <c r="R66" s="50"/>
       <c r="U66" s="107"/>
     </row>
@@ -20908,11 +20958,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="R68" s="50"/>
       <c r="S68" s="7"/>
@@ -20936,22 +20986,22 @@
       <c r="C70" s="119">
         <v>44377</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="563"/>
+      <c r="K70" s="564">
         <f>K66+K68</f>
         <v>125313.09999999951</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="565"/>
       <c r="R70" s="50"/>
       <c r="S70" s="7"/>
       <c r="U70" s="121"/>
@@ -20967,14 +21017,14 @@
       <c r="S71" s="7"/>
     </row>
     <row r="72" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I72" s="588" t="s">
+      <c r="I72" s="590" t="s">
         <v>610</v>
       </c>
-      <c r="J72" s="589"/>
-      <c r="K72" s="592">
+      <c r="J72" s="591"/>
+      <c r="K72" s="594">
         <v>163726</v>
       </c>
-      <c r="L72" s="593"/>
+      <c r="L72" s="595"/>
       <c r="R72" s="7"/>
       <c r="S72" s="7"/>
     </row>
@@ -20983,10 +21033,10 @@
       <c r="C73" s="128"/>
       <c r="D73" s="129"/>
       <c r="E73" s="7"/>
-      <c r="I73" s="590"/>
-      <c r="J73" s="591"/>
-      <c r="K73" s="594"/>
-      <c r="L73" s="595"/>
+      <c r="I73" s="592"/>
+      <c r="J73" s="593"/>
+      <c r="K73" s="596"/>
+      <c r="L73" s="597"/>
       <c r="M73" s="2"/>
       <c r="N73" s="60"/>
       <c r="O73" s="165"/>
@@ -21038,7 +21088,7 @@
       <c r="C76" s="130"/>
       <c r="E76" s="7"/>
       <c r="M76" s="4"/>
-      <c r="AC76" s="585"/>
+      <c r="AC76" s="614"/>
       <c r="AD76" s="342"/>
       <c r="AE76" s="342"/>
       <c r="AF76" s="342"/>
@@ -21051,7 +21101,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="273"/>
       <c r="M77" s="4"/>
-      <c r="AC77" s="585"/>
+      <c r="AC77" s="614"/>
       <c r="AD77" s="342"/>
       <c r="AE77" s="342"/>
       <c r="AF77" s="342"/>
@@ -21145,6 +21195,22 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AC76:AC77"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="I72:J73"/>
@@ -21160,22 +21226,6 @@
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
-    <mergeCell ref="AC76:AC77"/>
-    <mergeCell ref="R65:S65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.49" right="0.23622047244094491" top="0.47244094488188981" bottom="0.27559055118110237" header="0.70866141732283472" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22513,25 +22563,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="615" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="616"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -22541,27 +22591,27 @@
       <c r="L2" s="12"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="Q2" s="596" t="s">
+      <c r="Q2" s="598" t="s">
         <v>596</v>
       </c>
-      <c r="R2" s="596"/>
-      <c r="S2" s="596"/>
-      <c r="T2" s="596"/>
-      <c r="U2" s="596"/>
-      <c r="V2" s="596"/>
+      <c r="R2" s="598"/>
+      <c r="S2" s="598"/>
+      <c r="T2" s="598"/>
+      <c r="U2" s="598"/>
+      <c r="V2" s="598"/>
     </row>
     <row r="3" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -22569,12 +22619,12 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="Q3" s="596"/>
-      <c r="R3" s="596"/>
-      <c r="S3" s="596"/>
-      <c r="T3" s="596"/>
-      <c r="U3" s="596"/>
-      <c r="V3" s="596"/>
+      <c r="Q3" s="598"/>
+      <c r="R3" s="598"/>
+      <c r="S3" s="598"/>
+      <c r="T3" s="598"/>
+      <c r="U3" s="598"/>
+      <c r="V3" s="598"/>
     </row>
     <row r="4" spans="1:23" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -22587,14 +22637,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="573" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -22606,16 +22656,16 @@
       </c>
       <c r="O4" s="365"/>
       <c r="P4" s="29"/>
-      <c r="Q4" s="597" t="s">
+      <c r="Q4" s="599" t="s">
         <v>527</v>
       </c>
-      <c r="R4" s="598"/>
+      <c r="R4" s="600"/>
       <c r="S4" s="99"/>
-      <c r="T4" s="599" t="s">
+      <c r="T4" s="601" t="s">
         <v>567</v>
       </c>
-      <c r="U4" s="599"/>
-      <c r="V4" s="599"/>
+      <c r="U4" s="601"/>
+      <c r="V4" s="601"/>
       <c r="W4" s="99"/>
     </row>
     <row r="5" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23614,10 +23664,10 @@
         <v>0</v>
       </c>
       <c r="S23" s="99"/>
-      <c r="T23" s="604" t="s">
+      <c r="T23" s="606" t="s">
         <v>564</v>
       </c>
-      <c r="U23" s="605"/>
+      <c r="U23" s="607"/>
       <c r="V23" s="339">
         <f>SUM(V6:V22)</f>
         <v>2323600</v>
@@ -23721,11 +23771,11 @@
         <v>138607</v>
       </c>
       <c r="S25" s="99"/>
-      <c r="T25" s="606" t="s">
+      <c r="T25" s="608" t="s">
         <v>565</v>
       </c>
-      <c r="U25" s="607"/>
-      <c r="V25" s="610">
+      <c r="U25" s="609"/>
+      <c r="V25" s="612">
         <f>R29-V23</f>
         <v>163726</v>
       </c>
@@ -23774,9 +23824,9 @@
         <v>107480</v>
       </c>
       <c r="S26" s="99"/>
-      <c r="T26" s="608"/>
-      <c r="U26" s="609"/>
-      <c r="V26" s="611"/>
+      <c r="T26" s="610"/>
+      <c r="U26" s="611"/>
+      <c r="V26" s="613"/>
       <c r="W26" s="99"/>
     </row>
     <row r="27" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23899,10 +23949,10 @@
       </c>
       <c r="O29" s="7"/>
       <c r="P29" s="29"/>
-      <c r="Q29" s="600" t="s">
+      <c r="Q29" s="602" t="s">
         <v>562</v>
       </c>
-      <c r="R29" s="602">
+      <c r="R29" s="604">
         <f>SUM(R5:R28)</f>
         <v>2487326</v>
       </c>
@@ -23939,8 +23989,8 @@
       </c>
       <c r="O30" s="7"/>
       <c r="P30" s="373"/>
-      <c r="Q30" s="601"/>
-      <c r="R30" s="603"/>
+      <c r="Q30" s="603"/>
+      <c r="R30" s="605"/>
       <c r="S30" s="99"/>
       <c r="T30" s="99"/>
       <c r="U30" s="99"/>
@@ -24565,21 +24615,21 @@
       <c r="A50" s="60"/>
       <c r="B50" s="100"/>
       <c r="C50" s="4"/>
-      <c r="H50" s="548" t="s">
+      <c r="H50" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="549"/>
+      <c r="I50" s="555"/>
       <c r="J50" s="101"/>
-      <c r="K50" s="550">
+      <c r="K50" s="556">
         <f>I48+L48</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L50" s="551"/>
-      <c r="M50" s="552">
+      <c r="L50" s="557"/>
+      <c r="M50" s="558">
         <f>M48+N48</f>
         <v>612530</v>
       </c>
-      <c r="N50" s="553"/>
+      <c r="N50" s="559"/>
       <c r="O50" s="367"/>
       <c r="P50" s="102"/>
       <c r="Q50" s="320"/>
@@ -24591,10 +24641,10 @@
       <c r="W50" s="327"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D51" s="560" t="s">
+      <c r="D51" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="560"/>
+      <c r="E51" s="566"/>
       <c r="F51" s="103">
         <f>F48-K50-C48</f>
         <v>2702101.7199999997</v>
@@ -24603,22 +24653,22 @@
       <c r="J51" s="105"/>
     </row>
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D52" s="563" t="s">
+      <c r="D52" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E52" s="563"/>
+      <c r="E52" s="547"/>
       <c r="F52" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I52" s="564" t="s">
+      <c r="I52" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J52" s="565"/>
-      <c r="K52" s="566">
+      <c r="J52" s="549"/>
+      <c r="K52" s="550">
         <f>F54+F55+F56</f>
         <v>381077.72999999952</v>
       </c>
-      <c r="L52" s="567"/>
+      <c r="L52" s="551"/>
     </row>
     <row r="53" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="108"/>
@@ -24647,11 +24697,11 @@
         <v>21</v>
       </c>
       <c r="J54" s="115"/>
-      <c r="K54" s="568">
+      <c r="K54" s="552">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L54" s="569"/>
+      <c r="L54" s="553"/>
       <c r="M54" s="116"/>
     </row>
     <row r="55" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24669,22 +24719,22 @@
       <c r="C56" s="119">
         <v>44377</v>
       </c>
-      <c r="D56" s="554" t="s">
+      <c r="D56" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="555"/>
+      <c r="E56" s="561"/>
       <c r="F56" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I56" s="556" t="s">
+      <c r="I56" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J56" s="557"/>
-      <c r="K56" s="558">
+      <c r="J56" s="563"/>
+      <c r="K56" s="564">
         <f>K52+K54</f>
         <v>125313.3399999995</v>
       </c>
-      <c r="L56" s="559"/>
+      <c r="L56" s="565"/>
     </row>
     <row r="57" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C57" s="122"/>
@@ -24740,7 +24790,7 @@
       <c r="C62" s="130"/>
       <c r="E62" s="7"/>
       <c r="M62" s="4"/>
-      <c r="R62" s="585"/>
+      <c r="R62" s="614"/>
       <c r="S62" s="379"/>
       <c r="T62" s="379"/>
       <c r="U62" s="379"/>
@@ -24753,7 +24803,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="273"/>
       <c r="M63" s="4"/>
-      <c r="R63" s="585"/>
+      <c r="R63" s="614"/>
       <c r="S63" s="379"/>
       <c r="T63" s="379"/>
       <c r="U63" s="379"/>
@@ -24830,6 +24880,23 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="Q2:V3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T25:U26"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="Q29:Q30"/>
+    <mergeCell ref="R29:R30"/>
     <mergeCell ref="R62:R63"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
@@ -24839,23 +24906,6 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="I56:J56"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T25:U26"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="Q29:Q30"/>
-    <mergeCell ref="R29:R30"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="Q2:V3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24909,20 +24959,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="615" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -24932,7 +24982,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="616"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -24951,27 +25001,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="598" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="598"/>
+      <c r="AD2" s="598"/>
+      <c r="AE2" s="598"/>
+      <c r="AF2" s="598"/>
+      <c r="AG2" s="598"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -24979,13 +25029,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="634" t="s">
+      <c r="P3" s="617" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="636" t="s">
+      <c r="Q3" s="619" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="637"/>
+      <c r="S3" s="620"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -24995,12 +25045,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="598"/>
+      <c r="AC3" s="598"/>
+      <c r="AD3" s="598"/>
+      <c r="AE3" s="598"/>
+      <c r="AF3" s="598"/>
+      <c r="AG3" s="598"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -25013,14 +25063,14 @@
       <c r="D4" s="23">
         <v>44377</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="635" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="618" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -25031,10 +25081,10 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="634"/>
-      <c r="Q4" s="636"/>
+      <c r="P4" s="617"/>
+      <c r="Q4" s="619"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="637"/>
+      <c r="S4" s="620"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -25046,16 +25096,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="599" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="600"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="601" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="601"/>
+      <c r="AG4" s="601"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -26492,10 +26542,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="606" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="607"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -26627,11 +26677,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="608" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="609"/>
+      <c r="AG25" s="612">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -26700,9 +26750,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="610"/>
+      <c r="AF26" s="611"/>
+      <c r="AG26" s="613"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -26901,10 +26951,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="602" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="604">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -26967,8 +27017,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="603"/>
+      <c r="AC30" s="605"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -28721,16 +28771,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="548" t="s">
+      <c r="H69" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="549"/>
+      <c r="I69" s="555"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="550">
+      <c r="K69" s="556">
         <f>I67+L67</f>
         <v>587206.12</v>
       </c>
-      <c r="L69" s="551"/>
+      <c r="L69" s="557"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="367"/>
@@ -28747,40 +28797,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="560" t="s">
+      <c r="D70" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="560"/>
+      <c r="E70" s="566"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>3436910.52</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="561">
+      <c r="R70" s="545">
         <f>R67+S67</f>
         <v>10503773.959999999</v>
       </c>
-      <c r="S70" s="562"/>
+      <c r="S70" s="546"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="563" t="s">
+      <c r="D71" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="563"/>
+      <c r="E71" s="547"/>
       <c r="F71" s="95">
         <v>-3290264.27</v>
       </c>
-      <c r="I71" s="564" t="s">
+      <c r="I71" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="565"/>
-      <c r="K71" s="566">
+      <c r="J71" s="549"/>
+      <c r="K71" s="550">
         <f>F73+F74+F75</f>
         <v>426565.1</v>
       </c>
-      <c r="L71" s="567"/>
+      <c r="L71" s="551"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -28814,11 +28864,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="568">
+      <c r="K73" s="552">
         <f>-C4</f>
         <v>-308642.71999999997</v>
       </c>
-      <c r="L73" s="612"/>
+      <c r="L73" s="634"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -28841,22 +28891,22 @@
       <c r="C75" s="119">
         <v>44410</v>
       </c>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="561"/>
       <c r="F75" s="120">
         <v>250140.85</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="563"/>
+      <c r="K75" s="564">
         <f>K71+K73</f>
         <v>117922.38</v>
       </c>
-      <c r="L75" s="558"/>
+      <c r="L75" s="564"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -28871,14 +28921,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="613" t="s">
+      <c r="I77" s="635" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="614"/>
-      <c r="K77" s="617">
+      <c r="J77" s="636"/>
+      <c r="K77" s="639">
         <v>-383122.22</v>
       </c>
-      <c r="L77" s="618"/>
+      <c r="L77" s="640"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -28887,10 +28937,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="615"/>
-      <c r="J78" s="616"/>
-      <c r="K78" s="619"/>
-      <c r="L78" s="620"/>
+      <c r="I78" s="637"/>
+      <c r="J78" s="638"/>
+      <c r="K78" s="641"/>
+      <c r="L78" s="642"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="165"/>
@@ -28942,7 +28992,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="585"/>
+      <c r="AC81" s="614"/>
       <c r="AD81" s="440"/>
       <c r="AE81" s="440"/>
       <c r="AF81" s="440"/>
@@ -28955,7 +29005,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="585"/>
+      <c r="AC82" s="614"/>
       <c r="AD82" s="440"/>
       <c r="AE82" s="440"/>
       <c r="AF82" s="440"/>
@@ -29049,6 +29099,28 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AE25:AF26"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="M57:M58"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="M62:N63"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="M44:N44"/>
     <mergeCell ref="AG25:AG26"/>
     <mergeCell ref="AB29:AB30"/>
     <mergeCell ref="AC29:AC30"/>
@@ -29064,28 +29136,6 @@
     <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AE25:AF26"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="M57:M58"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M62:N63"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.27559055118110237" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30768,20 +30818,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="615" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>721</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -30791,7 +30841,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="616"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -30810,27 +30860,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="598" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="598"/>
+      <c r="AD2" s="598"/>
+      <c r="AE2" s="598"/>
+      <c r="AF2" s="598"/>
+      <c r="AG2" s="598"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -30841,13 +30891,13 @@
       <c r="O3" s="366" t="s">
         <v>753</v>
       </c>
-      <c r="P3" s="634" t="s">
+      <c r="P3" s="617" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="636" t="s">
+      <c r="Q3" s="619" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="637"/>
+      <c r="S3" s="620"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -30857,12 +30907,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="598"/>
+      <c r="AC3" s="598"/>
+      <c r="AD3" s="598"/>
+      <c r="AE3" s="598"/>
+      <c r="AF3" s="598"/>
+      <c r="AG3" s="598"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -30875,14 +30925,14 @@
       <c r="D4" s="23">
         <v>44411</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="635" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="618" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -30893,10 +30943,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="634"/>
-      <c r="Q4" s="636"/>
+      <c r="P4" s="617"/>
+      <c r="Q4" s="619"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="637"/>
+      <c r="S4" s="620"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -30908,16 +30958,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="599" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="600"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="601" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="601"/>
+      <c r="AG4" s="601"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -32405,10 +32455,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="606" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="607"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -32548,11 +32598,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="608" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="609"/>
+      <c r="AG25" s="612">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -32624,9 +32674,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="610"/>
+      <c r="AF26" s="611"/>
+      <c r="AG26" s="613"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -32836,10 +32886,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="602" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="604">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -32904,8 +32954,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="603"/>
+      <c r="AC30" s="605"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -34388,11 +34438,11 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="642">
+      <c r="M62" s="645">
         <f>M39-M58</f>
         <v>37331</v>
       </c>
-      <c r="N62" s="643"/>
+      <c r="N62" s="646"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -34424,8 +34474,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="644"/>
-      <c r="N63" s="645"/>
+      <c r="M63" s="647"/>
+      <c r="N63" s="648"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -34457,10 +34507,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="648">
+      <c r="M64" s="649">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="649"/>
+      <c r="N64" s="650"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -34491,10 +34541,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="650">
+      <c r="M65" s="651">
         <v>-163726</v>
       </c>
-      <c r="N65" s="651"/>
+      <c r="N65" s="652"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -34525,12 +34575,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="652">
+      <c r="M66" s="653">
         <f>SUM(M65+M64+M62)</f>
         <v>-509117.22</v>
       </c>
-      <c r="N66" s="653"/>
-      <c r="O66" s="646" t="s">
+      <c r="N66" s="654"/>
+      <c r="O66" s="643" t="s">
         <v>821</v>
       </c>
       <c r="P66" s="7"/>
@@ -34584,9 +34634,9 @@
         <f>SUM(L5:L66)</f>
         <v>482695.31000000006</v>
       </c>
-      <c r="M67" s="654"/>
-      <c r="N67" s="655"/>
-      <c r="O67" s="647"/>
+      <c r="M67" s="655"/>
+      <c r="N67" s="656"/>
+      <c r="O67" s="644"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
@@ -34618,16 +34668,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="548" t="s">
+      <c r="H69" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="549"/>
+      <c r="I69" s="555"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="550">
+      <c r="K69" s="556">
         <f>I67+L67</f>
         <v>518841.31000000006</v>
       </c>
-      <c r="L69" s="551"/>
+      <c r="L69" s="557"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="489"/>
@@ -34644,40 +34694,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="560" t="s">
+      <c r="D70" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="560"/>
+      <c r="E70" s="566"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>2539226.3499999996</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="561">
+      <c r="R70" s="545">
         <f>R67+S67</f>
         <v>7378939.6599999992</v>
       </c>
-      <c r="S70" s="562"/>
+      <c r="S70" s="546"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="563" t="s">
+      <c r="D71" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="563"/>
+      <c r="E71" s="547"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="564" t="s">
+      <c r="I71" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="565"/>
-      <c r="K71" s="566">
+      <c r="J71" s="549"/>
+      <c r="K71" s="550">
         <f>F73+F74+F75</f>
         <v>536310.85999999964</v>
       </c>
-      <c r="L71" s="567"/>
+      <c r="L71" s="551"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -34711,11 +34761,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="568">
+      <c r="K73" s="552">
         <f>-C4</f>
         <v>-250140.85</v>
       </c>
-      <c r="L73" s="612"/>
+      <c r="L73" s="634"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -34738,22 +34788,22 @@
       <c r="C75" s="119">
         <v>44439</v>
       </c>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="561"/>
       <c r="F75" s="120">
         <v>365611.59</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="563"/>
+      <c r="K75" s="564">
         <f>K71+K73</f>
         <v>286170.00999999966</v>
       </c>
-      <c r="L75" s="558"/>
+      <c r="L75" s="564"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -34768,14 +34818,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="638" t="s">
+      <c r="I77" s="657" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="639"/>
-      <c r="K77" s="642">
+      <c r="J77" s="658"/>
+      <c r="K77" s="645">
         <v>37331</v>
       </c>
-      <c r="L77" s="643"/>
+      <c r="L77" s="646"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -34784,10 +34834,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="640"/>
-      <c r="J78" s="641"/>
-      <c r="K78" s="644"/>
-      <c r="L78" s="645"/>
+      <c r="I78" s="659"/>
+      <c r="J78" s="660"/>
+      <c r="K78" s="647"/>
+      <c r="L78" s="648"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -34839,7 +34889,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="585"/>
+      <c r="AC81" s="614"/>
       <c r="AD81" s="486"/>
       <c r="AE81" s="486"/>
       <c r="AF81" s="486"/>
@@ -34852,7 +34902,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="585"/>
+      <c r="AC82" s="614"/>
       <c r="AD82" s="486"/>
       <c r="AE82" s="486"/>
       <c r="AF82" s="486"/>
@@ -34949,6 +34999,30 @@
     <sortCondition ref="N45:N55"/>
   </sortState>
   <mergeCells count="39">
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="M62:N63"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N67"/>
+    <mergeCell ref="M44:N44"/>
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
@@ -34964,30 +35038,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="M62:N63"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M66:N67"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36527,8 +36577,8 @@
   </sheetPr>
   <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36563,20 +36613,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="615" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>836</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -36586,7 +36636,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="616"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -36605,27 +36655,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="596" t="s">
+      <c r="AB2" s="598" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="596"/>
-      <c r="AD2" s="596"/>
-      <c r="AE2" s="596"/>
-      <c r="AF2" s="596"/>
-      <c r="AG2" s="596"/>
+      <c r="AC2" s="598"/>
+      <c r="AD2" s="598"/>
+      <c r="AE2" s="598"/>
+      <c r="AF2" s="598"/>
+      <c r="AG2" s="598"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -36633,13 +36683,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="634" t="s">
+      <c r="P3" s="617" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="636" t="s">
+      <c r="Q3" s="619" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="637" t="s">
+      <c r="S3" s="620" t="s">
         <v>868</v>
       </c>
       <c r="W3" s="213" t="s">
@@ -36651,12 +36701,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="596"/>
-      <c r="AC3" s="596"/>
-      <c r="AD3" s="596"/>
-      <c r="AE3" s="596"/>
-      <c r="AF3" s="596"/>
-      <c r="AG3" s="596"/>
+      <c r="AB3" s="598"/>
+      <c r="AC3" s="598"/>
+      <c r="AD3" s="598"/>
+      <c r="AE3" s="598"/>
+      <c r="AF3" s="598"/>
+      <c r="AG3" s="598"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -36669,14 +36719,14 @@
       <c r="D4" s="23">
         <v>44439</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="635" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="618" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -36687,10 +36737,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="634"/>
-      <c r="Q4" s="636"/>
+      <c r="P4" s="617"/>
+      <c r="Q4" s="619"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="637"/>
+      <c r="S4" s="620"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -36702,16 +36752,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="597" t="s">
+      <c r="AB4" s="599" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="598"/>
+      <c r="AC4" s="600"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="599" t="s">
+      <c r="AE4" s="601" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="599"/>
-      <c r="AG4" s="599"/>
+      <c r="AF4" s="601"/>
+      <c r="AG4" s="601"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -38182,10 +38232,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="604" t="s">
+      <c r="AE23" s="606" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="605"/>
+      <c r="AF23" s="607"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -38321,11 +38371,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="606" t="s">
+      <c r="AE25" s="608" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="607"/>
-      <c r="AG25" s="610">
+      <c r="AF25" s="609"/>
+      <c r="AG25" s="612">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -38395,9 +38445,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="608"/>
-      <c r="AF26" s="609"/>
-      <c r="AG26" s="611"/>
+      <c r="AE26" s="610"/>
+      <c r="AF26" s="611"/>
+      <c r="AG26" s="613"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -38599,10 +38649,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="600" t="s">
+      <c r="AB29" s="602" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="602">
+      <c r="AC29" s="604">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -38665,8 +38715,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="601"/>
-      <c r="AC30" s="603"/>
+      <c r="AB30" s="603"/>
+      <c r="AC30" s="605"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -39399,7 +39449,7 @@
       <c r="B44" s="353">
         <v>44460</v>
       </c>
-      <c r="C44" s="672">
+      <c r="C44" s="540">
         <v>20001.48</v>
       </c>
       <c r="D44" s="237" t="s">
@@ -39413,7 +39463,7 @@
       <c r="J44" s="299" t="s">
         <v>913</v>
       </c>
-      <c r="K44" s="675"/>
+      <c r="K44" s="543"/>
       <c r="L44" s="71">
         <v>33333.69</v>
       </c>
@@ -39808,7 +39858,7 @@
       <c r="C53" s="71">
         <v>10632</v>
       </c>
-      <c r="D53" s="673" t="s">
+      <c r="D53" s="541" t="s">
         <v>917</v>
       </c>
       <c r="E53" s="136"/>
@@ -39821,7 +39871,7 @@
       <c r="J53" s="299" t="s">
         <v>913</v>
       </c>
-      <c r="K53" s="676"/>
+      <c r="K53" s="544"/>
       <c r="L53" s="75">
         <v>32341</v>
       </c>
@@ -39854,7 +39904,7 @@
       <c r="C54" s="71">
         <v>545650</v>
       </c>
-      <c r="D54" s="674" t="s">
+      <c r="D54" s="542" t="s">
         <v>915</v>
       </c>
       <c r="E54" s="136"/>
@@ -40010,7 +40060,7 @@
       <c r="J58" s="528"/>
       <c r="K58" s="468"/>
       <c r="L58" s="50"/>
-      <c r="M58" s="656">
+      <c r="M58" s="661">
         <f t="shared" ref="M58" si="2">SUM(M45:M57)</f>
         <v>0</v>
       </c>
@@ -40044,7 +40094,7 @@
       <c r="J59" s="528"/>
       <c r="K59" s="243"/>
       <c r="L59" s="50"/>
-      <c r="M59" s="657"/>
+      <c r="M59" s="662"/>
       <c r="N59" s="42"/>
       <c r="O59" s="392"/>
       <c r="P59" s="7"/>
@@ -40139,10 +40189,10 @@
       <c r="J62" s="325"/>
       <c r="K62" s="359"/>
       <c r="L62" s="458"/>
-      <c r="M62" s="642">
+      <c r="M62" s="645">
         <v>-37331</v>
       </c>
-      <c r="N62" s="643"/>
+      <c r="N62" s="646"/>
       <c r="O62" s="392"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -40174,8 +40224,8 @@
       <c r="L63" s="50" t="s">
         <v>820</v>
       </c>
-      <c r="M63" s="644"/>
-      <c r="N63" s="645"/>
+      <c r="M63" s="647"/>
+      <c r="N63" s="648"/>
       <c r="O63" s="392"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -40207,10 +40257,10 @@
       <c r="L64" s="521" t="s">
         <v>818</v>
       </c>
-      <c r="M64" s="648">
+      <c r="M64" s="649">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="649"/>
+      <c r="N64" s="650"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -40241,10 +40291,10 @@
       <c r="L65" s="521" t="s">
         <v>819</v>
       </c>
-      <c r="M65" s="650">
+      <c r="M65" s="651">
         <v>-163726</v>
       </c>
-      <c r="N65" s="651"/>
+      <c r="N65" s="652"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -40275,12 +40325,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="652">
+      <c r="M66" s="653">
         <f>SUM(M65+M64+M62)</f>
         <v>-583779.22</v>
       </c>
-      <c r="N66" s="653"/>
-      <c r="O66" s="646"/>
+      <c r="N66" s="654"/>
+      <c r="O66" s="643"/>
       <c r="P66" s="7"/>
       <c r="Q66" s="7"/>
       <c r="R66" s="84">
@@ -40332,9 +40382,9 @@
         <f>SUM(L5:L66)</f>
         <v>538164.65</v>
       </c>
-      <c r="M67" s="654"/>
-      <c r="N67" s="655"/>
-      <c r="O67" s="647"/>
+      <c r="M67" s="655"/>
+      <c r="N67" s="656"/>
+      <c r="O67" s="644"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
@@ -40366,16 +40416,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="548" t="s">
+      <c r="H69" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="549"/>
+      <c r="I69" s="555"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="550">
+      <c r="K69" s="556">
         <f>I67+L67</f>
         <v>582925.65</v>
       </c>
-      <c r="L69" s="551"/>
+      <c r="L69" s="557"/>
       <c r="M69" s="470"/>
       <c r="N69" s="471"/>
       <c r="O69" s="489"/>
@@ -40392,40 +40442,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="560" t="s">
+      <c r="D70" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="560"/>
+      <c r="E70" s="566"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>1982428.1</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="561">
+      <c r="R70" s="545">
         <f>R67+S67</f>
         <v>8037614.7599999998</v>
       </c>
-      <c r="S70" s="562"/>
+      <c r="S70" s="546"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="563" t="s">
+      <c r="D71" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="563"/>
+      <c r="E71" s="547"/>
       <c r="F71" s="95">
         <v>-1915029.61</v>
       </c>
-      <c r="I71" s="564" t="s">
+      <c r="I71" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="565"/>
-      <c r="K71" s="566">
+      <c r="J71" s="549"/>
+      <c r="K71" s="550">
         <f>F73+F74+F75</f>
         <v>67398.489999999991</v>
       </c>
-      <c r="L71" s="567"/>
+      <c r="L71" s="551"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -40459,11 +40509,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="568">
+      <c r="K73" s="552">
         <f>-C4</f>
         <v>-365611.59</v>
       </c>
-      <c r="L73" s="612"/>
+      <c r="L73" s="634"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -40484,22 +40534,22 @@
     </row>
     <row r="75" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="119"/>
-      <c r="D75" s="554" t="s">
+      <c r="D75" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="555"/>
+      <c r="E75" s="561"/>
       <c r="F75" s="120">
         <v>0</v>
       </c>
-      <c r="I75" s="556" t="s">
+      <c r="I75" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="557"/>
-      <c r="K75" s="558">
+      <c r="J75" s="563"/>
+      <c r="K75" s="564">
         <f>K71+K73</f>
         <v>-298213.10000000003</v>
       </c>
-      <c r="L75" s="558"/>
+      <c r="L75" s="564"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -40514,14 +40564,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="638" t="s">
+      <c r="I77" s="657" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="639"/>
-      <c r="K77" s="642">
-        <v>0</v>
-      </c>
-      <c r="L77" s="643"/>
+      <c r="J77" s="658"/>
+      <c r="K77" s="645">
+        <v>0</v>
+      </c>
+      <c r="L77" s="646"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -40530,10 +40580,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="640"/>
-      <c r="J78" s="641"/>
-      <c r="K78" s="644"/>
-      <c r="L78" s="645"/>
+      <c r="I78" s="659"/>
+      <c r="J78" s="660"/>
+      <c r="K78" s="647"/>
+      <c r="L78" s="648"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="490"/>
@@ -40585,7 +40635,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="585"/>
+      <c r="AC81" s="614"/>
       <c r="AD81" s="526"/>
       <c r="AE81" s="526"/>
       <c r="AF81" s="526"/>
@@ -40598,7 +40648,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="585"/>
+      <c r="AC82" s="614"/>
       <c r="AD82" s="526"/>
       <c r="AE82" s="526"/>
       <c r="AF82" s="526"/>
@@ -40692,24 +40742,16 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="AB2:AG3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="M62:N63"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AE4:AG4"/>
@@ -40723,16 +40765,24 @@
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="M58:M59"/>
     <mergeCell ref="M60:N60"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="AB2:AG3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40748,7 +40798,7 @@
   </sheetPr>
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
@@ -43294,12 +43344,283 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="683"/>
+    <col min="4" max="4" width="20.7109375" style="126" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="682"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="685"/>
+      <c r="B2" s="688" t="s">
+        <v>924</v>
+      </c>
+      <c r="C2" s="685"/>
+      <c r="D2" s="686"/>
+      <c r="E2" s="687"/>
+    </row>
+    <row r="3" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="684" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="677"/>
+      <c r="D3" s="678" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="683">
+        <v>44477</v>
+      </c>
+      <c r="D4" s="126">
+        <v>400408</v>
+      </c>
+      <c r="E4" s="682" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="682" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="683">
+        <v>44484</v>
+      </c>
+      <c r="D6" s="126">
+        <v>140990</v>
+      </c>
+      <c r="E6" s="682" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="683">
+        <v>44484</v>
+      </c>
+      <c r="D7" s="680">
+        <v>160000</v>
+      </c>
+      <c r="E7" s="682" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="679">
+        <f>SUM(D6:D7)</f>
+        <v>300990</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="683">
+        <v>44491</v>
+      </c>
+      <c r="D10" s="126">
+        <v>140990</v>
+      </c>
+      <c r="E10" s="682" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="683">
+        <v>44491</v>
+      </c>
+      <c r="D11" s="126">
+        <v>119215</v>
+      </c>
+      <c r="E11" s="682" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="683">
+        <v>44491</v>
+      </c>
+      <c r="D12" s="680">
+        <v>114795</v>
+      </c>
+      <c r="E12" s="682" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="679">
+        <f>SUM(D10:D12)</f>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="683">
+        <v>44498</v>
+      </c>
+      <c r="D15" s="126">
+        <v>101653</v>
+      </c>
+      <c r="E15" s="682" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="683">
+        <v>44498</v>
+      </c>
+      <c r="D16" s="126">
+        <v>100960</v>
+      </c>
+      <c r="E16" s="682" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="683">
+        <v>44498</v>
+      </c>
+      <c r="D17" s="680">
+        <v>144101</v>
+      </c>
+      <c r="E17" s="682" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="679">
+        <f>SUM(D15:D17)</f>
+        <v>346714</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="683">
+        <v>44505</v>
+      </c>
+      <c r="D20" s="126">
+        <v>135458</v>
+      </c>
+      <c r="E20" s="682" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="683">
+        <v>44505</v>
+      </c>
+      <c r="D21" s="126">
+        <v>106822</v>
+      </c>
+      <c r="E21" s="682" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="683">
+        <v>44505</v>
+      </c>
+      <c r="D22" s="681">
+        <v>182359.5</v>
+      </c>
+      <c r="E22" s="682" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="683">
+        <v>44505</v>
+      </c>
+      <c r="D23" s="680">
+        <v>180000</v>
+      </c>
+      <c r="E23" s="682" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="679">
+        <f>SUM(D20:D23)</f>
+        <v>604639.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="683">
+        <v>44512</v>
+      </c>
+      <c r="D26" s="126">
+        <v>110014</v>
+      </c>
+      <c r="E26" s="682" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="683">
+        <v>44512</v>
+      </c>
+      <c r="D27" s="126">
+        <v>135122</v>
+      </c>
+      <c r="E27" s="682" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="683">
+        <v>44512</v>
+      </c>
+      <c r="D28" s="126">
+        <v>123450</v>
+      </c>
+      <c r="E28" s="682" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="683">
+        <v>44512</v>
+      </c>
+      <c r="D29" s="126">
+        <v>133234</v>
+      </c>
+      <c r="E29" s="682" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="683">
+        <v>44512</v>
+      </c>
+      <c r="D30" s="680">
+        <v>42853.04</v>
+      </c>
+      <c r="E30" s="682" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="679">
+        <f>SUM(D26:D30)</f>
+        <v>544673.04</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -43351,12 +43672,12 @@
     <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="32"/>
-      <c r="B49" s="658" t="s">
+      <c r="B49" s="663" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="659"/>
-      <c r="D49" s="659"/>
-      <c r="E49" s="660"/>
+      <c r="C49" s="664"/>
+      <c r="D49" s="664"/>
+      <c r="E49" s="665"/>
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -43680,32 +44001,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="663" t="s">
+      <c r="B1" s="672" t="s">
         <v>726</v>
       </c>
-      <c r="C1" s="663"/>
-      <c r="D1" s="663"/>
-      <c r="E1" s="663"/>
-      <c r="H1" s="664" t="s">
+      <c r="C1" s="672"/>
+      <c r="D1" s="672"/>
+      <c r="E1" s="672"/>
+      <c r="H1" s="673" t="s">
         <v>726</v>
       </c>
-      <c r="I1" s="664"/>
-      <c r="J1" s="664"/>
+      <c r="I1" s="673"/>
+      <c r="J1" s="673"/>
       <c r="K1" s="205"/>
       <c r="L1" s="205"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="663" t="s">
+      <c r="O1" s="672" t="s">
         <v>725</v>
       </c>
-      <c r="P1" s="663"/>
+      <c r="P1" s="672"/>
     </row>
     <row r="2" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="586" t="s">
+      <c r="E2" s="588" t="s">
         <v>562</v>
       </c>
       <c r="F2" s="496"/>
@@ -43731,7 +44052,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="365"/>
-      <c r="E3" s="586"/>
+      <c r="E3" s="588"/>
       <c r="F3" s="496"/>
       <c r="H3" s="444">
         <v>126476.5</v>
@@ -44477,11 +44798,11 @@
         <v>44396</v>
       </c>
       <c r="K21" s="495"/>
-      <c r="L21" s="668">
+      <c r="L21" s="666">
         <f>L16-H37</f>
         <v>-383122.2200000002</v>
       </c>
-      <c r="M21" s="669"/>
+      <c r="M21" s="667"/>
       <c r="O21" s="444">
         <v>0</v>
       </c>
@@ -44515,8 +44836,8 @@
         <v>44397</v>
       </c>
       <c r="K22" s="495"/>
-      <c r="L22" s="670"/>
-      <c r="M22" s="671"/>
+      <c r="L22" s="668"/>
+      <c r="M22" s="669"/>
       <c r="O22" s="444">
         <v>0</v>
       </c>
@@ -44954,8 +45275,8 @@
     </row>
     <row r="40" spans="7:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G40" s="272"/>
-      <c r="H40" s="666"/>
-      <c r="I40" s="666"/>
+      <c r="H40" s="675"/>
+      <c r="I40" s="675"/>
       <c r="O40" s="633" t="s">
         <v>567</v>
       </c>
@@ -45106,7 +45427,7 @@
     </row>
     <row r="53" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G53" s="272"/>
-      <c r="H53" s="667"/>
+      <c r="H53" s="676"/>
       <c r="I53" s="7"/>
       <c r="O53" s="621">
         <f>SUM(O41:O52)</f>
@@ -45117,7 +45438,7 @@
     </row>
     <row r="54" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G54" s="272"/>
-      <c r="H54" s="667"/>
+      <c r="H54" s="676"/>
       <c r="I54" s="7"/>
       <c r="O54" s="622"/>
       <c r="P54" s="475"/>
@@ -45133,8 +45454,8 @@
     </row>
     <row r="56" spans="7:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="G56" s="272"/>
-      <c r="H56" s="666"/>
-      <c r="I56" s="666"/>
+      <c r="H56" s="675"/>
+      <c r="I56" s="675"/>
       <c r="O56" s="623" t="s">
         <v>719</v>
       </c>
@@ -45151,8 +45472,8 @@
     </row>
     <row r="58" spans="7:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="272"/>
-      <c r="H58" s="665"/>
-      <c r="I58" s="665"/>
+      <c r="H58" s="674"/>
+      <c r="I58" s="674"/>
       <c r="O58" s="492">
         <f>O53-O37</f>
         <v>217886.90999999992</v>
@@ -45164,8 +45485,8 @@
     </row>
     <row r="59" spans="7:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="272"/>
-      <c r="H59" s="665"/>
-      <c r="I59" s="665"/>
+      <c r="H59" s="674"/>
+      <c r="I59" s="674"/>
       <c r="O59" s="505">
         <v>-383122.22</v>
       </c>
@@ -45193,24 +45514,14 @@
       <c r="P61" s="506"/>
     </row>
     <row r="62" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="O62" s="661">
+      <c r="O62" s="670">
         <f>SUM(O58:O61)</f>
         <v>-328961.31000000006</v>
       </c>
-      <c r="P62" s="662"/>
+      <c r="P62" s="671"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L16:L17"/>
     <mergeCell ref="H58:I59"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O37:O38"/>
@@ -45221,6 +45532,16 @@
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H53:H54"/>
     <mergeCell ref="H56:I56"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="O62:P62"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.13" top="0.43" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -45242,12 +45563,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32"/>
-      <c r="B1" s="658" t="s">
+      <c r="B1" s="663" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="659"/>
-      <c r="D1" s="659"/>
-      <c r="E1" s="660"/>
+      <c r="C1" s="664"/>
+      <c r="D1" s="664"/>
+      <c r="E1" s="665"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -45329,12 +45650,12 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32"/>
-      <c r="B9" s="658" t="s">
+      <c r="B9" s="663" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="659"/>
-      <c r="D9" s="659"/>
-      <c r="E9" s="660"/>
+      <c r="C9" s="664"/>
+      <c r="D9" s="664"/>
+      <c r="E9" s="665"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -45490,12 +45811,12 @@
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32"/>
-      <c r="B20" s="658" t="s">
+      <c r="B20" s="663" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="659"/>
-      <c r="D20" s="659"/>
-      <c r="E20" s="660"/>
+      <c r="C20" s="664"/>
+      <c r="D20" s="664"/>
+      <c r="E20" s="665"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -45653,12 +45974,12 @@
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
-      <c r="B31" s="658" t="s">
+      <c r="B31" s="663" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="659"/>
-      <c r="D31" s="659"/>
-      <c r="E31" s="660"/>
+      <c r="C31" s="664"/>
+      <c r="D31" s="664"/>
+      <c r="E31" s="665"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -45812,12 +46133,12 @@
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32"/>
-      <c r="B42" s="658" t="s">
+      <c r="B42" s="663" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="659"/>
-      <c r="D42" s="659"/>
-      <c r="E42" s="660"/>
+      <c r="C42" s="664"/>
+      <c r="D42" s="664"/>
+      <c r="E42" s="665"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -45971,12 +46292,12 @@
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="32"/>
-      <c r="B54" s="658" t="s">
+      <c r="B54" s="663" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="659"/>
-      <c r="D54" s="659"/>
-      <c r="E54" s="660"/>
+      <c r="C54" s="664"/>
+      <c r="D54" s="664"/>
+      <c r="E54" s="665"/>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -46217,17 +46538,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -46258,17 +46579,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -46297,14 +46618,14 @@
       <c r="D4" s="23">
         <v>44230</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="573" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -48843,61 +49164,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="555"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="556">
         <f>I62+L62</f>
         <v>259947.00000000003</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="557"/>
+      <c r="M64" s="558">
         <f>M62+N62</f>
         <v>2744320</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="559"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="566"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2374814.2599999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="561">
+      <c r="P65" s="545">
         <f>P62+Q62</f>
         <v>3144691.75</v>
       </c>
-      <c r="Q65" s="562"/>
+      <c r="Q65" s="546"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="563" t="s">
+      <c r="D66" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="563"/>
+      <c r="E66" s="547"/>
       <c r="F66" s="95">
         <v>-2261593.1</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>355407.6199999997</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="551"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -48934,11 +49255,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-209541.1</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -48962,22 +49283,22 @@
       <c r="C70" s="119">
         <v>44257</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="120">
         <v>223014.26</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="563"/>
+      <c r="K70" s="564">
         <f>K66+K68</f>
         <v>145866.5199999997</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="565"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -49078,12 +49399,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -49095,6 +49410,12 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -50365,17 +50686,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>429</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -50405,17 +50726,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -50444,14 +50765,14 @@
       <c r="D4" s="23">
         <v>44257</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="573" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -53053,61 +53374,61 @@
       <c r="A62" s="60"/>
       <c r="B62" s="100"/>
       <c r="C62" s="4"/>
-      <c r="H62" s="548" t="s">
+      <c r="H62" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="549"/>
+      <c r="I62" s="555"/>
       <c r="J62" s="101"/>
-      <c r="K62" s="550">
+      <c r="K62" s="556">
         <f>I60+L60</f>
         <v>781851.32000000007</v>
       </c>
-      <c r="L62" s="551"/>
-      <c r="M62" s="552">
+      <c r="L62" s="557"/>
+      <c r="M62" s="558">
         <f>M60+N60</f>
         <v>4064802.5</v>
       </c>
-      <c r="N62" s="553"/>
+      <c r="N62" s="559"/>
       <c r="O62" s="102"/>
       <c r="P62" s="99"/>
       <c r="Q62" s="99"/>
       <c r="S62" s="174"/>
     </row>
     <row r="63" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="560" t="s">
+      <c r="D63" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="560"/>
+      <c r="E63" s="566"/>
       <c r="F63" s="103">
         <f>F60-K62-C60</f>
         <v>3177878.1399999997</v>
       </c>
       <c r="I63" s="104"/>
       <c r="J63" s="105"/>
-      <c r="P63" s="561">
+      <c r="P63" s="545">
         <f>P60+Q60</f>
         <v>4585432.34</v>
       </c>
-      <c r="Q63" s="562"/>
+      <c r="Q63" s="546"/>
       <c r="S63" s="50"/>
     </row>
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="563" t="s">
+      <c r="D64" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="563"/>
+      <c r="E64" s="547"/>
       <c r="F64" s="95">
         <v>-3579271.89</v>
       </c>
-      <c r="I64" s="564" t="s">
+      <c r="I64" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J64" s="565"/>
-      <c r="K64" s="566">
+      <c r="J64" s="549"/>
+      <c r="K64" s="550">
         <f>F66+F67+F68</f>
         <v>-110332.85000000047</v>
       </c>
-      <c r="L64" s="567"/>
+      <c r="L64" s="551"/>
       <c r="P64" s="50"/>
       <c r="S64" s="107"/>
     </row>
@@ -53141,11 +53462,11 @@
         <v>21</v>
       </c>
       <c r="J66" s="115"/>
-      <c r="K66" s="568">
+      <c r="K66" s="552">
         <f>-C4</f>
         <v>-223014.26</v>
       </c>
-      <c r="L66" s="569"/>
+      <c r="L66" s="553"/>
       <c r="M66" s="116"/>
       <c r="P66" s="50"/>
       <c r="Q66" s="7"/>
@@ -53169,22 +53490,22 @@
       <c r="C68" s="119">
         <v>44291</v>
       </c>
-      <c r="D68" s="554" t="s">
+      <c r="D68" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="555"/>
+      <c r="E68" s="561"/>
       <c r="F68" s="120">
         <v>215362.9</v>
       </c>
-      <c r="I68" s="570" t="s">
+      <c r="I68" s="575" t="s">
         <v>431</v>
       </c>
-      <c r="J68" s="571"/>
-      <c r="K68" s="572">
+      <c r="J68" s="576"/>
+      <c r="K68" s="577">
         <f>K64+K66</f>
         <v>-333347.11000000045</v>
       </c>
-      <c r="L68" s="573"/>
+      <c r="L68" s="578"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
       <c r="S68" s="121"/>
@@ -53340,12 +53661,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="D63:E63"/>
     <mergeCell ref="P63:Q63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="I64:J64"/>
@@ -53357,6 +53672,12 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H62:I62"/>
     <mergeCell ref="K62:L62"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="D63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -54788,17 +55109,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>430</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -54828,17 +55149,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -54867,14 +55188,14 @@
       <c r="D4" s="23">
         <v>44291</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="573" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="574"/>
+      <c r="I4" s="580"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -57366,61 +57687,61 @@
       <c r="A58" s="60"/>
       <c r="B58" s="100"/>
       <c r="C58" s="4"/>
-      <c r="H58" s="548" t="s">
+      <c r="H58" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I58" s="549"/>
+      <c r="I58" s="555"/>
       <c r="J58" s="101"/>
-      <c r="K58" s="550">
+      <c r="K58" s="556">
         <f>I56+L56</f>
         <v>370346.35000000003</v>
       </c>
-      <c r="L58" s="575"/>
-      <c r="M58" s="552">
+      <c r="L58" s="581"/>
+      <c r="M58" s="558">
         <f>M56+N56</f>
         <v>3537422</v>
       </c>
-      <c r="N58" s="553"/>
+      <c r="N58" s="559"/>
       <c r="O58" s="102"/>
       <c r="P58" s="99"/>
       <c r="Q58" s="99"/>
       <c r="S58" s="174"/>
     </row>
     <row r="59" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="560" t="s">
+      <c r="D59" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="576"/>
+      <c r="E59" s="579"/>
       <c r="F59" s="103">
         <f>F56-K58-C56</f>
         <v>3048717.54</v>
       </c>
       <c r="I59" s="104"/>
       <c r="J59" s="105"/>
-      <c r="P59" s="561">
+      <c r="P59" s="545">
         <f>P56+Q56</f>
         <v>8073324.3200000003</v>
       </c>
-      <c r="Q59" s="562"/>
+      <c r="Q59" s="546"/>
       <c r="S59" s="50"/>
     </row>
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="563" t="s">
+      <c r="D60" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="563"/>
+      <c r="E60" s="547"/>
       <c r="F60" s="95">
         <v>-3102716.28</v>
       </c>
-      <c r="I60" s="564" t="s">
+      <c r="I60" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J60" s="565"/>
-      <c r="K60" s="566">
+      <c r="J60" s="549"/>
+      <c r="K60" s="550">
         <f>F62+F63+F64</f>
         <v>216465.62000000023</v>
       </c>
-      <c r="L60" s="567"/>
+      <c r="L60" s="551"/>
       <c r="P60" s="50"/>
       <c r="S60" s="107"/>
     </row>
@@ -57454,11 +57775,11 @@
         <v>21</v>
       </c>
       <c r="J62" s="115"/>
-      <c r="K62" s="568">
+      <c r="K62" s="552">
         <f>-C4</f>
         <v>-215362.9</v>
       </c>
-      <c r="L62" s="569"/>
+      <c r="L62" s="553"/>
       <c r="M62" s="116"/>
       <c r="P62" s="50"/>
       <c r="Q62" s="7"/>
@@ -57482,22 +57803,22 @@
       <c r="C64" s="119">
         <v>44320</v>
       </c>
-      <c r="D64" s="554" t="s">
+      <c r="D64" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="555"/>
+      <c r="E64" s="561"/>
       <c r="F64" s="120">
         <v>249311.35999999999</v>
       </c>
-      <c r="I64" s="556" t="s">
+      <c r="I64" s="562" t="s">
         <v>25</v>
       </c>
-      <c r="J64" s="557"/>
-      <c r="K64" s="558">
+      <c r="J64" s="563"/>
+      <c r="K64" s="564">
         <f>K60+K62</f>
         <v>1102.720000000234</v>
       </c>
-      <c r="L64" s="559"/>
+      <c r="L64" s="565"/>
       <c r="P64" s="50"/>
       <c r="Q64" s="7"/>
       <c r="S64" s="121"/>
@@ -57653,12 +57974,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="D59:E59"/>
     <mergeCell ref="P59:Q59"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="I60:J60"/>
@@ -57670,6 +57985,12 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -58552,17 +58873,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="540" t="s">
+      <c r="C1" s="567" t="s">
         <v>504</v>
       </c>
-      <c r="D1" s="540"/>
-      <c r="E1" s="540"/>
-      <c r="F1" s="540"/>
-      <c r="G1" s="540"/>
-      <c r="H1" s="540"/>
-      <c r="I1" s="540"/>
-      <c r="J1" s="540"/>
-      <c r="K1" s="540"/>
+      <c r="D1" s="567"/>
+      <c r="E1" s="567"/>
+      <c r="F1" s="567"/>
+      <c r="G1" s="567"/>
+      <c r="H1" s="567"/>
+      <c r="I1" s="567"/>
+      <c r="J1" s="567"/>
+      <c r="K1" s="567"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -58592,17 +58913,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="541" t="s">
+      <c r="B3" s="568" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="542"/>
+      <c r="C3" s="569"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="543" t="s">
+      <c r="H3" s="570" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="543"/>
+      <c r="I3" s="570"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -58631,14 +58952,14 @@
       <c r="D4" s="23">
         <v>44320</v>
       </c>
-      <c r="E4" s="544" t="s">
+      <c r="E4" s="571" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="545"/>
-      <c r="H4" s="546" t="s">
+      <c r="F4" s="572"/>
+      <c r="H4" s="573" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="547"/>
+      <c r="I4" s="574"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -61515,71 +61836,71 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="548" t="s">
+      <c r="H64" s="554" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="549"/>
+      <c r="I64" s="555"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="550">
+      <c r="K64" s="556">
         <f>I62+L62</f>
         <v>779034.56000000017</v>
       </c>
-      <c r="L64" s="551"/>
-      <c r="M64" s="552">
+      <c r="L64" s="557"/>
+      <c r="M64" s="558">
         <f>M62+N62</f>
         <v>4478181</v>
       </c>
-      <c r="N64" s="553"/>
+      <c r="N64" s="559"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="560" t="s">
+      <c r="D65" s="566" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="560"/>
+      <c r="E65" s="566"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>3602842.44</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="561">
+      <c r="P65" s="545">
         <f>P62+Q62</f>
         <v>5004562.5599999996</v>
       </c>
-      <c r="Q65" s="562"/>
+      <c r="Q65" s="546"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="577" t="s">
+      <c r="B66" s="582" t="s">
         <v>528</v>
       </c>
-      <c r="C66" s="578"/>
-      <c r="D66" s="560" t="s">
+      <c r="C66" s="583"/>
+      <c r="D66" s="566" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="560"/>
+      <c r="E66" s="566"/>
       <c r="F66" s="95">
         <v>-3854423.8</v>
       </c>
-      <c r="I66" s="564" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="565"/>
-      <c r="K66" s="566">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>14998.430000000139</v>
       </c>
-      <c r="L66" s="567"/>
+      <c r="L66" s="551"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
     <row r="67" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="579"/>
-      <c r="C67" s="580"/>
+      <c r="B67" s="584"/>
+      <c r="C67" s="585"/>
       <c r="D67" s="108"/>
       <c r="E67" s="60"/>
       <c r="F67" s="109">
@@ -61594,8 +61915,8 @@
       <c r="S67" s="50"/>
     </row>
     <row r="68" spans="2:19" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="581"/>
-      <c r="C68" s="582"/>
+      <c r="B68" s="586"/>
+      <c r="C68" s="587"/>
       <c r="E68" s="60" t="s">
         <v>20</v>
       </c>
@@ -61608,11 +61929,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="568">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-249311.35999999999</v>
       </c>
-      <c r="L68" s="569"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -61636,22 +61957,22 @@
       <c r="C70" s="119">
         <v>44353</v>
       </c>
-      <c r="D70" s="554" t="s">
+      <c r="D70" s="560" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="555"/>
+      <c r="E70" s="561"/>
       <c r="F70" s="120">
         <v>255764.39</v>
       </c>
-      <c r="I70" s="556" t="s">
+      <c r="I70" s="562" t="s">
         <v>431</v>
       </c>
-      <c r="J70" s="557"/>
-      <c r="K70" s="558">
+      <c r="J70" s="563"/>
+      <c r="K70" s="564">
         <f>K66+K68</f>
         <v>-234312.92999999985</v>
       </c>
-      <c r="L70" s="559"/>
+      <c r="L70" s="565"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -61807,11 +62128,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -61825,6 +62141,11 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="B66:C68"/>
     <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>